<commit_message>
Modification du programme et du plan de tests
</commit_message>
<xml_diff>
--- a/PEA/Plan de test/Plan de tests - PEA.xlsx
+++ b/PEA/Plan de test/Plan de tests - PEA.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mon Drive\BTS CIEL - 2ème année\Projet final - gestion d'accès\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robin\Documents\GITHUB\ACCES_CAMPUS\Acc-s-campus-\PEA\Plan de test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64C4BFDD-9843-49C6-985D-516329DC0F61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3B7CE011-0258-40C9-A5BD-B005CBAB91AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{21D66C90-57CB-4BB7-B44F-BA6973DF79EF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{21D66C90-57CB-4BB7-B44F-BA6973DF79EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Microcontrôleur" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="108">
   <si>
     <t>Identification du Test</t>
   </si>
@@ -206,24 +206,6 @@
     <t>Putty</t>
   </si>
   <si>
-    <t>Nous devons observer des informations sur la ligne Ethernet.</t>
-  </si>
-  <si>
-    <t>Si les informations décoder corresponde au information envoyé</t>
-  </si>
-  <si>
-    <t>Placer les sondes de l'oscilloscope sur les pins 5,6,1, 2 vérifier la bonne réception et l'envoie des données. Utiliser le badge RFID pour lancer la séquence primaire.</t>
-  </si>
-  <si>
-    <t>Visualiser le serial monitor avec putty et lire les messages écrit dans le console.</t>
-  </si>
-  <si>
-    <t>Nous devons lire des messages dans la console.</t>
-  </si>
-  <si>
-    <t>Si un message de validation d'envoie est écrit.</t>
-  </si>
-  <si>
     <t>T3.1</t>
   </si>
   <si>
@@ -296,9 +278,6 @@
     <t>Si la tension est de 5V, alors la tension de sortie est bonne.</t>
   </si>
   <si>
-    <t>Identification du Plan de Tests</t>
-  </si>
-  <si>
     <t>Référence du module testé</t>
   </si>
   <si>
@@ -350,9 +329,6 @@
     <t>Tester le bon fonctionnement du jalon 1 de la PEA</t>
   </si>
   <si>
-    <t>Tests unitaires et test d'intégration</t>
-  </si>
-  <si>
     <t>Laboratoire</t>
   </si>
   <si>
@@ -363,6 +339,298 @@
   </si>
   <si>
     <t>Manipulation d'outils de mesure et d'un serial monitor.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identification du Plan de Tests </t>
+  </si>
+  <si>
+    <t>Tests unitaires</t>
+  </si>
+  <si>
+    <t>Bloc testé.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La PEA doit avoir le code de téléverser dans son microcontrôleur. Le système doit être alimenter et connecté au réseaux L'utilisateur doit disposer de 2 badges RFID adapté, dont il connait l'UID. L'UID de l'un des 2 badges doit être validé par la base de données. </t>
+  </si>
+  <si>
+    <t>Poser le badge RFID valide sur le capteur RFID.</t>
+  </si>
+  <si>
+    <r>
+      <t>La réponse du serveur, lu dans le serial monitor doit être la suivante :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="3" tint="0.249977111117893"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> HTTP/1.1 200 OK
+date: Tue, 04 Apr 2025 08:15:32 GMT
+server: uvicorn
+content-length: 67
+content-type: application/json
+{"nom":</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="6" tint="0.59999389629810485"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>"nom lier au badge"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="3" tint="0.249977111117893"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>,"prenom":</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="6" tint="0.59999389629810485"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>"prénom lier au badge"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="3" tint="0.249977111117893"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>,"role":</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="6" tint="0.59999389629810485"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>"rôle lié au badge"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="3" tint="0.249977111117893"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>,"autorise":</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="6" tint="0.59999389629810485"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>true</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="3" tint="0.249977111117893"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>}</t>
+    </r>
+  </si>
+  <si>
+    <t>un Serial monitor</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>Poser le badge RFID invalide sur le capteur RFID</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">La réponse du serveur, lu dans le serial monitor doit être la suivante : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="3" tint="0.249977111117893"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">HTTP/1.1 403 Forbidden
+date: Wed, 02 Apr 2025 08:13:46 GMT
+server: uvicorn
+content-length: 27
+content-type: application/json
+Connection: close
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="3" tint="0.249977111117893"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>{"detail":"Accès refusé"}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Le test est réussi si le message contient le code: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>HTTP/1.1 200 OK ,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">et le mesage : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>{"nom":"nom lier au badge","prenom":"prénom lier au badge","role":"rôle lié au badge","autorise":true}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Le test est réussi si le message contient le code : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>HTTP/1.1 403</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>, et le message : {</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>"detail":"Accès refusé"}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Le code "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>HTTP/1.1 200</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>OK</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>" as bien été obtenue avec les informations de l'utilisateur.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Le code "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>HTTP/1.1 403 Forbidden</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>" as bien été obtenue avec le message de refus.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -372,7 +640,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -425,6 +693,24 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="3" tint="0.249977111117893"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="6" tint="0.59999389629810485"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -470,7 +756,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -725,11 +1011,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -786,9 +1085,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -827,58 +1123,17 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -886,21 +1141,59 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -908,10 +1201,31 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -920,26 +1234,29 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -959,7 +1276,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1281,68 +1598,68 @@
       <selection activeCell="D4" sqref="D4:I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="6" max="6" width="9.28515625" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" ht="15.75" thickBot="1"/>
-    <row r="3" spans="2:9" ht="26.25" thickBot="1">
-      <c r="B3" s="57" t="s">
+    <row r="2" spans="2:9" ht="15" thickBot="1"/>
+    <row r="3" spans="2:9" ht="28.2" thickBot="1">
+      <c r="B3" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="58"/>
-      <c r="D3" s="59" t="s">
+      <c r="C3" s="40"/>
+      <c r="D3" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="40"/>
-      <c r="F3" s="41"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="35"/>
       <c r="G3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="59" t="s">
+      <c r="H3" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="41"/>
-    </row>
-    <row r="4" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B4" s="52" t="s">
+      <c r="I3" s="35"/>
+    </row>
+    <row r="4" spans="2:9" ht="15" thickBot="1">
+      <c r="B4" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="41"/>
-      <c r="D4" s="53" t="s">
+      <c r="C4" s="35"/>
+      <c r="D4" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="38"/>
-    </row>
-    <row r="5" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B5" s="52" t="s">
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="44"/>
+    </row>
+    <row r="5" spans="2:9" ht="15" thickBot="1">
+      <c r="B5" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="41"/>
-      <c r="D5" s="39" t="s">
+      <c r="C5" s="35"/>
+      <c r="D5" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
       <c r="G5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="54">
+      <c r="H5" s="38">
         <v>45734</v>
       </c>
-      <c r="I5" s="41"/>
+      <c r="I5" s="35"/>
     </row>
     <row r="6" spans="2:9" ht="42" customHeight="1" thickBot="1">
-      <c r="B6" s="55" t="s">
+      <c r="B6" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="56"/>
+      <c r="C6" s="48"/>
       <c r="D6" s="3" t="s">
         <v>7</v>
       </c>
@@ -1357,32 +1674,32 @@
       </c>
       <c r="I6" s="5"/>
     </row>
-    <row r="7" spans="2:9" ht="46.15" customHeight="1" thickBot="1">
-      <c r="B7" s="42" t="s">
+    <row r="7" spans="2:9" ht="46.2" customHeight="1" thickBot="1">
+      <c r="B7" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="43"/>
-      <c r="D7" s="61" t="s">
+      <c r="C7" s="50"/>
+      <c r="D7" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
-      <c r="I7" s="46"/>
-    </row>
-    <row r="8" spans="2:9" ht="26.25" thickBot="1">
+      <c r="E7" s="52"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="52"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="53"/>
+    </row>
+    <row r="8" spans="2:9" ht="28.2" thickBot="1">
       <c r="B8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="47" t="s">
+      <c r="C8" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="48"/>
-      <c r="E8" s="47" t="s">
+      <c r="D8" s="55"/>
+      <c r="E8" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="49"/>
+      <c r="F8" s="56"/>
       <c r="G8" s="10" t="s">
         <v>14</v>
       </c>
@@ -1397,104 +1714,104 @@
       <c r="B9" s="13">
         <v>1</v>
       </c>
-      <c r="C9" s="62" t="s">
+      <c r="C9" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="51"/>
-      <c r="E9" s="62" t="s">
+      <c r="D9" s="58"/>
+      <c r="E9" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="51"/>
+      <c r="F9" s="58"/>
       <c r="G9" s="14" t="s">
         <v>27</v>
       </c>
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
     </row>
-    <row r="10" spans="2:9" ht="15.75" thickBot="1">
+    <row r="10" spans="2:9" ht="15" thickBot="1">
       <c r="B10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="35" t="s">
+      <c r="C10" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
       <c r="H10" s="7" t="s">
         <v>19</v>
       </c>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" spans="2:9" ht="28.9" customHeight="1" thickBot="1">
-      <c r="B11" s="37" t="s">
+    <row r="11" spans="2:9" ht="28.95" customHeight="1" thickBot="1">
+      <c r="B11" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="38"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="41"/>
-    </row>
-    <row r="12" spans="2:9" ht="15.75" thickBot="1"/>
-    <row r="13" spans="2:9" ht="26.25" thickBot="1">
-      <c r="B13" s="57" t="s">
+      <c r="C11" s="44"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="35"/>
+    </row>
+    <row r="12" spans="2:9" ht="15" thickBot="1"/>
+    <row r="13" spans="2:9" ht="28.2" thickBot="1">
+      <c r="B13" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="58"/>
-      <c r="D13" s="59" t="s">
+      <c r="C13" s="40"/>
+      <c r="D13" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="40"/>
-      <c r="F13" s="41"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="35"/>
       <c r="G13" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H13" s="59" t="s">
+      <c r="H13" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="I13" s="41"/>
-    </row>
-    <row r="14" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B14" s="52" t="s">
+      <c r="I13" s="35"/>
+    </row>
+    <row r="14" spans="2:9" ht="15" thickBot="1">
+      <c r="B14" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="41"/>
-      <c r="D14" s="53" t="s">
+      <c r="C14" s="35"/>
+      <c r="D14" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="38"/>
-    </row>
-    <row r="15" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B15" s="52" t="s">
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="44"/>
+    </row>
+    <row r="15" spans="2:9" ht="15" thickBot="1">
+      <c r="B15" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="41"/>
-      <c r="D15" s="39" t="s">
+      <c r="C15" s="35"/>
+      <c r="D15" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="40"/>
-      <c r="F15" s="40"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
       <c r="G15" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H15" s="54">
+      <c r="H15" s="38">
         <v>45734</v>
       </c>
-      <c r="I15" s="41"/>
-    </row>
-    <row r="16" spans="2:9" ht="39" thickBot="1">
-      <c r="B16" s="55" t="s">
+      <c r="I15" s="35"/>
+    </row>
+    <row r="16" spans="2:9" ht="42" thickBot="1">
+      <c r="B16" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="56"/>
+      <c r="C16" s="48"/>
       <c r="D16" s="3" t="s">
         <v>7</v>
       </c>
@@ -1509,32 +1826,32 @@
       </c>
       <c r="I16" s="5"/>
     </row>
-    <row r="17" spans="2:9" ht="28.9" customHeight="1" thickBot="1">
-      <c r="B17" s="42" t="s">
+    <row r="17" spans="2:9" ht="28.95" customHeight="1" thickBot="1">
+      <c r="B17" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="43"/>
-      <c r="D17" s="61" t="s">
+      <c r="C17" s="50"/>
+      <c r="D17" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45"/>
-      <c r="I17" s="46"/>
-    </row>
-    <row r="18" spans="2:9" ht="26.25" thickBot="1">
+      <c r="E17" s="52"/>
+      <c r="F17" s="52"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="52"/>
+      <c r="I17" s="53"/>
+    </row>
+    <row r="18" spans="2:9" ht="28.2" thickBot="1">
       <c r="B18" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="47" t="s">
+      <c r="C18" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="48"/>
-      <c r="E18" s="47" t="s">
+      <c r="D18" s="55"/>
+      <c r="E18" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="F18" s="49"/>
+      <c r="F18" s="56"/>
       <c r="G18" s="10" t="s">
         <v>14</v>
       </c>
@@ -1545,108 +1862,108 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="2:9" ht="39" thickBot="1">
+    <row r="19" spans="2:9" ht="42" thickBot="1">
       <c r="B19" s="13">
         <v>1</v>
       </c>
-      <c r="C19" s="62" t="s">
+      <c r="C19" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="D19" s="51"/>
-      <c r="E19" s="62" t="s">
+      <c r="D19" s="58"/>
+      <c r="E19" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="F19" s="51"/>
+      <c r="F19" s="58"/>
       <c r="G19" s="14" t="s">
         <v>35</v>
       </c>
       <c r="H19" s="14"/>
       <c r="I19" s="14"/>
     </row>
-    <row r="20" spans="2:9" ht="15.75" thickBot="1">
+    <row r="20" spans="2:9" ht="15" thickBot="1">
       <c r="B20" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="35" t="s">
+      <c r="C20" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="36"/>
-      <c r="E20" s="36"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="36"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="43"/>
       <c r="H20" s="7" t="s">
         <v>19</v>
       </c>
       <c r="I20" s="6"/>
     </row>
-    <row r="21" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B21" s="37" t="s">
+    <row r="21" spans="2:9" ht="15" thickBot="1">
+      <c r="B21" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="38"/>
-      <c r="D21" s="39"/>
-      <c r="E21" s="40"/>
-      <c r="F21" s="40"/>
-      <c r="G21" s="40"/>
-      <c r="H21" s="40"/>
-      <c r="I21" s="41"/>
-    </row>
-    <row r="22" spans="2:9" ht="15.75" thickBot="1"/>
-    <row r="23" spans="2:9" ht="26.25" thickBot="1">
-      <c r="B23" s="57" t="s">
+      <c r="C21" s="44"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="37"/>
+      <c r="G21" s="37"/>
+      <c r="H21" s="37"/>
+      <c r="I21" s="35"/>
+    </row>
+    <row r="22" spans="2:9" ht="15" thickBot="1"/>
+    <row r="23" spans="2:9" ht="28.2" thickBot="1">
+      <c r="B23" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C23" s="58"/>
-      <c r="D23" s="59" t="s">
+      <c r="C23" s="40"/>
+      <c r="D23" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="E23" s="40"/>
-      <c r="F23" s="41"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="35"/>
       <c r="G23" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H23" s="60" t="s">
+      <c r="H23" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="I23" s="41"/>
-    </row>
-    <row r="24" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B24" s="52" t="s">
+      <c r="I23" s="35"/>
+    </row>
+    <row r="24" spans="2:9" ht="15" thickBot="1">
+      <c r="B24" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="C24" s="41"/>
-      <c r="D24" s="53" t="s">
+      <c r="C24" s="35"/>
+      <c r="D24" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="E24" s="36"/>
-      <c r="F24" s="36"/>
-      <c r="G24" s="36"/>
-      <c r="H24" s="36"/>
-      <c r="I24" s="38"/>
-    </row>
-    <row r="25" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B25" s="52" t="s">
+      <c r="E24" s="43"/>
+      <c r="F24" s="43"/>
+      <c r="G24" s="43"/>
+      <c r="H24" s="43"/>
+      <c r="I24" s="44"/>
+    </row>
+    <row r="25" spans="2:9" ht="15" thickBot="1">
+      <c r="B25" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="C25" s="41"/>
-      <c r="D25" s="39" t="s">
+      <c r="C25" s="35"/>
+      <c r="D25" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="E25" s="40"/>
-      <c r="F25" s="40"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="37"/>
       <c r="G25" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H25" s="54">
+      <c r="H25" s="38">
         <v>45734</v>
       </c>
-      <c r="I25" s="41"/>
-    </row>
-    <row r="26" spans="2:9" ht="27" thickBot="1">
-      <c r="B26" s="55" t="s">
+      <c r="I25" s="35"/>
+    </row>
+    <row r="26" spans="2:9" ht="24.6" thickBot="1">
+      <c r="B26" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="56"/>
+      <c r="C26" s="48"/>
       <c r="D26" s="3" t="s">
         <v>7</v>
       </c>
@@ -1662,32 +1979,32 @@
       </c>
       <c r="I26" s="5"/>
     </row>
-    <row r="27" spans="2:9" ht="32.450000000000003" customHeight="1" thickBot="1">
-      <c r="B27" s="42" t="s">
+    <row r="27" spans="2:9" ht="32.4" customHeight="1" thickBot="1">
+      <c r="B27" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="43"/>
-      <c r="D27" s="44" t="s">
+      <c r="C27" s="50"/>
+      <c r="D27" s="60" t="s">
         <v>36</v>
       </c>
-      <c r="E27" s="45"/>
-      <c r="F27" s="45"/>
-      <c r="G27" s="45"/>
-      <c r="H27" s="45"/>
-      <c r="I27" s="46"/>
-    </row>
-    <row r="28" spans="2:9" ht="26.25" thickBot="1">
+      <c r="E27" s="52"/>
+      <c r="F27" s="52"/>
+      <c r="G27" s="52"/>
+      <c r="H27" s="52"/>
+      <c r="I27" s="53"/>
+    </row>
+    <row r="28" spans="2:9" ht="28.2" thickBot="1">
       <c r="B28" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="47" t="s">
+      <c r="C28" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="D28" s="48"/>
-      <c r="E28" s="47" t="s">
+      <c r="D28" s="55"/>
+      <c r="E28" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="F28" s="49"/>
+      <c r="F28" s="56"/>
       <c r="G28" s="10" t="s">
         <v>14</v>
       </c>
@@ -1698,72 +2015,75 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="2:9" ht="39" thickBot="1">
+    <row r="29" spans="2:9" ht="42" thickBot="1">
       <c r="B29" s="13">
         <v>1</v>
       </c>
-      <c r="C29" s="50" t="s">
+      <c r="C29" s="61" t="s">
         <v>42</v>
       </c>
-      <c r="D29" s="51"/>
-      <c r="E29" s="50" t="s">
+      <c r="D29" s="58"/>
+      <c r="E29" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="F29" s="51"/>
+      <c r="F29" s="58"/>
       <c r="G29" s="17" t="s">
         <v>44</v>
       </c>
       <c r="H29" s="14"/>
       <c r="I29" s="14"/>
     </row>
-    <row r="30" spans="2:9" ht="15.75" thickBot="1">
+    <row r="30" spans="2:9" ht="15" thickBot="1">
       <c r="B30" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C30" s="35" t="s">
+      <c r="C30" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="D30" s="36"/>
-      <c r="E30" s="36"/>
-      <c r="F30" s="36"/>
-      <c r="G30" s="36"/>
+      <c r="D30" s="43"/>
+      <c r="E30" s="43"/>
+      <c r="F30" s="43"/>
+      <c r="G30" s="43"/>
       <c r="H30" s="7" t="s">
         <v>19</v>
       </c>
       <c r="I30" s="6"/>
     </row>
-    <row r="31" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B31" s="37" t="s">
+    <row r="31" spans="2:9" ht="15" thickBot="1">
+      <c r="B31" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="C31" s="38"/>
-      <c r="D31" s="39"/>
-      <c r="E31" s="40"/>
-      <c r="F31" s="40"/>
-      <c r="G31" s="40"/>
-      <c r="H31" s="40"/>
-      <c r="I31" s="41"/>
+      <c r="C31" s="44"/>
+      <c r="D31" s="36"/>
+      <c r="E31" s="37"/>
+      <c r="F31" s="37"/>
+      <c r="G31" s="37"/>
+      <c r="H31" s="37"/>
+      <c r="I31" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:I4"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:I11"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:I7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:I31"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D27:I27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:I21"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:I24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="H25:I25"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="E19:F19"/>
     <mergeCell ref="B13:C13"/>
@@ -1779,27 +2099,24 @@
     <mergeCell ref="D17:I17"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="E18:F18"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:I21"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:I24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:I31"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D27:I27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:I11"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:I7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1809,73 +2126,77 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7081FA0-4B60-41EA-8343-4988B4EF9AE5}">
   <dimension ref="B1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:I3"/>
+    <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="92" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6:I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="7" max="7" width="21.109375" customWidth="1"/>
+    <col min="8" max="8" width="18.5546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="15.75" thickBot="1"/>
-    <row r="2" spans="2:9" ht="26.25" thickBot="1">
-      <c r="B2" s="57" t="s">
+    <row r="1" spans="2:9" ht="15" thickBot="1"/>
+    <row r="2" spans="2:9" ht="15" thickBot="1">
+      <c r="B2" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="60" t="s">
-        <v>55</v>
-      </c>
-      <c r="E2" s="40"/>
-      <c r="F2" s="41"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="59" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="37"/>
+      <c r="F2" s="35"/>
       <c r="G2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="60" t="s">
+        <v>96</v>
+      </c>
+      <c r="H2" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="I2" s="41"/>
-    </row>
-    <row r="3" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B3" s="52" t="s">
+      <c r="I2" s="35"/>
+    </row>
+    <row r="3" spans="2:9" ht="15" thickBot="1">
+      <c r="B3" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="41"/>
-      <c r="D3" s="53" t="s">
+      <c r="C3" s="35"/>
+      <c r="D3" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="38"/>
-    </row>
-    <row r="4" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B4" s="52" t="s">
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="44"/>
+    </row>
+    <row r="4" spans="2:9" ht="15" thickBot="1">
+      <c r="B4" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="41"/>
-      <c r="D4" s="39" t="s">
+      <c r="C4" s="35"/>
+      <c r="D4" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
       <c r="G4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="54">
-        <v>45734</v>
-      </c>
-      <c r="I4" s="41"/>
-    </row>
-    <row r="5" spans="2:9" ht="27" thickBot="1">
-      <c r="B5" s="55" t="s">
+      <c r="H4" s="38">
+        <v>45747</v>
+      </c>
+      <c r="I4" s="35"/>
+    </row>
+    <row r="5" spans="2:9" ht="24.6" thickBot="1">
+      <c r="B5" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="56"/>
+      <c r="C5" s="48"/>
       <c r="D5" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>48</v>
+        <v>100</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>8</v>
@@ -1888,32 +2209,32 @@
       </c>
       <c r="I5" s="5"/>
     </row>
-    <row r="6" spans="2:9" ht="30" customHeight="1" thickBot="1">
-      <c r="B6" s="42" t="s">
+    <row r="6" spans="2:9" ht="42.6" customHeight="1" thickBot="1">
+      <c r="B6" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="43"/>
-      <c r="D6" s="44" t="s">
-        <v>36</v>
-      </c>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="45"/>
-      <c r="I6" s="46"/>
-    </row>
-    <row r="7" spans="2:9" ht="26.25" thickBot="1">
+      <c r="C6" s="50"/>
+      <c r="D6" s="60" t="s">
+        <v>97</v>
+      </c>
+      <c r="E6" s="52"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="52"/>
+      <c r="I6" s="53"/>
+    </row>
+    <row r="7" spans="2:9" ht="28.2" thickBot="1">
       <c r="B7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="47" t="s">
+      <c r="C7" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="48"/>
-      <c r="E7" s="47" t="s">
+      <c r="D7" s="55"/>
+      <c r="E7" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="49"/>
+      <c r="F7" s="56"/>
       <c r="G7" s="10" t="s">
         <v>14</v>
       </c>
@@ -1924,72 +2245,85 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="2:9" ht="88.15" customHeight="1" thickBot="1">
-      <c r="B8" s="13">
+    <row r="8" spans="2:9" ht="190.2" customHeight="1" thickBot="1">
+      <c r="B8" s="81">
         <v>1</v>
       </c>
-      <c r="C8" s="50" t="s">
-        <v>51</v>
-      </c>
-      <c r="D8" s="51"/>
-      <c r="E8" s="50" t="s">
-        <v>49</v>
-      </c>
-      <c r="F8" s="51"/>
-      <c r="G8" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-    </row>
-    <row r="9" spans="2:9" ht="62.45" customHeight="1" thickBot="1">
-      <c r="B9" s="20">
+      <c r="C8" s="82" t="s">
+        <v>98</v>
+      </c>
+      <c r="D8" s="83"/>
+      <c r="E8" s="82" t="s">
+        <v>99</v>
+      </c>
+      <c r="F8" s="83"/>
+      <c r="G8" s="84" t="s">
+        <v>104</v>
+      </c>
+      <c r="H8" s="84" t="s">
+        <v>106</v>
+      </c>
+      <c r="I8" s="84" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" ht="190.2" customHeight="1" thickBot="1">
+      <c r="B9" s="85">
         <v>2</v>
       </c>
-      <c r="C9" s="64" t="s">
-        <v>52</v>
+      <c r="C9" s="63" t="s">
+        <v>102</v>
       </c>
       <c r="D9" s="64"/>
-      <c r="E9" s="64" t="s">
-        <v>53</v>
-      </c>
-      <c r="F9" s="64"/>
-      <c r="G9" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-    </row>
-    <row r="10" spans="2:9" ht="15.75" thickBot="1">
+      <c r="E9" s="87" t="s">
+        <v>103</v>
+      </c>
+      <c r="F9" s="88"/>
+      <c r="G9" s="86" t="s">
+        <v>105</v>
+      </c>
+      <c r="H9" s="86" t="s">
+        <v>107</v>
+      </c>
+      <c r="I9" s="17" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" ht="15" thickBot="1">
       <c r="B10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="35" t="s">
+      <c r="C10" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
       <c r="H10" s="7" t="s">
         <v>19</v>
       </c>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B11" s="37" t="s">
+    <row r="11" spans="2:9" ht="15" thickBot="1">
+      <c r="B11" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="38"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="41"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:I11"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="B2:C2"/>
@@ -2005,13 +2339,9 @@
     <mergeCell ref="D6:I6"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="E7:F7"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:I11"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2023,68 +2353,68 @@
       <selection activeCell="D4" sqref="D4:I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="2" spans="2:9" ht="15.75" thickBot="1"/>
-    <row r="3" spans="2:9" ht="26.25" thickBot="1">
-      <c r="B3" s="57" t="s">
+    <row r="2" spans="2:9" ht="15" thickBot="1"/>
+    <row r="3" spans="2:9" ht="28.2" thickBot="1">
+      <c r="B3" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="58"/>
-      <c r="D3" s="60" t="s">
+      <c r="C3" s="40"/>
+      <c r="D3" s="59" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="40"/>
-      <c r="F3" s="41"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="35"/>
       <c r="G3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="60" t="s">
-        <v>65</v>
-      </c>
-      <c r="I3" s="41"/>
-    </row>
-    <row r="4" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B4" s="52" t="s">
+      <c r="H3" s="59" t="s">
+        <v>59</v>
+      </c>
+      <c r="I3" s="35"/>
+    </row>
+    <row r="4" spans="2:9" ht="15" thickBot="1">
+      <c r="B4" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="41"/>
-      <c r="D4" s="53" t="s">
-        <v>64</v>
-      </c>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="38"/>
-    </row>
-    <row r="5" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B5" s="52" t="s">
+      <c r="C4" s="35"/>
+      <c r="D4" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="44"/>
+    </row>
+    <row r="5" spans="2:9" ht="15" thickBot="1">
+      <c r="B5" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="41"/>
-      <c r="D5" s="63" t="s">
+      <c r="C5" s="35"/>
+      <c r="D5" s="62" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
       <c r="G5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="54">
+      <c r="H5" s="38">
         <v>45734</v>
       </c>
-      <c r="I5" s="41"/>
-    </row>
-    <row r="6" spans="2:9" ht="39" thickBot="1">
-      <c r="B6" s="55" t="s">
+      <c r="I5" s="35"/>
+    </row>
+    <row r="6" spans="2:9" ht="42" thickBot="1">
+      <c r="B6" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="56"/>
+      <c r="C6" s="48"/>
       <c r="D6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="22" t="s">
+      <c r="E6" s="21" t="s">
         <v>48</v>
       </c>
       <c r="F6" s="3" t="s">
@@ -2097,31 +2427,31 @@
       <c r="I6" s="5"/>
     </row>
     <row r="7" spans="2:9" ht="33" customHeight="1" thickBot="1">
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="43"/>
-      <c r="D7" s="44" t="s">
-        <v>66</v>
-      </c>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
-      <c r="I7" s="46"/>
-    </row>
-    <row r="8" spans="2:9" ht="26.25" thickBot="1">
+      <c r="C7" s="50"/>
+      <c r="D7" s="60" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="52"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="52"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="53"/>
+    </row>
+    <row r="8" spans="2:9" ht="28.2" thickBot="1">
       <c r="B8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="47" t="s">
+      <c r="C8" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="48"/>
-      <c r="E8" s="47" t="s">
+      <c r="D8" s="55"/>
+      <c r="E8" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="49"/>
+      <c r="F8" s="56"/>
       <c r="G8" s="10" t="s">
         <v>14</v>
       </c>
@@ -2132,62 +2462,54 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="2:9" ht="77.25" thickBot="1">
+    <row r="9" spans="2:9" ht="83.4" thickBot="1">
       <c r="B9" s="13">
         <v>1</v>
       </c>
-      <c r="C9" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="D9" s="51"/>
-      <c r="E9" s="50" t="s">
-        <v>68</v>
-      </c>
-      <c r="F9" s="51"/>
+      <c r="C9" s="61" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="58"/>
+      <c r="E9" s="61" t="s">
+        <v>62</v>
+      </c>
+      <c r="F9" s="58"/>
       <c r="G9" s="14" t="s">
         <v>27</v>
       </c>
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
     </row>
-    <row r="10" spans="2:9" ht="15.75" thickBot="1">
+    <row r="10" spans="2:9" ht="15" thickBot="1">
       <c r="B10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="35" t="s">
+      <c r="C10" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
       <c r="H10" s="7" t="s">
         <v>19</v>
       </c>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B11" s="37" t="s">
+    <row r="11" spans="2:9" ht="15" thickBot="1">
+      <c r="B11" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="38"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="41"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:I4"/>
     <mergeCell ref="C10:G10"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="D11:I11"/>
@@ -2198,6 +2520,14 @@
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="E9:F9"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2211,64 +2541,64 @@
       <selection activeCell="D5" sqref="D5:I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="3" spans="2:9" ht="15.75" thickBot="1"/>
-    <row r="4" spans="2:9" ht="26.25" thickBot="1">
-      <c r="B4" s="57" t="s">
+    <row r="3" spans="2:9" ht="15" thickBot="1"/>
+    <row r="4" spans="2:9" ht="28.2" thickBot="1">
+      <c r="B4" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="58"/>
-      <c r="D4" s="60" t="s">
-        <v>62</v>
-      </c>
-      <c r="E4" s="40"/>
-      <c r="F4" s="41"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="59" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" s="37"/>
+      <c r="F4" s="35"/>
       <c r="G4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="60" t="s">
-        <v>56</v>
-      </c>
-      <c r="I4" s="41"/>
-    </row>
-    <row r="5" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B5" s="52" t="s">
+      <c r="H4" s="59" t="s">
+        <v>50</v>
+      </c>
+      <c r="I4" s="35"/>
+    </row>
+    <row r="5" spans="2:9" ht="15" thickBot="1">
+      <c r="B5" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="41"/>
-      <c r="D5" s="53" t="s">
-        <v>57</v>
-      </c>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="38"/>
-    </row>
-    <row r="6" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B6" s="52" t="s">
+      <c r="C5" s="35"/>
+      <c r="D5" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="44"/>
+    </row>
+    <row r="6" spans="2:9" ht="15" thickBot="1">
+      <c r="B6" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="41"/>
-      <c r="D6" s="39" t="s">
+      <c r="C6" s="35"/>
+      <c r="D6" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
       <c r="G6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="54">
+      <c r="H6" s="38">
         <v>45734</v>
       </c>
-      <c r="I6" s="41"/>
-    </row>
-    <row r="7" spans="2:9" ht="27" thickBot="1">
-      <c r="B7" s="55" t="s">
+      <c r="I6" s="35"/>
+    </row>
+    <row r="7" spans="2:9" ht="24.6" thickBot="1">
+      <c r="B7" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="56"/>
+      <c r="C7" s="48"/>
       <c r="D7" s="3" t="s">
         <v>7</v>
       </c>
@@ -2282,32 +2612,32 @@
       </c>
       <c r="I7" s="5"/>
     </row>
-    <row r="8" spans="2:9" ht="28.9" customHeight="1" thickBot="1">
-      <c r="B8" s="42" t="s">
+    <row r="8" spans="2:9" ht="28.95" customHeight="1" thickBot="1">
+      <c r="B8" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="43"/>
-      <c r="D8" s="44" t="s">
-        <v>58</v>
-      </c>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="46"/>
-    </row>
-    <row r="9" spans="2:9" ht="26.25" thickBot="1">
+      <c r="C8" s="50"/>
+      <c r="D8" s="60" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="52"/>
+      <c r="F8" s="52"/>
+      <c r="G8" s="52"/>
+      <c r="H8" s="52"/>
+      <c r="I8" s="53"/>
+    </row>
+    <row r="9" spans="2:9" ht="28.2" thickBot="1">
       <c r="B9" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="47" t="s">
+      <c r="C9" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="48"/>
-      <c r="E9" s="47" t="s">
+      <c r="D9" s="55"/>
+      <c r="E9" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="49"/>
+      <c r="F9" s="56"/>
       <c r="G9" s="10" t="s">
         <v>14</v>
       </c>
@@ -2318,62 +2648,54 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="2:9" ht="79.150000000000006" customHeight="1" thickBot="1">
+    <row r="10" spans="2:9" ht="79.2" customHeight="1" thickBot="1">
       <c r="B10" s="13">
         <v>1</v>
       </c>
-      <c r="C10" s="50" t="s">
-        <v>59</v>
-      </c>
-      <c r="D10" s="51"/>
-      <c r="E10" s="50" t="s">
-        <v>60</v>
-      </c>
-      <c r="F10" s="51"/>
+      <c r="C10" s="61" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="58"/>
+      <c r="E10" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" s="58"/>
       <c r="G10" s="17" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
     </row>
-    <row r="11" spans="2:9" ht="15.75" thickBot="1">
+    <row r="11" spans="2:9" ht="15" thickBot="1">
       <c r="B11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="35" t="s">
+      <c r="C11" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
       <c r="H11" s="7" t="s">
         <v>19</v>
       </c>
       <c r="I11" s="6"/>
     </row>
-    <row r="12" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B12" s="37" t="s">
+    <row r="12" spans="2:9" ht="15" thickBot="1">
+      <c r="B12" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="38"/>
-      <c r="D12" s="39"/>
-      <c r="E12" s="40"/>
-      <c r="F12" s="40"/>
-      <c r="G12" s="40"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="41"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:I5"/>
     <mergeCell ref="C11:G11"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="D12:I12"/>
@@ -2384,6 +2706,14 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="E10:F10"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:I5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2397,105 +2727,105 @@
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="2:9" ht="15.75" thickBot="1"/>
-    <row r="2" spans="2:9" ht="26.25" thickBot="1">
-      <c r="B2" s="57" t="s">
+    <row r="1" spans="2:9" ht="15" thickBot="1"/>
+    <row r="2" spans="2:9" ht="28.2" thickBot="1">
+      <c r="B2" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="60" t="s">
-        <v>63</v>
-      </c>
-      <c r="E2" s="40"/>
-      <c r="F2" s="41"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="59" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="37"/>
+      <c r="F2" s="35"/>
       <c r="G2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="60" t="s">
-        <v>69</v>
-      </c>
-      <c r="I2" s="41"/>
+      <c r="H2" s="59" t="s">
+        <v>63</v>
+      </c>
+      <c r="I2" s="35"/>
     </row>
     <row r="3" spans="2:9" ht="15" customHeight="1" thickBot="1">
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="41"/>
-      <c r="D3" s="53" t="s">
-        <v>70</v>
-      </c>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="38"/>
-    </row>
-    <row r="4" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B4" s="52" t="s">
+      <c r="C3" s="35"/>
+      <c r="D3" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="44"/>
+    </row>
+    <row r="4" spans="2:9" ht="15" thickBot="1">
+      <c r="B4" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="41"/>
-      <c r="D4" s="39" t="s">
+      <c r="C4" s="35"/>
+      <c r="D4" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
       <c r="G4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="54">
+      <c r="H4" s="38">
         <v>45734</v>
       </c>
-      <c r="I4" s="41"/>
-    </row>
-    <row r="5" spans="2:9" ht="27" thickBot="1">
-      <c r="B5" s="55" t="s">
+      <c r="I4" s="35"/>
+    </row>
+    <row r="5" spans="2:9" ht="24.6" thickBot="1">
+      <c r="B5" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="56"/>
+      <c r="C5" s="48"/>
       <c r="D5" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="15"/>
-      <c r="F5" s="21" t="s">
+      <c r="F5" s="20" t="s">
         <v>8</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="H5" s="16" t="s">
         <v>41</v>
       </c>
       <c r="I5" s="5"/>
     </row>
-    <row r="6" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B6" s="42" t="s">
+    <row r="6" spans="2:9" ht="15" thickBot="1">
+      <c r="B6" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="43"/>
-      <c r="D6" s="44" t="s">
-        <v>72</v>
-      </c>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="45"/>
-      <c r="I6" s="46"/>
-    </row>
-    <row r="7" spans="2:9" ht="26.25" thickBot="1">
+      <c r="C6" s="50"/>
+      <c r="D6" s="60" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" s="52"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="52"/>
+      <c r="I6" s="53"/>
+    </row>
+    <row r="7" spans="2:9" ht="28.2" thickBot="1">
       <c r="B7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="47" t="s">
+      <c r="C7" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="48"/>
-      <c r="E7" s="47" t="s">
+      <c r="D7" s="55"/>
+      <c r="E7" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="49"/>
+      <c r="F7" s="56"/>
       <c r="G7" s="10" t="s">
         <v>14</v>
       </c>
@@ -2506,20 +2836,20 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="2:9" ht="51.75" thickBot="1">
+    <row r="8" spans="2:9" ht="69.599999999999994" thickBot="1">
       <c r="B8" s="13">
         <v>1</v>
       </c>
-      <c r="C8" s="50" t="s">
-        <v>73</v>
-      </c>
-      <c r="D8" s="51"/>
-      <c r="E8" s="50" t="s">
-        <v>74</v>
-      </c>
-      <c r="F8" s="51"/>
+      <c r="C8" s="61" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="58"/>
+      <c r="E8" s="61" t="s">
+        <v>68</v>
+      </c>
+      <c r="F8" s="58"/>
       <c r="G8" s="17" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
@@ -2528,50 +2858,55 @@
       <c r="B9" s="13">
         <v>2</v>
       </c>
-      <c r="C9" s="65" t="s">
-        <v>76</v>
-      </c>
-      <c r="D9" s="66"/>
-      <c r="E9" s="65" t="s">
-        <v>77</v>
-      </c>
-      <c r="F9" s="66"/>
+      <c r="C9" s="63" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="64"/>
+      <c r="E9" s="63" t="s">
+        <v>71</v>
+      </c>
+      <c r="F9" s="64"/>
       <c r="G9" s="17" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
     </row>
-    <row r="10" spans="2:9" ht="15.75" thickBot="1">
+    <row r="10" spans="2:9" ht="15" thickBot="1">
       <c r="B10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="35" t="s">
+      <c r="C10" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
       <c r="H10" s="7" t="s">
         <v>19</v>
       </c>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B11" s="37" t="s">
+    <row r="11" spans="2:9" ht="15" thickBot="1">
+      <c r="B11" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="38"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="41"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:I11"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="D2:F2"/>
@@ -2587,11 +2922,6 @@
     <mergeCell ref="D6:I6"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:I11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2601,246 +2931,253 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD219FCF-77B2-490B-816E-2F75E9617605}">
   <dimension ref="B1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="35.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" customWidth="1"/>
+    <col min="3" max="3" width="35.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" customWidth="1"/>
+    <col min="5" max="5" width="17.5546875" customWidth="1"/>
+    <col min="6" max="6" width="19.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="15.75" thickBot="1"/>
-    <row r="2" spans="2:6" ht="55.15" customHeight="1" thickBot="1">
-      <c r="B2" s="75" t="s">
+    <row r="1" spans="2:6" ht="15" thickBot="1"/>
+    <row r="2" spans="2:6" ht="55.2" customHeight="1" thickBot="1">
+      <c r="B2" s="69" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="70"/>
+      <c r="D2" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" s="23" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="15" thickBot="1">
+      <c r="B3" s="71" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="66"/>
+      <c r="D3" s="67" t="s">
+        <v>89</v>
+      </c>
+      <c r="E3" s="68"/>
+      <c r="F3" s="66"/>
+    </row>
+    <row r="4" spans="2:6" ht="15" thickBot="1">
+      <c r="B4" s="72" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" s="73"/>
+      <c r="D4" s="74" t="s">
+        <v>95</v>
+      </c>
+      <c r="E4" s="75"/>
+      <c r="F4" s="73"/>
+    </row>
+    <row r="5" spans="2:6" ht="15" thickBot="1">
+      <c r="B5" s="65" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" s="66"/>
+      <c r="D5" s="67" t="s">
+        <v>90</v>
+      </c>
+      <c r="E5" s="68"/>
+      <c r="F5" s="66"/>
+    </row>
+    <row r="6" spans="2:6" ht="42" thickBot="1">
+      <c r="B6" s="77" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" s="78"/>
+      <c r="D6" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="E6" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="F6" s="25" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="15" thickBot="1">
+      <c r="B7" s="79" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" s="80"/>
+      <c r="D7" s="80"/>
+      <c r="E7" s="80"/>
+      <c r="F7" s="78"/>
+    </row>
+    <row r="8" spans="2:6" ht="18" customHeight="1" thickBot="1">
+      <c r="B8" s="76" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="76"/>
-      <c r="D2" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="E2" s="23" t="s">
+      <c r="C8" s="68"/>
+      <c r="D8" s="66"/>
+      <c r="E8" s="76" t="s">
         <v>80</v>
       </c>
-      <c r="F2" s="24" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B3" s="77" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="69"/>
-      <c r="D3" s="74" t="s">
-        <v>96</v>
-      </c>
-      <c r="E3" s="68"/>
-      <c r="F3" s="69"/>
-    </row>
-    <row r="4" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B4" s="78" t="s">
-        <v>81</v>
-      </c>
-      <c r="C4" s="79"/>
-      <c r="D4" s="80" t="s">
-        <v>97</v>
-      </c>
-      <c r="E4" s="81"/>
-      <c r="F4" s="79"/>
-    </row>
-    <row r="5" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B5" s="82" t="s">
-        <v>82</v>
-      </c>
-      <c r="C5" s="69"/>
-      <c r="D5" s="74" t="s">
-        <v>98</v>
-      </c>
-      <c r="E5" s="68"/>
-      <c r="F5" s="69"/>
-    </row>
-    <row r="6" spans="2:6" ht="39" thickBot="1">
-      <c r="B6" s="70" t="s">
-        <v>83</v>
-      </c>
-      <c r="C6" s="71"/>
-      <c r="D6" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="E6" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="F6" s="26" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B7" s="72" t="s">
-        <v>85</v>
-      </c>
-      <c r="C7" s="73"/>
-      <c r="D7" s="73"/>
-      <c r="E7" s="73"/>
-      <c r="F7" s="71"/>
-    </row>
-    <row r="8" spans="2:6" ht="18" customHeight="1" thickBot="1">
-      <c r="B8" s="67" t="s">
-        <v>86</v>
-      </c>
-      <c r="C8" s="68"/>
-      <c r="D8" s="69"/>
-      <c r="E8" s="67" t="s">
-        <v>87</v>
-      </c>
-      <c r="F8" s="69"/>
+      <c r="F8" s="66"/>
     </row>
     <row r="9" spans="2:6" ht="36.6" customHeight="1" thickBot="1">
-      <c r="B9" s="74" t="s">
-        <v>100</v>
+      <c r="B9" s="67" t="s">
+        <v>92</v>
       </c>
       <c r="C9" s="68"/>
       <c r="D9" s="68"/>
-      <c r="E9" s="74"/>
-      <c r="F9" s="69"/>
-    </row>
-    <row r="10" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B10" s="67" t="s">
-        <v>88</v>
+      <c r="E9" s="67"/>
+      <c r="F9" s="66"/>
+    </row>
+    <row r="10" spans="2:6" ht="15" thickBot="1">
+      <c r="B10" s="76" t="s">
+        <v>81</v>
       </c>
       <c r="C10" s="68"/>
       <c r="D10" s="68"/>
       <c r="E10" s="68"/>
-      <c r="F10" s="69"/>
-    </row>
-    <row r="11" spans="2:6" ht="20.45" customHeight="1" thickBot="1">
-      <c r="B11" s="27" t="s">
-        <v>89</v>
-      </c>
-      <c r="C11" s="28" t="s">
-        <v>90</v>
-      </c>
-      <c r="D11" s="28" t="s">
-        <v>91</v>
-      </c>
-      <c r="E11" s="28" t="s">
-        <v>92</v>
-      </c>
-      <c r="F11" s="28" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" ht="26.25" thickBot="1">
-      <c r="B12" s="29" t="s">
+      <c r="F10" s="66"/>
+    </row>
+    <row r="11" spans="2:6" ht="20.399999999999999" customHeight="1" thickBot="1">
+      <c r="B11" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="C11" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="E11" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="F11" s="27" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="27" thickBot="1">
+      <c r="B12" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="30" t="s">
+      <c r="C12" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="31" t="s">
+      <c r="D12" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="30" t="s">
+      <c r="E12" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="30"/>
-    </row>
-    <row r="13" spans="2:6" ht="26.25" thickBot="1">
-      <c r="B13" s="29" t="s">
+      <c r="F12" s="29"/>
+    </row>
+    <row r="13" spans="2:6" ht="27" thickBot="1">
+      <c r="B13" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="30" t="s">
+      <c r="C13" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="31" t="s">
+      <c r="D13" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="30" t="s">
+      <c r="E13" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="F13" s="30"/>
-    </row>
-    <row r="14" spans="2:6" ht="39" thickBot="1">
-      <c r="B14" s="29" t="s">
+      <c r="F13" s="29"/>
+    </row>
+    <row r="14" spans="2:6" ht="40.200000000000003" thickBot="1">
+      <c r="B14" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="30" t="s">
+      <c r="C14" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="31" t="s">
+      <c r="D14" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="E14" s="30" t="s">
+      <c r="E14" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="30"/>
+      <c r="F14" s="29"/>
     </row>
     <row r="15" spans="2:6" ht="30" customHeight="1" thickBot="1">
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="33" t="s">
-        <v>64</v>
-      </c>
-      <c r="D15" s="31" t="s">
+      <c r="C15" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="E15" s="30" t="s">
+      <c r="E15" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="F15" s="32"/>
-    </row>
-    <row r="16" spans="2:6" ht="30.75" thickBot="1">
-      <c r="B16" s="29" t="s">
-        <v>55</v>
-      </c>
-      <c r="C16" s="33" t="s">
+      <c r="F15" s="31"/>
+    </row>
+    <row r="16" spans="2:6" ht="29.4" thickBot="1">
+      <c r="B16" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="31" t="s">
+      <c r="D16" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="30" t="s">
+      <c r="E16" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="F16" s="32"/>
-    </row>
-    <row r="17" spans="2:8" ht="26.25" thickBot="1">
-      <c r="B17" s="29" t="s">
-        <v>62</v>
+      <c r="F16" s="31"/>
+    </row>
+    <row r="17" spans="2:8" ht="28.2" thickBot="1">
+      <c r="B17" s="28" t="s">
+        <v>56</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="D17" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="E17" s="30" t="s">
+      <c r="E17" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="F17" s="34"/>
+      <c r="F17" s="33"/>
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
     </row>
-    <row r="18" spans="2:8" ht="30.75" thickBot="1">
-      <c r="B18" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="C18" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="D18" s="31" t="s">
+    <row r="18" spans="2:8" ht="29.4" thickBot="1">
+      <c r="B18" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="E18" s="30" t="s">
+      <c r="E18" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="F18" s="32"/>
+      <c r="F18" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="E9:F9"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="D5:F5"/>
     <mergeCell ref="B2:C2"/>
@@ -2848,13 +3185,6 @@
     <mergeCell ref="D3:F3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="D4:F4"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="E9:F9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Ajout du plan de tests intégration
</commit_message>
<xml_diff>
--- a/PEA/Plan de test/Plan de tests - PEA.xlsx
+++ b/PEA/Plan de test/Plan de tests - PEA.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robin\Documents\GITHUB\ACCES_CAMPUS\Acc-s-campus-\PEA\Plan de test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3B7CE011-0258-40C9-A5BD-B005CBAB91AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5038E7C3-6082-4FD1-92B9-AF8ED54CE6C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{21D66C90-57CB-4BB7-B44F-BA6973DF79EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Microcontrôleur" sheetId="1" r:id="rId1"/>
-    <sheet name="Convertisseur Ethernet" sheetId="2" r:id="rId2"/>
+    <sheet name="Ethernet" sheetId="2" r:id="rId2"/>
     <sheet name="RFID" sheetId="4" r:id="rId3"/>
     <sheet name="Gâche" sheetId="3" r:id="rId4"/>
     <sheet name="Alimentation PoE" sheetId="5" r:id="rId5"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="95">
   <si>
     <t>Identification du Test</t>
   </si>
@@ -197,9 +197,6 @@
     <t>T2.1</t>
   </si>
   <si>
-    <t>Communication Ethernet</t>
-  </si>
-  <si>
     <t>Le test permet de vérifier que la communication Ethernet est valide.</t>
   </si>
   <si>
@@ -345,292 +342,6 @@
   </si>
   <si>
     <t>Tests unitaires</t>
-  </si>
-  <si>
-    <t>Bloc testé.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">La PEA doit avoir le code de téléverser dans son microcontrôleur. Le système doit être alimenter et connecté au réseaux L'utilisateur doit disposer de 2 badges RFID adapté, dont il connait l'UID. L'UID de l'un des 2 badges doit être validé par la base de données. </t>
-  </si>
-  <si>
-    <t>Poser le badge RFID valide sur le capteur RFID.</t>
-  </si>
-  <si>
-    <r>
-      <t>La réponse du serveur, lu dans le serial monitor doit être la suivante :</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="3" tint="0.249977111117893"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> HTTP/1.1 200 OK
-date: Tue, 04 Apr 2025 08:15:32 GMT
-server: uvicorn
-content-length: 67
-content-type: application/json
-{"nom":</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="6" tint="0.59999389629810485"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>"nom lier au badge"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="3" tint="0.249977111117893"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>,"prenom":</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="6" tint="0.59999389629810485"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>"prénom lier au badge"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="3" tint="0.249977111117893"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>,"role":</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="6" tint="0.59999389629810485"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>"rôle lié au badge"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="3" tint="0.249977111117893"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>,"autorise":</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="6" tint="0.59999389629810485"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>true</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="3" tint="0.249977111117893"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>}</t>
-    </r>
-  </si>
-  <si>
-    <t>un Serial monitor</t>
-  </si>
-  <si>
-    <t>O</t>
-  </si>
-  <si>
-    <t>Poser le badge RFID invalide sur le capteur RFID</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">La réponse du serveur, lu dans le serial monitor doit être la suivante : </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="3" tint="0.249977111117893"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">HTTP/1.1 403 Forbidden
-date: Wed, 02 Apr 2025 08:13:46 GMT
-server: uvicorn
-content-length: 27
-content-type: application/json
-Connection: close
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="3" tint="0.249977111117893"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>{"detail":"Accès refusé"}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Le test est réussi si le message contient le code: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>HTTP/1.1 200 OK ,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">et le mesage : </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>{"nom":"nom lier au badge","prenom":"prénom lier au badge","role":"rôle lié au badge","autorise":true}</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Le test est réussi si le message contient le code : </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>HTTP/1.1 403</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>, et le message : {</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>"detail":"Accès refusé"}</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Le code "</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>HTTP/1.1 200</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>OK</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>" as bien été obtenue avec les informations de l'utilisateur.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Le code "</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>HTTP/1.1 403 Forbidden</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>" as bien été obtenue avec le message de refus.</t>
-    </r>
   </si>
 </sst>
 </file>
@@ -640,7 +351,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -693,24 +404,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color theme="3" tint="0.249977111117893"/>
-      <name val="Arial Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="6" tint="0.59999389629810485"/>
-      <name val="Arial Narrow"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -756,7 +449,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -1011,24 +704,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1123,17 +803,49 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1141,73 +853,52 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1223,41 +914,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1594,7 +1250,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E407FD9-0AE4-4A1C-B2E0-3161C8BCECA8}">
   <dimension ref="B2:I31"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D4" sqref="D4:I4"/>
     </sheetView>
   </sheetViews>
@@ -1606,60 +1262,60 @@
   <sheetData>
     <row r="2" spans="2:9" ht="15" thickBot="1"/>
     <row r="3" spans="2:9" ht="28.2" thickBot="1">
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="40"/>
-      <c r="D3" s="41" t="s">
+      <c r="C3" s="54"/>
+      <c r="D3" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="37"/>
-      <c r="F3" s="35"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="40"/>
       <c r="G3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="41" t="s">
+      <c r="H3" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="35"/>
+      <c r="I3" s="40"/>
     </row>
     <row r="4" spans="2:9" ht="15" thickBot="1">
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="42" t="s">
+      <c r="C4" s="40"/>
+      <c r="D4" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="44"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="37"/>
     </row>
     <row r="5" spans="2:9" ht="15" thickBot="1">
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="35"/>
-      <c r="D5" s="36" t="s">
+      <c r="C5" s="40"/>
+      <c r="D5" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
       <c r="G5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="38">
+      <c r="H5" s="59">
         <v>45734</v>
       </c>
-      <c r="I5" s="35"/>
+      <c r="I5" s="40"/>
     </row>
     <row r="6" spans="2:9" ht="42" customHeight="1" thickBot="1">
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="48"/>
+      <c r="C6" s="52"/>
       <c r="D6" s="3" t="s">
         <v>7</v>
       </c>
@@ -1675,31 +1331,31 @@
       <c r="I6" s="5"/>
     </row>
     <row r="7" spans="2:9" ht="46.2" customHeight="1" thickBot="1">
-      <c r="B7" s="49" t="s">
+      <c r="B7" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="50"/>
-      <c r="D7" s="51" t="s">
+      <c r="C7" s="42"/>
+      <c r="D7" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="52"/>
-      <c r="F7" s="52"/>
-      <c r="G7" s="52"/>
-      <c r="H7" s="52"/>
-      <c r="I7" s="53"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="44"/>
+      <c r="H7" s="44"/>
+      <c r="I7" s="45"/>
     </row>
     <row r="8" spans="2:9" ht="28.2" thickBot="1">
       <c r="B8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="54" t="s">
+      <c r="C8" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="55"/>
-      <c r="E8" s="54" t="s">
+      <c r="D8" s="47"/>
+      <c r="E8" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="56"/>
+      <c r="F8" s="48"/>
       <c r="G8" s="10" t="s">
         <v>14</v>
       </c>
@@ -1714,14 +1370,14 @@
       <c r="B9" s="13">
         <v>1</v>
       </c>
-      <c r="C9" s="57" t="s">
+      <c r="C9" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="58"/>
-      <c r="E9" s="57" t="s">
+      <c r="D9" s="50"/>
+      <c r="E9" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="58"/>
+      <c r="F9" s="50"/>
       <c r="G9" s="14" t="s">
         <v>27</v>
       </c>
@@ -1732,86 +1388,86 @@
       <c r="B10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="45" t="s">
+      <c r="C10" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="35"/>
       <c r="H10" s="7" t="s">
         <v>19</v>
       </c>
       <c r="I10" s="6"/>
     </row>
     <row r="11" spans="2:9" ht="28.95" customHeight="1" thickBot="1">
-      <c r="B11" s="46" t="s">
+      <c r="B11" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="44"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="37"/>
-      <c r="H11" s="37"/>
-      <c r="I11" s="35"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="40"/>
     </row>
     <row r="12" spans="2:9" ht="15" thickBot="1"/>
     <row r="13" spans="2:9" ht="28.2" thickBot="1">
-      <c r="B13" s="39" t="s">
+      <c r="B13" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="40"/>
-      <c r="D13" s="41" t="s">
+      <c r="C13" s="54"/>
+      <c r="D13" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="37"/>
-      <c r="F13" s="35"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="40"/>
       <c r="G13" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H13" s="41" t="s">
+      <c r="H13" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="I13" s="35"/>
+      <c r="I13" s="40"/>
     </row>
     <row r="14" spans="2:9" ht="15" thickBot="1">
-      <c r="B14" s="34" t="s">
+      <c r="B14" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="35"/>
-      <c r="D14" s="42" t="s">
+      <c r="C14" s="40"/>
+      <c r="D14" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="43"/>
-      <c r="I14" s="44"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="37"/>
     </row>
     <row r="15" spans="2:9" ht="15" thickBot="1">
-      <c r="B15" s="34" t="s">
+      <c r="B15" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="35"/>
-      <c r="D15" s="36" t="s">
+      <c r="C15" s="40"/>
+      <c r="D15" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="39"/>
       <c r="G15" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H15" s="38">
+      <c r="H15" s="59">
         <v>45734</v>
       </c>
-      <c r="I15" s="35"/>
+      <c r="I15" s="40"/>
     </row>
     <row r="16" spans="2:9" ht="42" thickBot="1">
-      <c r="B16" s="47" t="s">
+      <c r="B16" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="48"/>
+      <c r="C16" s="52"/>
       <c r="D16" s="3" t="s">
         <v>7</v>
       </c>
@@ -1827,31 +1483,31 @@
       <c r="I16" s="5"/>
     </row>
     <row r="17" spans="2:9" ht="28.95" customHeight="1" thickBot="1">
-      <c r="B17" s="49" t="s">
+      <c r="B17" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="50"/>
-      <c r="D17" s="51" t="s">
+      <c r="C17" s="42"/>
+      <c r="D17" s="61" t="s">
         <v>36</v>
       </c>
-      <c r="E17" s="52"/>
-      <c r="F17" s="52"/>
-      <c r="G17" s="52"/>
-      <c r="H17" s="52"/>
-      <c r="I17" s="53"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="44"/>
+      <c r="I17" s="45"/>
     </row>
     <row r="18" spans="2:9" ht="28.2" thickBot="1">
       <c r="B18" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="54" t="s">
+      <c r="C18" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="55"/>
-      <c r="E18" s="54" t="s">
+      <c r="D18" s="47"/>
+      <c r="E18" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="F18" s="56"/>
+      <c r="F18" s="48"/>
       <c r="G18" s="10" t="s">
         <v>14</v>
       </c>
@@ -1866,14 +1522,14 @@
       <c r="B19" s="13">
         <v>1</v>
       </c>
-      <c r="C19" s="57" t="s">
+      <c r="C19" s="60" t="s">
         <v>34</v>
       </c>
-      <c r="D19" s="58"/>
-      <c r="E19" s="57" t="s">
+      <c r="D19" s="50"/>
+      <c r="E19" s="60" t="s">
         <v>33</v>
       </c>
-      <c r="F19" s="58"/>
+      <c r="F19" s="50"/>
       <c r="G19" s="14" t="s">
         <v>35</v>
       </c>
@@ -1884,86 +1540,86 @@
       <c r="B20" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="45" t="s">
+      <c r="C20" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="43"/>
-      <c r="E20" s="43"/>
-      <c r="F20" s="43"/>
-      <c r="G20" s="43"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="35"/>
+      <c r="G20" s="35"/>
       <c r="H20" s="7" t="s">
         <v>19</v>
       </c>
       <c r="I20" s="6"/>
     </row>
     <row r="21" spans="2:9" ht="15" thickBot="1">
-      <c r="B21" s="46" t="s">
+      <c r="B21" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="44"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="37"/>
-      <c r="G21" s="37"/>
-      <c r="H21" s="37"/>
-      <c r="I21" s="35"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="39"/>
+      <c r="G21" s="39"/>
+      <c r="H21" s="39"/>
+      <c r="I21" s="40"/>
     </row>
     <row r="22" spans="2:9" ht="15" thickBot="1"/>
     <row r="23" spans="2:9" ht="28.2" thickBot="1">
-      <c r="B23" s="39" t="s">
+      <c r="B23" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="C23" s="40"/>
-      <c r="D23" s="41" t="s">
+      <c r="C23" s="54"/>
+      <c r="D23" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="E23" s="37"/>
-      <c r="F23" s="35"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="40"/>
       <c r="G23" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H23" s="59" t="s">
+      <c r="H23" s="56" t="s">
         <v>37</v>
       </c>
-      <c r="I23" s="35"/>
+      <c r="I23" s="40"/>
     </row>
     <row r="24" spans="2:9" ht="15" thickBot="1">
-      <c r="B24" s="34" t="s">
+      <c r="B24" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="C24" s="35"/>
-      <c r="D24" s="42" t="s">
+      <c r="C24" s="40"/>
+      <c r="D24" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="E24" s="43"/>
-      <c r="F24" s="43"/>
-      <c r="G24" s="43"/>
-      <c r="H24" s="43"/>
-      <c r="I24" s="44"/>
+      <c r="E24" s="35"/>
+      <c r="F24" s="35"/>
+      <c r="G24" s="35"/>
+      <c r="H24" s="35"/>
+      <c r="I24" s="37"/>
     </row>
     <row r="25" spans="2:9" ht="15" thickBot="1">
-      <c r="B25" s="34" t="s">
+      <c r="B25" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="C25" s="35"/>
-      <c r="D25" s="36" t="s">
+      <c r="C25" s="40"/>
+      <c r="D25" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="E25" s="37"/>
-      <c r="F25" s="37"/>
+      <c r="E25" s="39"/>
+      <c r="F25" s="39"/>
       <c r="G25" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H25" s="38">
+      <c r="H25" s="59">
         <v>45734</v>
       </c>
-      <c r="I25" s="35"/>
+      <c r="I25" s="40"/>
     </row>
     <row r="26" spans="2:9" ht="24.6" thickBot="1">
-      <c r="B26" s="47" t="s">
+      <c r="B26" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="48"/>
+      <c r="C26" s="52"/>
       <c r="D26" s="3" t="s">
         <v>7</v>
       </c>
@@ -1980,31 +1636,31 @@
       <c r="I26" s="5"/>
     </row>
     <row r="27" spans="2:9" ht="32.4" customHeight="1" thickBot="1">
-      <c r="B27" s="49" t="s">
+      <c r="B27" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="50"/>
-      <c r="D27" s="60" t="s">
+      <c r="C27" s="42"/>
+      <c r="D27" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="E27" s="52"/>
-      <c r="F27" s="52"/>
-      <c r="G27" s="52"/>
-      <c r="H27" s="52"/>
-      <c r="I27" s="53"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="44"/>
+      <c r="G27" s="44"/>
+      <c r="H27" s="44"/>
+      <c r="I27" s="45"/>
     </row>
     <row r="28" spans="2:9" ht="28.2" thickBot="1">
       <c r="B28" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="54" t="s">
+      <c r="C28" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="D28" s="55"/>
-      <c r="E28" s="54" t="s">
+      <c r="D28" s="47"/>
+      <c r="E28" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="F28" s="56"/>
+      <c r="F28" s="48"/>
       <c r="G28" s="10" t="s">
         <v>14</v>
       </c>
@@ -2019,14 +1675,14 @@
       <c r="B29" s="13">
         <v>1</v>
       </c>
-      <c r="C29" s="61" t="s">
+      <c r="C29" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="D29" s="58"/>
-      <c r="E29" s="61" t="s">
+      <c r="D29" s="50"/>
+      <c r="E29" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="F29" s="58"/>
+      <c r="F29" s="50"/>
       <c r="G29" s="17" t="s">
         <v>44</v>
       </c>
@@ -2037,53 +1693,50 @@
       <c r="B30" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C30" s="45" t="s">
+      <c r="C30" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="D30" s="43"/>
-      <c r="E30" s="43"/>
-      <c r="F30" s="43"/>
-      <c r="G30" s="43"/>
+      <c r="D30" s="35"/>
+      <c r="E30" s="35"/>
+      <c r="F30" s="35"/>
+      <c r="G30" s="35"/>
       <c r="H30" s="7" t="s">
         <v>19</v>
       </c>
       <c r="I30" s="6"/>
     </row>
     <row r="31" spans="2:9" ht="15" thickBot="1">
-      <c r="B31" s="46" t="s">
+      <c r="B31" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="C31" s="44"/>
-      <c r="D31" s="36"/>
-      <c r="E31" s="37"/>
-      <c r="F31" s="37"/>
-      <c r="G31" s="37"/>
-      <c r="H31" s="37"/>
-      <c r="I31" s="35"/>
+      <c r="C31" s="37"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="39"/>
+      <c r="F31" s="39"/>
+      <c r="G31" s="39"/>
+      <c r="H31" s="39"/>
+      <c r="I31" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:I31"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D27:I27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:I21"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:I24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:I4"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:I11"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:I7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="E19:F19"/>
     <mergeCell ref="B13:C13"/>
@@ -2099,24 +1752,27 @@
     <mergeCell ref="D17:I17"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="E18:F18"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:I11"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:I7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:I4"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:I21"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:I24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:I31"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D27:I27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:F29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2124,222 +1780,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7081FA0-4B60-41EA-8343-4988B4EF9AE5}">
-  <dimension ref="B1:I11"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="92" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:I6"/>
+    <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="92" workbookViewId="0">
+      <selection activeCell="Q25" sqref="Q25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
-  <cols>
-    <col min="7" max="7" width="21.109375" customWidth="1"/>
-    <col min="8" max="8" width="18.5546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:9" ht="15" thickBot="1"/>
-    <row r="2" spans="2:9" ht="15" thickBot="1">
-      <c r="B2" s="39" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="59" t="s">
-        <v>49</v>
-      </c>
-      <c r="E2" s="37"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="H2" s="59" t="s">
-        <v>46</v>
-      </c>
-      <c r="I2" s="35"/>
-    </row>
-    <row r="3" spans="2:9" ht="15" thickBot="1">
-      <c r="B3" s="34" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="35"/>
-      <c r="D3" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="44"/>
-    </row>
-    <row r="4" spans="2:9" ht="15" thickBot="1">
-      <c r="B4" s="34" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="36" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H4" s="38">
-        <v>45747</v>
-      </c>
-      <c r="I4" s="35"/>
-    </row>
-    <row r="5" spans="2:9" ht="24.6" thickBot="1">
-      <c r="B5" s="47" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="48"/>
-      <c r="D5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="I5" s="5"/>
-    </row>
-    <row r="6" spans="2:9" ht="42.6" customHeight="1" thickBot="1">
-      <c r="B6" s="49" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="50"/>
-      <c r="D6" s="60" t="s">
-        <v>97</v>
-      </c>
-      <c r="E6" s="52"/>
-      <c r="F6" s="52"/>
-      <c r="G6" s="52"/>
-      <c r="H6" s="52"/>
-      <c r="I6" s="53"/>
-    </row>
-    <row r="7" spans="2:9" ht="28.2" thickBot="1">
-      <c r="B7" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="54" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="55"/>
-      <c r="E7" s="54" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="56"/>
-      <c r="G7" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="I7" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" ht="190.2" customHeight="1" thickBot="1">
-      <c r="B8" s="81">
-        <v>1</v>
-      </c>
-      <c r="C8" s="82" t="s">
-        <v>98</v>
-      </c>
-      <c r="D8" s="83"/>
-      <c r="E8" s="82" t="s">
-        <v>99</v>
-      </c>
-      <c r="F8" s="83"/>
-      <c r="G8" s="84" t="s">
-        <v>104</v>
-      </c>
-      <c r="H8" s="84" t="s">
-        <v>106</v>
-      </c>
-      <c r="I8" s="84" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" ht="190.2" customHeight="1" thickBot="1">
-      <c r="B9" s="85">
-        <v>2</v>
-      </c>
-      <c r="C9" s="63" t="s">
-        <v>102</v>
-      </c>
-      <c r="D9" s="64"/>
-      <c r="E9" s="87" t="s">
-        <v>103</v>
-      </c>
-      <c r="F9" s="88"/>
-      <c r="G9" s="86" t="s">
-        <v>105</v>
-      </c>
-      <c r="H9" s="86" t="s">
-        <v>107</v>
-      </c>
-      <c r="I9" s="17" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" ht="15" thickBot="1">
-      <c r="B10" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="45" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="I10" s="6"/>
-    </row>
-    <row r="11" spans="2:9" ht="15" thickBot="1">
-      <c r="B11" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="44"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="37"/>
-      <c r="H11" s="37"/>
-      <c r="I11" s="35"/>
-    </row>
-  </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:I11"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:I3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:I6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:F7"/>
-  </mergeCells>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
@@ -2357,65 +1805,65 @@
   <sheetData>
     <row r="2" spans="2:9" ht="15" thickBot="1"/>
     <row r="3" spans="2:9" ht="28.2" thickBot="1">
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="40"/>
-      <c r="D3" s="59" t="s">
+      <c r="C3" s="54"/>
+      <c r="D3" s="56" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="37"/>
-      <c r="F3" s="35"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="40"/>
       <c r="G3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="59" t="s">
-        <v>59</v>
-      </c>
-      <c r="I3" s="35"/>
+      <c r="H3" s="56" t="s">
+        <v>58</v>
+      </c>
+      <c r="I3" s="40"/>
     </row>
     <row r="4" spans="2:9" ht="15" thickBot="1">
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="44"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="58" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="37"/>
     </row>
     <row r="5" spans="2:9" ht="15" thickBot="1">
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="35"/>
-      <c r="D5" s="62" t="s">
+      <c r="C5" s="40"/>
+      <c r="D5" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
       <c r="G5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="38">
+      <c r="H5" s="59">
         <v>45734</v>
       </c>
-      <c r="I5" s="35"/>
+      <c r="I5" s="40"/>
     </row>
     <row r="6" spans="2:9" ht="42" thickBot="1">
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="48"/>
+      <c r="C6" s="52"/>
       <c r="D6" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>8</v>
@@ -2427,31 +1875,31 @@
       <c r="I6" s="5"/>
     </row>
     <row r="7" spans="2:9" ht="33" customHeight="1" thickBot="1">
-      <c r="B7" s="49" t="s">
+      <c r="B7" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="50"/>
-      <c r="D7" s="60" t="s">
-        <v>60</v>
-      </c>
-      <c r="E7" s="52"/>
-      <c r="F7" s="52"/>
-      <c r="G7" s="52"/>
-      <c r="H7" s="52"/>
-      <c r="I7" s="53"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="44"/>
+      <c r="H7" s="44"/>
+      <c r="I7" s="45"/>
     </row>
     <row r="8" spans="2:9" ht="28.2" thickBot="1">
       <c r="B8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="54" t="s">
+      <c r="C8" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="55"/>
-      <c r="E8" s="54" t="s">
+      <c r="D8" s="47"/>
+      <c r="E8" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="56"/>
+      <c r="F8" s="48"/>
       <c r="G8" s="10" t="s">
         <v>14</v>
       </c>
@@ -2466,14 +1914,14 @@
       <c r="B9" s="13">
         <v>1</v>
       </c>
-      <c r="C9" s="61" t="s">
+      <c r="C9" s="49" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="50"/>
+      <c r="E9" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="D9" s="58"/>
-      <c r="E9" s="61" t="s">
-        <v>62</v>
-      </c>
-      <c r="F9" s="58"/>
+      <c r="F9" s="50"/>
       <c r="G9" s="14" t="s">
         <v>27</v>
       </c>
@@ -2484,32 +1932,40 @@
       <c r="B10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="45" t="s">
+      <c r="C10" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="35"/>
       <c r="H10" s="7" t="s">
         <v>19</v>
       </c>
       <c r="I10" s="6"/>
     </row>
     <row r="11" spans="2:9" ht="15" thickBot="1">
-      <c r="B11" s="46" t="s">
+      <c r="B11" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="44"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="37"/>
-      <c r="H11" s="37"/>
-      <c r="I11" s="35"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:I4"/>
     <mergeCell ref="C10:G10"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="D11:I11"/>
@@ -2520,14 +1976,6 @@
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="E9:F9"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2545,60 +1993,60 @@
   <sheetData>
     <row r="3" spans="2:9" ht="15" thickBot="1"/>
     <row r="4" spans="2:9" ht="28.2" thickBot="1">
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="D4" s="59" t="s">
-        <v>56</v>
-      </c>
-      <c r="E4" s="37"/>
-      <c r="F4" s="35"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="56" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" s="39"/>
+      <c r="F4" s="40"/>
       <c r="G4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="59" t="s">
+      <c r="H4" s="56" t="s">
+        <v>49</v>
+      </c>
+      <c r="I4" s="40"/>
+    </row>
+    <row r="5" spans="2:9" ht="15" thickBot="1">
+      <c r="B5" s="57" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="40"/>
+      <c r="D5" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="I4" s="35"/>
-    </row>
-    <row r="5" spans="2:9" ht="15" thickBot="1">
-      <c r="B5" s="34" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="35"/>
-      <c r="D5" s="42" t="s">
-        <v>51</v>
-      </c>
-      <c r="E5" s="43"/>
-      <c r="F5" s="43"/>
-      <c r="G5" s="43"/>
-      <c r="H5" s="43"/>
-      <c r="I5" s="44"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="37"/>
     </row>
     <row r="6" spans="2:9" ht="15" thickBot="1">
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="35"/>
-      <c r="D6" s="36" t="s">
+      <c r="C6" s="40"/>
+      <c r="D6" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
       <c r="G6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="38">
+      <c r="H6" s="59">
         <v>45734</v>
       </c>
-      <c r="I6" s="35"/>
+      <c r="I6" s="40"/>
     </row>
     <row r="7" spans="2:9" ht="24.6" thickBot="1">
-      <c r="B7" s="47" t="s">
+      <c r="B7" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="48"/>
+      <c r="C7" s="52"/>
       <c r="D7" s="3" t="s">
         <v>7</v>
       </c>
@@ -2613,31 +2061,31 @@
       <c r="I7" s="5"/>
     </row>
     <row r="8" spans="2:9" ht="28.95" customHeight="1" thickBot="1">
-      <c r="B8" s="49" t="s">
+      <c r="B8" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="50"/>
-      <c r="D8" s="60" t="s">
-        <v>52</v>
-      </c>
-      <c r="E8" s="52"/>
-      <c r="F8" s="52"/>
-      <c r="G8" s="52"/>
-      <c r="H8" s="52"/>
-      <c r="I8" s="53"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="45"/>
     </row>
     <row r="9" spans="2:9" ht="28.2" thickBot="1">
       <c r="B9" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="54" t="s">
+      <c r="C9" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="55"/>
-      <c r="E9" s="54" t="s">
+      <c r="D9" s="47"/>
+      <c r="E9" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="56"/>
+      <c r="F9" s="48"/>
       <c r="G9" s="10" t="s">
         <v>14</v>
       </c>
@@ -2652,16 +2100,16 @@
       <c r="B10" s="13">
         <v>1</v>
       </c>
-      <c r="C10" s="61" t="s">
+      <c r="C10" s="49" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="50"/>
+      <c r="E10" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="D10" s="58"/>
-      <c r="E10" s="61" t="s">
+      <c r="F10" s="50"/>
+      <c r="G10" s="17" t="s">
         <v>54</v>
-      </c>
-      <c r="F10" s="58"/>
-      <c r="G10" s="17" t="s">
-        <v>55</v>
       </c>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
@@ -2670,32 +2118,40 @@
       <c r="B11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="45" t="s">
+      <c r="C11" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
       <c r="H11" s="7" t="s">
         <v>19</v>
       </c>
       <c r="I11" s="6"/>
     </row>
     <row r="12" spans="2:9" ht="15" thickBot="1">
-      <c r="B12" s="46" t="s">
+      <c r="B12" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="44"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
-      <c r="I12" s="35"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:I5"/>
     <mergeCell ref="C11:G11"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="D12:I12"/>
@@ -2706,14 +2162,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="E10:F10"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:I5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2731,60 +2179,60 @@
   <sheetData>
     <row r="1" spans="2:9" ht="15" thickBot="1"/>
     <row r="2" spans="2:9" ht="28.2" thickBot="1">
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="59" t="s">
-        <v>57</v>
-      </c>
-      <c r="E2" s="37"/>
-      <c r="F2" s="35"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="56" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="39"/>
+      <c r="F2" s="40"/>
       <c r="G2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="59" t="s">
+      <c r="H2" s="56" t="s">
+        <v>62</v>
+      </c>
+      <c r="I2" s="40"/>
+    </row>
+    <row r="3" spans="2:9" ht="15" customHeight="1" thickBot="1">
+      <c r="B3" s="57" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="40"/>
+      <c r="D3" s="58" t="s">
         <v>63</v>
       </c>
-      <c r="I2" s="35"/>
-    </row>
-    <row r="3" spans="2:9" ht="15" customHeight="1" thickBot="1">
-      <c r="B3" s="34" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="35"/>
-      <c r="D3" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="44"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="37"/>
     </row>
     <row r="4" spans="2:9" ht="15" thickBot="1">
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="36" t="s">
+      <c r="C4" s="40"/>
+      <c r="D4" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
       <c r="G4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="38">
+      <c r="H4" s="59">
         <v>45734</v>
       </c>
-      <c r="I4" s="35"/>
+      <c r="I4" s="40"/>
     </row>
     <row r="5" spans="2:9" ht="24.6" thickBot="1">
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="48"/>
+      <c r="C5" s="52"/>
       <c r="D5" s="3" t="s">
         <v>7</v>
       </c>
@@ -2793,7 +2241,7 @@
         <v>8</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H5" s="16" t="s">
         <v>41</v>
@@ -2801,31 +2249,31 @@
       <c r="I5" s="5"/>
     </row>
     <row r="6" spans="2:9" ht="15" thickBot="1">
-      <c r="B6" s="49" t="s">
+      <c r="B6" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="50"/>
-      <c r="D6" s="60" t="s">
-        <v>66</v>
-      </c>
-      <c r="E6" s="52"/>
-      <c r="F6" s="52"/>
-      <c r="G6" s="52"/>
-      <c r="H6" s="52"/>
-      <c r="I6" s="53"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="45"/>
     </row>
     <row r="7" spans="2:9" ht="28.2" thickBot="1">
       <c r="B7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="54" t="s">
+      <c r="C7" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="55"/>
-      <c r="E7" s="54" t="s">
+      <c r="D7" s="47"/>
+      <c r="E7" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="56"/>
+      <c r="F7" s="48"/>
       <c r="G7" s="10" t="s">
         <v>14</v>
       </c>
@@ -2840,16 +2288,16 @@
       <c r="B8" s="13">
         <v>1</v>
       </c>
-      <c r="C8" s="61" t="s">
+      <c r="C8" s="49" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" s="50"/>
+      <c r="E8" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="D8" s="58"/>
-      <c r="E8" s="61" t="s">
+      <c r="F8" s="50"/>
+      <c r="G8" s="17" t="s">
         <v>68</v>
-      </c>
-      <c r="F8" s="58"/>
-      <c r="G8" s="17" t="s">
-        <v>69</v>
       </c>
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
@@ -2858,16 +2306,16 @@
       <c r="B9" s="13">
         <v>2</v>
       </c>
-      <c r="C9" s="63" t="s">
+      <c r="C9" s="62" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" s="63"/>
+      <c r="E9" s="62" t="s">
         <v>70</v>
       </c>
-      <c r="D9" s="64"/>
-      <c r="E9" s="63" t="s">
+      <c r="F9" s="63"/>
+      <c r="G9" s="17" t="s">
         <v>71</v>
-      </c>
-      <c r="F9" s="64"/>
-      <c r="G9" s="17" t="s">
-        <v>72</v>
       </c>
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
@@ -2876,37 +2324,32 @@
       <c r="B10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="45" t="s">
+      <c r="C10" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="35"/>
       <c r="H10" s="7" t="s">
         <v>19</v>
       </c>
       <c r="I10" s="6"/>
     </row>
     <row r="11" spans="2:9" ht="15" thickBot="1">
-      <c r="B11" s="46" t="s">
+      <c r="B11" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="44"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="37"/>
-      <c r="H11" s="37"/>
-      <c r="I11" s="35"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:I11"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="D2:F2"/>
@@ -2922,6 +2365,11 @@
     <mergeCell ref="D6:I6"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:I11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2931,8 +2379,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD219FCF-77B2-490B-816E-2F75E9617605}">
   <dimension ref="B1:H18"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -2945,121 +2393,121 @@
   <sheetData>
     <row r="1" spans="2:6" ht="15" thickBot="1"/>
     <row r="2" spans="2:6" ht="55.2" customHeight="1" thickBot="1">
-      <c r="B2" s="69" t="s">
+      <c r="B2" s="74" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="75"/>
+      <c r="D2" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" s="23" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="15" thickBot="1">
+      <c r="B3" s="76" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="67"/>
+      <c r="D3" s="72" t="s">
+        <v>88</v>
+      </c>
+      <c r="E3" s="66"/>
+      <c r="F3" s="67"/>
+    </row>
+    <row r="4" spans="2:6" ht="15" thickBot="1">
+      <c r="B4" s="77" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="78"/>
+      <c r="D4" s="79" t="s">
         <v>94</v>
       </c>
-      <c r="C2" s="70"/>
-      <c r="D2" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="E2" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="F2" s="23" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" ht="15" thickBot="1">
-      <c r="B3" s="71" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="66"/>
-      <c r="D3" s="67" t="s">
+      <c r="E4" s="80"/>
+      <c r="F4" s="78"/>
+    </row>
+    <row r="5" spans="2:6" ht="15" thickBot="1">
+      <c r="B5" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" s="67"/>
+      <c r="D5" s="72" t="s">
         <v>89</v>
       </c>
-      <c r="E3" s="68"/>
-      <c r="F3" s="66"/>
-    </row>
-    <row r="4" spans="2:6" ht="15" thickBot="1">
-      <c r="B4" s="72" t="s">
-        <v>74</v>
-      </c>
-      <c r="C4" s="73"/>
-      <c r="D4" s="74" t="s">
-        <v>95</v>
-      </c>
-      <c r="E4" s="75"/>
-      <c r="F4" s="73"/>
-    </row>
-    <row r="5" spans="2:6" ht="15" thickBot="1">
-      <c r="B5" s="65" t="s">
+      <c r="E5" s="66"/>
+      <c r="F5" s="67"/>
+    </row>
+    <row r="6" spans="2:6" ht="42" thickBot="1">
+      <c r="B6" s="68" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="66"/>
-      <c r="D5" s="67" t="s">
+      <c r="C6" s="69"/>
+      <c r="D6" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="E5" s="68"/>
-      <c r="F5" s="66"/>
-    </row>
-    <row r="6" spans="2:6" ht="42" thickBot="1">
-      <c r="B6" s="77" t="s">
+      <c r="E6" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="C6" s="78"/>
-      <c r="D6" s="18" t="s">
+      <c r="F6" s="25" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="15" thickBot="1">
+      <c r="B7" s="70" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" s="71"/>
+      <c r="D7" s="71"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="69"/>
+    </row>
+    <row r="8" spans="2:6" ht="18" customHeight="1" thickBot="1">
+      <c r="B8" s="65" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="66"/>
+      <c r="D8" s="67"/>
+      <c r="E8" s="65" t="s">
+        <v>79</v>
+      </c>
+      <c r="F8" s="67"/>
+    </row>
+    <row r="9" spans="2:6" ht="36.6" customHeight="1" thickBot="1">
+      <c r="B9" s="72" t="s">
         <v>91</v>
       </c>
-      <c r="E6" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="F6" s="25" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="15" thickBot="1">
-      <c r="B7" s="79" t="s">
-        <v>78</v>
-      </c>
-      <c r="C7" s="80"/>
-      <c r="D7" s="80"/>
-      <c r="E7" s="80"/>
-      <c r="F7" s="78"/>
-    </row>
-    <row r="8" spans="2:6" ht="18" customHeight="1" thickBot="1">
-      <c r="B8" s="76" t="s">
-        <v>79</v>
-      </c>
-      <c r="C8" s="68"/>
-      <c r="D8" s="66"/>
-      <c r="E8" s="76" t="s">
+      <c r="C9" s="66"/>
+      <c r="D9" s="66"/>
+      <c r="E9" s="72"/>
+      <c r="F9" s="67"/>
+    </row>
+    <row r="10" spans="2:6" ht="15" thickBot="1">
+      <c r="B10" s="65" t="s">
         <v>80</v>
       </c>
-      <c r="F8" s="66"/>
-    </row>
-    <row r="9" spans="2:6" ht="36.6" customHeight="1" thickBot="1">
-      <c r="B9" s="67" t="s">
-        <v>92</v>
-      </c>
-      <c r="C9" s="68"/>
-      <c r="D9" s="68"/>
-      <c r="E9" s="67"/>
-      <c r="F9" s="66"/>
-    </row>
-    <row r="10" spans="2:6" ht="15" thickBot="1">
-      <c r="B10" s="76" t="s">
-        <v>81</v>
-      </c>
-      <c r="C10" s="68"/>
-      <c r="D10" s="68"/>
-      <c r="E10" s="68"/>
-      <c r="F10" s="66"/>
+      <c r="C10" s="66"/>
+      <c r="D10" s="66"/>
+      <c r="E10" s="66"/>
+      <c r="F10" s="67"/>
     </row>
     <row r="11" spans="2:6" ht="20.399999999999999" customHeight="1" thickBot="1">
       <c r="B11" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="C11" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="C11" s="27" t="s">
+      <c r="D11" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="D11" s="27" t="s">
+      <c r="E11" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="E11" s="27" t="s">
+      <c r="F11" s="27" t="s">
         <v>85</v>
-      </c>
-      <c r="F11" s="27" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="27" thickBot="1">
@@ -3112,7 +2560,7 @@
         <v>45</v>
       </c>
       <c r="C15" s="32" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D15" s="30" t="s">
         <v>5</v>
@@ -3124,10 +2572,10 @@
     </row>
     <row r="16" spans="2:6" ht="29.4" thickBot="1">
       <c r="B16" s="28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C16" s="32" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D16" s="30" t="s">
         <v>5</v>
@@ -3139,10 +2587,10 @@
     </row>
     <row r="17" spans="2:8" ht="28.2" thickBot="1">
       <c r="B17" s="28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D17" s="30" t="s">
         <v>5</v>
@@ -3156,10 +2604,10 @@
     </row>
     <row r="18" spans="2:8" ht="29.4" thickBot="1">
       <c r="B18" s="28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C18" s="32" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D18" s="30" t="s">
         <v>5</v>
@@ -3171,6 +2619,13 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:F4"/>
     <mergeCell ref="B10:F10"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B7:F7"/>
@@ -3178,13 +2633,6 @@
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="E9:F9"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:F4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Amélioration du plan de tests
</commit_message>
<xml_diff>
--- a/PEA/Plan de test/Plan de tests - PEA.xlsx
+++ b/PEA/Plan de test/Plan de tests - PEA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robin\Documents\GITHUB\ACCES_CAMPUS\Acc-s-campus-\PEA\Plan de test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5038E7C3-6082-4FD1-92B9-AF8ED54CE6C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2FA7BAB-811C-49F9-B1E0-D1C88635D5A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{21D66C90-57CB-4BB7-B44F-BA6973DF79EF}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="109">
   <si>
     <t>Identification du Test</t>
   </si>
@@ -155,9 +155,6 @@
   </si>
   <si>
     <t>Bon fonctionnement de la séquence - PEA</t>
-  </si>
-  <si>
-    <t>T1.3</t>
   </si>
   <si>
     <t>Le test permet de vérifier que tout le programme s'effectue normalement.</t>
@@ -197,15 +194,9 @@
     <t>T2.1</t>
   </si>
   <si>
-    <t>Le test permet de vérifier que la communication Ethernet est valide.</t>
-  </si>
-  <si>
     <t>Putty</t>
   </si>
   <si>
-    <t>T3.1</t>
-  </si>
-  <si>
     <t>Fonctionnement de la gâche</t>
   </si>
   <si>
@@ -323,18 +314,12 @@
     <t>PEA</t>
   </si>
   <si>
-    <t>Tester le bon fonctionnement du jalon 1 de la PEA</t>
-  </si>
-  <si>
     <t>Laboratoire</t>
   </si>
   <si>
     <t xml:space="preserve">Oscilloscope, multimètre </t>
   </si>
   <si>
-    <t>L'utilisateur doit disposer d'un badge RFID valide et dont il connait l'UID.</t>
-  </si>
-  <si>
     <t>Manipulation d'outils de mesure et d'un serial monitor.</t>
   </si>
   <si>
@@ -342,6 +327,63 @@
   </si>
   <si>
     <t>Tests unitaires</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>Référence du bloc testé :</t>
+  </si>
+  <si>
+    <t xml:space="preserve">W5500 - Interface Ethernet </t>
+  </si>
+  <si>
+    <t>Multimètres</t>
+  </si>
+  <si>
+    <t>Passer le multimètre en mode voltmètres - tension fixe. Placer les pins du multimètre sur les pins 28 et 27.</t>
+  </si>
+  <si>
+    <t>Une tension doit être mesuré sur le multimètre.</t>
+  </si>
+  <si>
+    <t>Si la tension est de 3.3V.</t>
+  </si>
+  <si>
+    <t>Le test permet de vérifier que l'interface Ethernet est alimenté correctement.</t>
+  </si>
+  <si>
+    <t>Tester le bon fonctionnement de la PEA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L'utilisateur doit disposer d'un badge RFID valide et dont il connait l'UID. Le montage doit être </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tester le bon fonctionnement des composants sur PCB </t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>Le test permet de vérifier que l'interface Ethernet communiquer correctement en SPI avec le microcontrolleur</t>
+  </si>
+  <si>
+    <t>W5500 - Interface Ethernet + µC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La PEA doit avoir le code de téléverser dans son microcontrôleur. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Placer les sondes de l'oscilloscope sur les pins 35 (MOSI) et 34 (MISO). Passer le trigger de l'oscilloscope en mode Single pour capturé le signal au premier front.                              Image du schéma : </t>
+  </si>
+  <si>
+    <t>L'oscilloscope dois afficher le résultat suivant : (Capture d'oscilloscope )</t>
+  </si>
+  <si>
+    <t>Le test est réussi si la trame reçu est la même.</t>
+  </si>
+  <si>
+    <t>T2</t>
   </si>
 </sst>
 </file>
@@ -351,7 +393,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -403,6 +445,14 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -705,10 +755,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -803,49 +854,17 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -853,23 +872,58 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -877,14 +931,32 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -893,29 +965,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -929,6 +987,94 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>27598</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>715802</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>740775</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1918538</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C2F71A07-F5F7-95D2-D7C1-ED2639BED21F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1598014" y="2502827"/>
+          <a:ext cx="1498385" cy="1202736"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>34056</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>1339223</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1501008" cy="1202736"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B5505F7-DDAF-4812-8F45-E624CBF70BFE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1609717" y="7151087"/>
+          <a:ext cx="1501008" cy="1202736"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1250,72 +1396,73 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E407FD9-0AE4-4A1C-B2E0-3161C8BCECA8}">
   <dimension ref="B2:I31"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:I4"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
     <col min="6" max="6" width="9.33203125" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" customWidth="1"/>
+    <col min="7" max="7" width="22.21875" customWidth="1"/>
+    <col min="8" max="8" width="19.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="15" thickBot="1"/>
-    <row r="3" spans="2:9" ht="28.2" thickBot="1">
-      <c r="B3" s="53" t="s">
+    <row r="3" spans="2:9" ht="19.2" customHeight="1" thickBot="1">
+      <c r="B3" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="54"/>
-      <c r="D3" s="55" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" s="39"/>
-      <c r="F3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="E3" s="37"/>
+      <c r="F3" s="35"/>
       <c r="G3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H3" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="H3" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="40"/>
+      <c r="I3" s="35"/>
     </row>
     <row r="4" spans="2:9" ht="15" thickBot="1">
-      <c r="B4" s="57" t="s">
+      <c r="B4" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="D4" s="58" t="s">
+      <c r="C4" s="35"/>
+      <c r="D4" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="37"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="44"/>
     </row>
     <row r="5" spans="2:9" ht="15" thickBot="1">
-      <c r="B5" s="57" t="s">
+      <c r="B5" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="40"/>
-      <c r="D5" s="38" t="s">
+      <c r="C5" s="35"/>
+      <c r="D5" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
       <c r="G5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="59">
+      <c r="H5" s="38">
         <v>45734</v>
       </c>
-      <c r="I5" s="40"/>
-    </row>
-    <row r="6" spans="2:9" ht="42" customHeight="1" thickBot="1">
-      <c r="B6" s="51" t="s">
+      <c r="I5" s="35"/>
+    </row>
+    <row r="6" spans="2:9" ht="18.600000000000001" customHeight="1" thickBot="1">
+      <c r="B6" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="52"/>
+      <c r="C6" s="48"/>
       <c r="D6" s="3" t="s">
         <v>7</v>
       </c>
@@ -1330,32 +1477,32 @@
       </c>
       <c r="I6" s="5"/>
     </row>
-    <row r="7" spans="2:9" ht="46.2" customHeight="1" thickBot="1">
-      <c r="B7" s="41" t="s">
+    <row r="7" spans="2:9" ht="31.8" customHeight="1" thickBot="1">
+      <c r="B7" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="42"/>
-      <c r="D7" s="61" t="s">
+      <c r="C7" s="50"/>
+      <c r="D7" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="44"/>
-      <c r="F7" s="44"/>
-      <c r="G7" s="44"/>
-      <c r="H7" s="44"/>
-      <c r="I7" s="45"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="52"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="53"/>
     </row>
     <row r="8" spans="2:9" ht="28.2" thickBot="1">
       <c r="B8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="46" t="s">
+      <c r="C8" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="47"/>
-      <c r="E8" s="46" t="s">
+      <c r="D8" s="55"/>
+      <c r="E8" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="48"/>
+      <c r="F8" s="56"/>
       <c r="G8" s="10" t="s">
         <v>14</v>
       </c>
@@ -1370,14 +1517,14 @@
       <c r="B9" s="13">
         <v>1</v>
       </c>
-      <c r="C9" s="60" t="s">
+      <c r="C9" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="50"/>
-      <c r="E9" s="60" t="s">
+      <c r="D9" s="58"/>
+      <c r="E9" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="50"/>
+      <c r="F9" s="58"/>
       <c r="G9" s="14" t="s">
         <v>27</v>
       </c>
@@ -1388,86 +1535,86 @@
       <c r="B10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="34" t="s">
+      <c r="C10" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
       <c r="H10" s="7" t="s">
         <v>19</v>
       </c>
       <c r="I10" s="6"/>
     </row>
     <row r="11" spans="2:9" ht="28.95" customHeight="1" thickBot="1">
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="37"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="40"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="35"/>
     </row>
     <row r="12" spans="2:9" ht="15" thickBot="1"/>
     <row r="13" spans="2:9" ht="28.2" thickBot="1">
-      <c r="B13" s="53" t="s">
+      <c r="B13" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="54"/>
-      <c r="D13" s="55" t="s">
+      <c r="C13" s="40"/>
+      <c r="D13" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="39"/>
-      <c r="F13" s="40"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="35"/>
       <c r="G13" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H13" s="55" t="s">
+      <c r="H13" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="I13" s="40"/>
+      <c r="I13" s="35"/>
     </row>
     <row r="14" spans="2:9" ht="15" thickBot="1">
-      <c r="B14" s="57" t="s">
+      <c r="B14" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="40"/>
-      <c r="D14" s="58" t="s">
+      <c r="C14" s="35"/>
+      <c r="D14" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="37"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="44"/>
     </row>
     <row r="15" spans="2:9" ht="15" thickBot="1">
-      <c r="B15" s="57" t="s">
+      <c r="B15" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="40"/>
-      <c r="D15" s="38" t="s">
+      <c r="C15" s="35"/>
+      <c r="D15" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="39"/>
-      <c r="F15" s="39"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
       <c r="G15" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H15" s="59">
+      <c r="H15" s="38">
         <v>45734</v>
       </c>
-      <c r="I15" s="40"/>
+      <c r="I15" s="35"/>
     </row>
     <row r="16" spans="2:9" ht="42" thickBot="1">
-      <c r="B16" s="51" t="s">
+      <c r="B16" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="52"/>
+      <c r="C16" s="48"/>
       <c r="D16" s="3" t="s">
         <v>7</v>
       </c>
@@ -1483,31 +1630,31 @@
       <c r="I16" s="5"/>
     </row>
     <row r="17" spans="2:9" ht="28.95" customHeight="1" thickBot="1">
-      <c r="B17" s="41" t="s">
+      <c r="B17" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="42"/>
-      <c r="D17" s="61" t="s">
+      <c r="C17" s="50"/>
+      <c r="D17" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="E17" s="44"/>
-      <c r="F17" s="44"/>
-      <c r="G17" s="44"/>
-      <c r="H17" s="44"/>
-      <c r="I17" s="45"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="52"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="52"/>
+      <c r="I17" s="53"/>
     </row>
     <row r="18" spans="2:9" ht="28.2" thickBot="1">
       <c r="B18" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="46" t="s">
+      <c r="C18" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="47"/>
-      <c r="E18" s="46" t="s">
+      <c r="D18" s="55"/>
+      <c r="E18" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="F18" s="48"/>
+      <c r="F18" s="56"/>
       <c r="G18" s="10" t="s">
         <v>14</v>
       </c>
@@ -1522,14 +1669,14 @@
       <c r="B19" s="13">
         <v>1</v>
       </c>
-      <c r="C19" s="60" t="s">
+      <c r="C19" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="D19" s="50"/>
-      <c r="E19" s="60" t="s">
+      <c r="D19" s="58"/>
+      <c r="E19" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="F19" s="50"/>
+      <c r="F19" s="58"/>
       <c r="G19" s="14" t="s">
         <v>35</v>
       </c>
@@ -1540,127 +1687,127 @@
       <c r="B20" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="34" t="s">
+      <c r="C20" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="35"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="35"/>
-      <c r="G20" s="35"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="43"/>
       <c r="H20" s="7" t="s">
         <v>19</v>
       </c>
       <c r="I20" s="6"/>
     </row>
     <row r="21" spans="2:9" ht="15" thickBot="1">
-      <c r="B21" s="36" t="s">
+      <c r="B21" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="37"/>
-      <c r="D21" s="38"/>
-      <c r="E21" s="39"/>
-      <c r="F21" s="39"/>
-      <c r="G21" s="39"/>
-      <c r="H21" s="39"/>
-      <c r="I21" s="40"/>
+      <c r="C21" s="44"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="37"/>
+      <c r="G21" s="37"/>
+      <c r="H21" s="37"/>
+      <c r="I21" s="35"/>
     </row>
     <row r="22" spans="2:9" ht="15" thickBot="1"/>
     <row r="23" spans="2:9" ht="28.2" thickBot="1">
-      <c r="B23" s="53" t="s">
+      <c r="B23" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C23" s="54"/>
-      <c r="D23" s="55" t="s">
+      <c r="C23" s="40"/>
+      <c r="D23" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="E23" s="39"/>
-      <c r="F23" s="40"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="35"/>
       <c r="G23" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H23" s="56" t="s">
+      <c r="H23" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="I23" s="40"/>
+      <c r="I23" s="35"/>
     </row>
     <row r="24" spans="2:9" ht="15" thickBot="1">
-      <c r="B24" s="57" t="s">
+      <c r="B24" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="C24" s="40"/>
-      <c r="D24" s="58" t="s">
-        <v>39</v>
-      </c>
-      <c r="E24" s="35"/>
-      <c r="F24" s="35"/>
-      <c r="G24" s="35"/>
-      <c r="H24" s="35"/>
-      <c r="I24" s="37"/>
+      <c r="C24" s="35"/>
+      <c r="D24" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="E24" s="43"/>
+      <c r="F24" s="43"/>
+      <c r="G24" s="43"/>
+      <c r="H24" s="43"/>
+      <c r="I24" s="44"/>
     </row>
     <row r="25" spans="2:9" ht="15" thickBot="1">
-      <c r="B25" s="57" t="s">
+      <c r="B25" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="C25" s="40"/>
-      <c r="D25" s="38" t="s">
+      <c r="C25" s="35"/>
+      <c r="D25" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="E25" s="39"/>
-      <c r="F25" s="39"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="37"/>
       <c r="G25" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H25" s="59">
+      <c r="H25" s="38">
         <v>45734</v>
       </c>
-      <c r="I25" s="40"/>
+      <c r="I25" s="35"/>
     </row>
     <row r="26" spans="2:9" ht="24.6" thickBot="1">
-      <c r="B26" s="51" t="s">
+      <c r="B26" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="52"/>
+      <c r="C26" s="48"/>
       <c r="D26" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>8</v>
       </c>
       <c r="G26" s="6"/>
       <c r="H26" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I26" s="5"/>
     </row>
     <row r="27" spans="2:9" ht="32.4" customHeight="1" thickBot="1">
-      <c r="B27" s="41" t="s">
+      <c r="B27" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="42"/>
-      <c r="D27" s="43" t="s">
+      <c r="C27" s="50"/>
+      <c r="D27" s="60" t="s">
         <v>36</v>
       </c>
-      <c r="E27" s="44"/>
-      <c r="F27" s="44"/>
-      <c r="G27" s="44"/>
-      <c r="H27" s="44"/>
-      <c r="I27" s="45"/>
+      <c r="E27" s="52"/>
+      <c r="F27" s="52"/>
+      <c r="G27" s="52"/>
+      <c r="H27" s="52"/>
+      <c r="I27" s="53"/>
     </row>
     <row r="28" spans="2:9" ht="28.2" thickBot="1">
       <c r="B28" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="46" t="s">
+      <c r="C28" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="D28" s="47"/>
-      <c r="E28" s="46" t="s">
+      <c r="D28" s="55"/>
+      <c r="E28" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="F28" s="48"/>
+      <c r="F28" s="56"/>
       <c r="G28" s="10" t="s">
         <v>14</v>
       </c>
@@ -1675,16 +1822,16 @@
       <c r="B29" s="13">
         <v>1</v>
       </c>
-      <c r="C29" s="49" t="s">
+      <c r="C29" s="61" t="s">
+        <v>41</v>
+      </c>
+      <c r="D29" s="58"/>
+      <c r="E29" s="61" t="s">
         <v>42</v>
       </c>
-      <c r="D29" s="50"/>
-      <c r="E29" s="49" t="s">
+      <c r="F29" s="58"/>
+      <c r="G29" s="17" t="s">
         <v>43</v>
-      </c>
-      <c r="F29" s="50"/>
-      <c r="G29" s="17" t="s">
-        <v>44</v>
       </c>
       <c r="H29" s="14"/>
       <c r="I29" s="14"/>
@@ -1693,50 +1840,53 @@
       <c r="B30" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C30" s="34" t="s">
+      <c r="C30" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="D30" s="35"/>
-      <c r="E30" s="35"/>
-      <c r="F30" s="35"/>
-      <c r="G30" s="35"/>
+      <c r="D30" s="43"/>
+      <c r="E30" s="43"/>
+      <c r="F30" s="43"/>
+      <c r="G30" s="43"/>
       <c r="H30" s="7" t="s">
         <v>19</v>
       </c>
       <c r="I30" s="6"/>
     </row>
     <row r="31" spans="2:9" ht="15" thickBot="1">
-      <c r="B31" s="36" t="s">
+      <c r="B31" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="C31" s="37"/>
-      <c r="D31" s="38"/>
-      <c r="E31" s="39"/>
-      <c r="F31" s="39"/>
-      <c r="G31" s="39"/>
-      <c r="H31" s="39"/>
-      <c r="I31" s="40"/>
+      <c r="C31" s="44"/>
+      <c r="D31" s="36"/>
+      <c r="E31" s="37"/>
+      <c r="F31" s="37"/>
+      <c r="G31" s="37"/>
+      <c r="H31" s="37"/>
+      <c r="I31" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:I4"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:I11"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:I7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:I31"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D27:I27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:I21"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:I24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="H25:I25"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="E19:F19"/>
     <mergeCell ref="B13:C13"/>
@@ -1752,27 +1902,24 @@
     <mergeCell ref="D17:I17"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="E18:F18"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:I21"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:I24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:I31"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D27:I27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:I11"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:I7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1780,16 +1927,332 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7081FA0-4B60-41EA-8343-4988B4EF9AE5}">
-  <dimension ref="A1"/>
+  <dimension ref="B2:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="92" workbookViewId="0">
-      <selection activeCell="Q25" sqref="Q25"/>
+    <sheetView tabSelected="1" zoomScale="118" zoomScaleNormal="92" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
-  <sheetData/>
+  <cols>
+    <col min="7" max="7" width="17.21875" customWidth="1"/>
+    <col min="8" max="8" width="19.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9" ht="15" thickBot="1"/>
+    <row r="3" spans="2:9" ht="18.600000000000001" customHeight="1" thickBot="1">
+      <c r="B3" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="40"/>
+      <c r="D3" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="E3" s="37"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="82" t="s">
+        <v>91</v>
+      </c>
+      <c r="H3" s="41" t="s">
+        <v>92</v>
+      </c>
+      <c r="I3" s="35"/>
+    </row>
+    <row r="4" spans="2:9" ht="15" thickBot="1">
+      <c r="B4" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="35"/>
+      <c r="D4" s="42" t="s">
+        <v>97</v>
+      </c>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="44"/>
+    </row>
+    <row r="5" spans="2:9" ht="15" thickBot="1">
+      <c r="B5" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="35"/>
+      <c r="D5" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="38"/>
+      <c r="I5" s="35"/>
+    </row>
+    <row r="6" spans="2:9" ht="19.8" customHeight="1" thickBot="1">
+      <c r="B6" s="47" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="48"/>
+      <c r="D6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="5"/>
+    </row>
+    <row r="7" spans="2:9" ht="15" thickBot="1">
+      <c r="B7" s="49" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="50"/>
+      <c r="D7" s="51" t="s">
+        <v>104</v>
+      </c>
+      <c r="E7" s="52"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="52"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="53"/>
+    </row>
+    <row r="8" spans="2:9" ht="28.2" thickBot="1">
+      <c r="B8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="54" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="55"/>
+      <c r="E8" s="54" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="56"/>
+      <c r="G8" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" ht="162" customHeight="1" thickBot="1">
+      <c r="B9" s="13">
+        <v>1</v>
+      </c>
+      <c r="C9" s="57" t="s">
+        <v>94</v>
+      </c>
+      <c r="D9" s="58"/>
+      <c r="E9" s="57" t="s">
+        <v>95</v>
+      </c>
+      <c r="F9" s="58"/>
+      <c r="G9" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+    </row>
+    <row r="10" spans="2:9" ht="15" thickBot="1">
+      <c r="B10" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="45" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I10" s="6"/>
+    </row>
+    <row r="12" spans="2:9" ht="15" thickBot="1"/>
+    <row r="13" spans="2:9" ht="19.8" customHeight="1" thickBot="1">
+      <c r="B13" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="40"/>
+      <c r="D13" s="41" t="s">
+        <v>108</v>
+      </c>
+      <c r="E13" s="37"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="82" t="s">
+        <v>91</v>
+      </c>
+      <c r="H13" s="41" t="s">
+        <v>103</v>
+      </c>
+      <c r="I13" s="35"/>
+    </row>
+    <row r="14" spans="2:9" ht="15" thickBot="1">
+      <c r="B14" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="35"/>
+      <c r="D14" s="42" t="s">
+        <v>102</v>
+      </c>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="44"/>
+    </row>
+    <row r="15" spans="2:9" ht="15" thickBot="1">
+      <c r="B15" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="35"/>
+      <c r="D15" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H15" s="38"/>
+      <c r="I15" s="35"/>
+    </row>
+    <row r="16" spans="2:9" ht="15" thickBot="1">
+      <c r="B16" s="47" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="48"/>
+      <c r="D16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I16" s="5"/>
+    </row>
+    <row r="17" spans="2:9" ht="15" thickBot="1">
+      <c r="B17" s="49" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="50"/>
+      <c r="D17" s="51" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" s="52"/>
+      <c r="F17" s="52"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="52"/>
+      <c r="I17" s="53"/>
+    </row>
+    <row r="18" spans="2:9" ht="28.2" thickBot="1">
+      <c r="B18" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="54" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="55"/>
+      <c r="E18" s="54" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="56"/>
+      <c r="G18" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" ht="212.4" customHeight="1" thickBot="1">
+      <c r="B19" s="13">
+        <v>1</v>
+      </c>
+      <c r="C19" s="57" t="s">
+        <v>105</v>
+      </c>
+      <c r="D19" s="58"/>
+      <c r="E19" s="57" t="s">
+        <v>106</v>
+      </c>
+      <c r="F19" s="58"/>
+      <c r="G19" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+    </row>
+    <row r="20" spans="2:9" ht="15" thickBot="1">
+      <c r="B20" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="45" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I20" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="32">
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:I17"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:I14"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:I7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:I4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="H5:I5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1805,65 +2268,65 @@
   <sheetData>
     <row r="2" spans="2:9" ht="15" thickBot="1"/>
     <row r="3" spans="2:9" ht="28.2" thickBot="1">
-      <c r="B3" s="53" t="s">
+      <c r="B3" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="54"/>
-      <c r="D3" s="56" t="s">
-        <v>45</v>
-      </c>
-      <c r="E3" s="39"/>
-      <c r="F3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="59" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" s="37"/>
+      <c r="F3" s="35"/>
       <c r="G3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="56" t="s">
-        <v>58</v>
-      </c>
-      <c r="I3" s="40"/>
+      <c r="H3" s="59" t="s">
+        <v>55</v>
+      </c>
+      <c r="I3" s="35"/>
     </row>
     <row r="4" spans="2:9" ht="15" thickBot="1">
-      <c r="B4" s="57" t="s">
+      <c r="B4" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="D4" s="58" t="s">
-        <v>57</v>
-      </c>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="37"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="44"/>
     </row>
     <row r="5" spans="2:9" ht="15" thickBot="1">
-      <c r="B5" s="57" t="s">
+      <c r="B5" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="40"/>
-      <c r="D5" s="64" t="s">
+      <c r="C5" s="35"/>
+      <c r="D5" s="62" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
       <c r="G5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="59">
+      <c r="H5" s="38">
         <v>45734</v>
       </c>
-      <c r="I5" s="40"/>
+      <c r="I5" s="35"/>
     </row>
     <row r="6" spans="2:9" ht="42" thickBot="1">
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="52"/>
+      <c r="C6" s="48"/>
       <c r="D6" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>8</v>
@@ -1875,31 +2338,31 @@
       <c r="I6" s="5"/>
     </row>
     <row r="7" spans="2:9" ht="33" customHeight="1" thickBot="1">
-      <c r="B7" s="41" t="s">
+      <c r="B7" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="42"/>
-      <c r="D7" s="43" t="s">
-        <v>59</v>
-      </c>
-      <c r="E7" s="44"/>
-      <c r="F7" s="44"/>
-      <c r="G7" s="44"/>
-      <c r="H7" s="44"/>
-      <c r="I7" s="45"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="60" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7" s="52"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="52"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="53"/>
     </row>
     <row r="8" spans="2:9" ht="28.2" thickBot="1">
       <c r="B8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="46" t="s">
+      <c r="C8" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="47"/>
-      <c r="E8" s="46" t="s">
+      <c r="D8" s="55"/>
+      <c r="E8" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="48"/>
+      <c r="F8" s="56"/>
       <c r="G8" s="10" t="s">
         <v>14</v>
       </c>
@@ -1914,14 +2377,14 @@
       <c r="B9" s="13">
         <v>1</v>
       </c>
-      <c r="C9" s="49" t="s">
-        <v>60</v>
-      </c>
-      <c r="D9" s="50"/>
-      <c r="E9" s="49" t="s">
-        <v>61</v>
-      </c>
-      <c r="F9" s="50"/>
+      <c r="C9" s="61" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="58"/>
+      <c r="E9" s="61" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" s="58"/>
       <c r="G9" s="14" t="s">
         <v>27</v>
       </c>
@@ -1932,40 +2395,32 @@
       <c r="B10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="34" t="s">
+      <c r="C10" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
       <c r="H10" s="7" t="s">
         <v>19</v>
       </c>
       <c r="I10" s="6"/>
     </row>
     <row r="11" spans="2:9" ht="15" thickBot="1">
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="37"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="40"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:I4"/>
     <mergeCell ref="C10:G10"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="D11:I11"/>
@@ -1976,6 +2431,14 @@
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="E9:F9"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1993,60 +2456,60 @@
   <sheetData>
     <row r="3" spans="2:9" ht="15" thickBot="1"/>
     <row r="4" spans="2:9" ht="28.2" thickBot="1">
-      <c r="B4" s="53" t="s">
+      <c r="B4" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="54"/>
-      <c r="D4" s="56" t="s">
-        <v>55</v>
-      </c>
-      <c r="E4" s="39"/>
-      <c r="F4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="59" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="37"/>
+      <c r="F4" s="35"/>
       <c r="G4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="56" t="s">
-        <v>49</v>
-      </c>
-      <c r="I4" s="40"/>
+      <c r="H4" s="59" t="s">
+        <v>46</v>
+      </c>
+      <c r="I4" s="35"/>
     </row>
     <row r="5" spans="2:9" ht="15" thickBot="1">
-      <c r="B5" s="57" t="s">
+      <c r="B5" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="40"/>
-      <c r="D5" s="58" t="s">
-        <v>50</v>
-      </c>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="37"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="44"/>
     </row>
     <row r="6" spans="2:9" ht="15" thickBot="1">
-      <c r="B6" s="57" t="s">
+      <c r="B6" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="40"/>
-      <c r="D6" s="38" t="s">
+      <c r="C6" s="35"/>
+      <c r="D6" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
       <c r="G6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="59">
+      <c r="H6" s="38">
         <v>45734</v>
       </c>
-      <c r="I6" s="40"/>
+      <c r="I6" s="35"/>
     </row>
     <row r="7" spans="2:9" ht="24.6" thickBot="1">
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="52"/>
+      <c r="C7" s="48"/>
       <c r="D7" s="3" t="s">
         <v>7</v>
       </c>
@@ -2056,36 +2519,36 @@
       </c>
       <c r="G7" s="19"/>
       <c r="H7" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I7" s="5"/>
     </row>
     <row r="8" spans="2:9" ht="28.95" customHeight="1" thickBot="1">
-      <c r="B8" s="41" t="s">
+      <c r="B8" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="42"/>
-      <c r="D8" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="E8" s="44"/>
-      <c r="F8" s="44"/>
-      <c r="G8" s="44"/>
-      <c r="H8" s="44"/>
-      <c r="I8" s="45"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="60" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="52"/>
+      <c r="F8" s="52"/>
+      <c r="G8" s="52"/>
+      <c r="H8" s="52"/>
+      <c r="I8" s="53"/>
     </row>
     <row r="9" spans="2:9" ht="28.2" thickBot="1">
       <c r="B9" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="46" t="s">
+      <c r="C9" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="47"/>
-      <c r="E9" s="46" t="s">
+      <c r="D9" s="55"/>
+      <c r="E9" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="48"/>
+      <c r="F9" s="56"/>
       <c r="G9" s="10" t="s">
         <v>14</v>
       </c>
@@ -2100,16 +2563,16 @@
       <c r="B10" s="13">
         <v>1</v>
       </c>
-      <c r="C10" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="D10" s="50"/>
-      <c r="E10" s="49" t="s">
-        <v>53</v>
-      </c>
-      <c r="F10" s="50"/>
+      <c r="C10" s="61" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="58"/>
+      <c r="E10" s="61" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="58"/>
       <c r="G10" s="17" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
@@ -2118,40 +2581,32 @@
       <c r="B11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="34" t="s">
+      <c r="C11" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
       <c r="H11" s="7" t="s">
         <v>19</v>
       </c>
       <c r="I11" s="6"/>
     </row>
     <row r="12" spans="2:9" ht="15" thickBot="1">
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="37"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="40"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:I5"/>
     <mergeCell ref="C11:G11"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="D12:I12"/>
@@ -2162,6 +2617,14 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="E10:F10"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:I5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2179,60 +2642,60 @@
   <sheetData>
     <row r="1" spans="2:9" ht="15" thickBot="1"/>
     <row r="2" spans="2:9" ht="28.2" thickBot="1">
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="56" t="s">
-        <v>56</v>
-      </c>
-      <c r="E2" s="39"/>
-      <c r="F2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="59" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" s="37"/>
+      <c r="F2" s="35"/>
       <c r="G2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="56" t="s">
-        <v>62</v>
-      </c>
-      <c r="I2" s="40"/>
+      <c r="H2" s="59" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2" s="35"/>
     </row>
     <row r="3" spans="2:9" ht="15" customHeight="1" thickBot="1">
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="40"/>
-      <c r="D3" s="58" t="s">
-        <v>63</v>
-      </c>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="37"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="44"/>
     </row>
     <row r="4" spans="2:9" ht="15" thickBot="1">
-      <c r="B4" s="57" t="s">
+      <c r="B4" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="D4" s="38" t="s">
+      <c r="C4" s="35"/>
+      <c r="D4" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
       <c r="G4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="59">
+      <c r="H4" s="38">
         <v>45734</v>
       </c>
-      <c r="I4" s="40"/>
+      <c r="I4" s="35"/>
     </row>
     <row r="5" spans="2:9" ht="24.6" thickBot="1">
-      <c r="B5" s="51" t="s">
+      <c r="B5" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="52"/>
+      <c r="C5" s="48"/>
       <c r="D5" s="3" t="s">
         <v>7</v>
       </c>
@@ -2241,39 +2704,39 @@
         <v>8</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I5" s="5"/>
     </row>
     <row r="6" spans="2:9" ht="15" thickBot="1">
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="42"/>
-      <c r="D6" s="43" t="s">
-        <v>65</v>
-      </c>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="45"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="60" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" s="52"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="52"/>
+      <c r="I6" s="53"/>
     </row>
     <row r="7" spans="2:9" ht="28.2" thickBot="1">
       <c r="B7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="46" t="s">
+      <c r="C7" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="47"/>
-      <c r="E7" s="46" t="s">
+      <c r="D7" s="55"/>
+      <c r="E7" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="48"/>
+      <c r="F7" s="56"/>
       <c r="G7" s="10" t="s">
         <v>14</v>
       </c>
@@ -2288,16 +2751,16 @@
       <c r="B8" s="13">
         <v>1</v>
       </c>
-      <c r="C8" s="49" t="s">
-        <v>66</v>
-      </c>
-      <c r="D8" s="50"/>
-      <c r="E8" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="F8" s="50"/>
+      <c r="C8" s="61" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="58"/>
+      <c r="E8" s="61" t="s">
+        <v>64</v>
+      </c>
+      <c r="F8" s="58"/>
       <c r="G8" s="17" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
@@ -2306,16 +2769,16 @@
       <c r="B9" s="13">
         <v>2</v>
       </c>
-      <c r="C9" s="62" t="s">
-        <v>69</v>
-      </c>
-      <c r="D9" s="63"/>
-      <c r="E9" s="62" t="s">
-        <v>70</v>
-      </c>
-      <c r="F9" s="63"/>
+      <c r="C9" s="63" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" s="64"/>
+      <c r="E9" s="63" t="s">
+        <v>67</v>
+      </c>
+      <c r="F9" s="64"/>
       <c r="G9" s="17" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
@@ -2324,32 +2787,37 @@
       <c r="B10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="34" t="s">
+      <c r="C10" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
       <c r="H10" s="7" t="s">
         <v>19</v>
       </c>
       <c r="I10" s="6"/>
     </row>
     <row r="11" spans="2:9" ht="15" thickBot="1">
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="37"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="40"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:I11"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="D2:F2"/>
@@ -2365,11 +2833,6 @@
     <mergeCell ref="D6:I6"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:I11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2377,10 +2840,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD219FCF-77B2-490B-816E-2F75E9617605}">
-  <dimension ref="B1:H18"/>
+  <dimension ref="B1:H37"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -2393,232 +2856,377 @@
   <sheetData>
     <row r="1" spans="2:6" ht="15" thickBot="1"/>
     <row r="2" spans="2:6" ht="55.2" customHeight="1" thickBot="1">
-      <c r="B2" s="74" t="s">
-        <v>93</v>
-      </c>
-      <c r="C2" s="75"/>
+      <c r="B2" s="69" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="70"/>
       <c r="D2" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" s="23" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="15" thickBot="1">
+      <c r="B3" s="71" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="66"/>
+      <c r="D3" s="67" t="s">
+        <v>98</v>
+      </c>
+      <c r="E3" s="68"/>
+      <c r="F3" s="66"/>
+    </row>
+    <row r="4" spans="2:6" ht="15" thickBot="1">
+      <c r="B4" s="72" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="73"/>
+      <c r="D4" s="74" t="s">
+        <v>89</v>
+      </c>
+      <c r="E4" s="75"/>
+      <c r="F4" s="73"/>
+    </row>
+    <row r="5" spans="2:6" ht="15" thickBot="1">
+      <c r="B5" s="65" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="66"/>
+      <c r="D5" s="67" t="s">
+        <v>85</v>
+      </c>
+      <c r="E5" s="68"/>
+      <c r="F5" s="66"/>
+    </row>
+    <row r="6" spans="2:6" ht="42" thickBot="1">
+      <c r="B6" s="77" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="78"/>
+      <c r="D6" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="E2" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="F2" s="23" t="s">
+      <c r="E6" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="F6" s="25" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="15" thickBot="1">
-      <c r="B3" s="76" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="67"/>
-      <c r="D3" s="72" t="s">
-        <v>88</v>
-      </c>
-      <c r="E3" s="66"/>
-      <c r="F3" s="67"/>
-    </row>
-    <row r="4" spans="2:6" ht="15" thickBot="1">
-      <c r="B4" s="77" t="s">
-        <v>73</v>
-      </c>
-      <c r="C4" s="78"/>
-      <c r="D4" s="79" t="s">
-        <v>94</v>
-      </c>
-      <c r="E4" s="80"/>
-      <c r="F4" s="78"/>
-    </row>
-    <row r="5" spans="2:6" ht="15" thickBot="1">
-      <c r="B5" s="73" t="s">
+    <row r="7" spans="2:6" ht="15" thickBot="1">
+      <c r="B7" s="79" t="s">
         <v>74</v>
       </c>
-      <c r="C5" s="67"/>
-      <c r="D5" s="72" t="s">
-        <v>89</v>
-      </c>
-      <c r="E5" s="66"/>
-      <c r="F5" s="67"/>
-    </row>
-    <row r="6" spans="2:6" ht="42" thickBot="1">
-      <c r="B6" s="68" t="s">
+      <c r="C7" s="80"/>
+      <c r="D7" s="80"/>
+      <c r="E7" s="80"/>
+      <c r="F7" s="78"/>
+    </row>
+    <row r="8" spans="2:6" ht="18" customHeight="1" thickBot="1">
+      <c r="B8" s="76" t="s">
         <v>75</v>
       </c>
-      <c r="C6" s="69"/>
-      <c r="D6" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="E6" s="24" t="s">
+      <c r="C8" s="68"/>
+      <c r="D8" s="66"/>
+      <c r="E8" s="76" t="s">
         <v>76</v>
       </c>
-      <c r="F6" s="25" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="15" thickBot="1">
-      <c r="B7" s="70" t="s">
+      <c r="F8" s="66"/>
+    </row>
+    <row r="9" spans="2:6" ht="36.6" customHeight="1" thickBot="1">
+      <c r="B9" s="67" t="s">
+        <v>99</v>
+      </c>
+      <c r="C9" s="68"/>
+      <c r="D9" s="68"/>
+      <c r="E9" s="67"/>
+      <c r="F9" s="66"/>
+    </row>
+    <row r="10" spans="2:6" ht="15" thickBot="1">
+      <c r="B10" s="76" t="s">
         <v>77</v>
       </c>
-      <c r="C7" s="71"/>
-      <c r="D7" s="71"/>
-      <c r="E7" s="71"/>
-      <c r="F7" s="69"/>
-    </row>
-    <row r="8" spans="2:6" ht="18" customHeight="1" thickBot="1">
-      <c r="B8" s="65" t="s">
-        <v>78</v>
-      </c>
-      <c r="C8" s="66"/>
-      <c r="D8" s="67"/>
-      <c r="E8" s="65" t="s">
-        <v>79</v>
-      </c>
-      <c r="F8" s="67"/>
-    </row>
-    <row r="9" spans="2:6" ht="36.6" customHeight="1" thickBot="1">
-      <c r="B9" s="72" t="s">
-        <v>91</v>
-      </c>
-      <c r="C9" s="66"/>
-      <c r="D9" s="66"/>
-      <c r="E9" s="72"/>
-      <c r="F9" s="67"/>
-    </row>
-    <row r="10" spans="2:6" ht="15" thickBot="1">
-      <c r="B10" s="65" t="s">
-        <v>80</v>
-      </c>
-      <c r="C10" s="66"/>
-      <c r="D10" s="66"/>
-      <c r="E10" s="66"/>
-      <c r="F10" s="67"/>
+      <c r="C10" s="68"/>
+      <c r="D10" s="68"/>
+      <c r="E10" s="68"/>
+      <c r="F10" s="66"/>
     </row>
     <row r="11" spans="2:6" ht="20.399999999999999" customHeight="1" thickBot="1">
       <c r="B11" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="D11" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="C11" s="27" t="s">
+      <c r="F11" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="D11" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="E11" s="27" t="s">
-        <v>84</v>
-      </c>
-      <c r="F11" s="27" t="s">
-        <v>85</v>
-      </c>
     </row>
     <row r="12" spans="2:6" ht="27" thickBot="1">
-      <c r="B12" s="28" t="s">
-        <v>21</v>
+      <c r="B12" s="81" t="s">
+        <v>90</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>39</v>
+        <v>97</v>
       </c>
       <c r="D12" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="29" t="s">
-        <v>23</v>
-      </c>
+      <c r="E12" s="29"/>
       <c r="F12" s="29"/>
     </row>
-    <row r="13" spans="2:6" ht="27" thickBot="1">
-      <c r="B13" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" s="30" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" s="29" t="s">
-        <v>23</v>
-      </c>
+    <row r="13" spans="2:6" ht="15" thickBot="1">
+      <c r="B13" s="28"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="29"/>
       <c r="F13" s="29"/>
     </row>
-    <row r="14" spans="2:6" ht="40.200000000000003" thickBot="1">
-      <c r="B14" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" s="30" t="s">
-        <v>5</v>
-      </c>
-      <c r="E14" s="29" t="s">
-        <v>23</v>
-      </c>
+    <row r="14" spans="2:6" ht="15" thickBot="1">
+      <c r="B14" s="28"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="29"/>
       <c r="F14" s="29"/>
     </row>
     <row r="15" spans="2:6" ht="30" customHeight="1" thickBot="1">
-      <c r="B15" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" s="32" t="s">
-        <v>57</v>
-      </c>
-      <c r="D15" s="30" t="s">
-        <v>5</v>
-      </c>
-      <c r="E15" s="29" t="s">
-        <v>23</v>
-      </c>
+      <c r="B15" s="28"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="29"/>
       <c r="F15" s="31"/>
     </row>
-    <row r="16" spans="2:6" ht="29.4" thickBot="1">
-      <c r="B16" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="C16" s="32" t="s">
-        <v>46</v>
-      </c>
-      <c r="D16" s="30" t="s">
-        <v>5</v>
-      </c>
-      <c r="E16" s="29" t="s">
-        <v>23</v>
-      </c>
+    <row r="16" spans="2:6" ht="15" thickBot="1">
+      <c r="B16" s="28"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="29"/>
       <c r="F16" s="31"/>
     </row>
-    <row r="17" spans="2:8" ht="28.2" thickBot="1">
-      <c r="B17" s="28" t="s">
-        <v>55</v>
-      </c>
-      <c r="C17" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="D17" s="30" t="s">
-        <v>5</v>
-      </c>
-      <c r="E17" s="29" t="s">
-        <v>23</v>
-      </c>
+    <row r="17" spans="2:8" ht="15" thickBot="1">
+      <c r="B17" s="28"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="29"/>
       <c r="F17" s="33"/>
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
     </row>
-    <row r="18" spans="2:8" ht="29.4" thickBot="1">
-      <c r="B18" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="C18" s="32" t="s">
-        <v>63</v>
-      </c>
-      <c r="D18" s="30" t="s">
+    <row r="18" spans="2:8" ht="15" thickBot="1">
+      <c r="B18" s="28"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="31"/>
+    </row>
+    <row r="20" spans="2:8" ht="15" thickBot="1"/>
+    <row r="21" spans="2:8" ht="27" thickBot="1">
+      <c r="B21" s="69" t="s">
+        <v>88</v>
+      </c>
+      <c r="C21" s="70"/>
+      <c r="D21" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="E21" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="F21" s="23" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="15" thickBot="1">
+      <c r="B22" s="71" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="66"/>
+      <c r="D22" s="67" t="s">
+        <v>100</v>
+      </c>
+      <c r="E22" s="68"/>
+      <c r="F22" s="66"/>
+    </row>
+    <row r="23" spans="2:8" ht="15" thickBot="1">
+      <c r="B23" s="72" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="73"/>
+      <c r="D23" s="74" t="s">
+        <v>89</v>
+      </c>
+      <c r="E23" s="75"/>
+      <c r="F23" s="73"/>
+    </row>
+    <row r="24" spans="2:8" ht="15" thickBot="1">
+      <c r="B24" s="65" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" s="66"/>
+      <c r="D24" s="67" t="s">
+        <v>85</v>
+      </c>
+      <c r="E24" s="68"/>
+      <c r="F24" s="66"/>
+    </row>
+    <row r="25" spans="2:8" ht="42" thickBot="1">
+      <c r="B25" s="77" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" s="78"/>
+      <c r="D25" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="E25" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="F25" s="25" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" ht="15" thickBot="1">
+      <c r="B26" s="79" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" s="80"/>
+      <c r="D26" s="80"/>
+      <c r="E26" s="80"/>
+      <c r="F26" s="78"/>
+    </row>
+    <row r="27" spans="2:8" ht="15" thickBot="1">
+      <c r="B27" s="76" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27" s="68"/>
+      <c r="D27" s="66"/>
+      <c r="E27" s="76" t="s">
+        <v>76</v>
+      </c>
+      <c r="F27" s="66"/>
+    </row>
+    <row r="28" spans="2:8" ht="32.4" customHeight="1" thickBot="1">
+      <c r="B28" s="67" t="s">
+        <v>99</v>
+      </c>
+      <c r="C28" s="68"/>
+      <c r="D28" s="68"/>
+      <c r="E28" s="67"/>
+      <c r="F28" s="66"/>
+    </row>
+    <row r="29" spans="2:8" ht="15" thickBot="1">
+      <c r="B29" s="76" t="s">
+        <v>77</v>
+      </c>
+      <c r="C29" s="68"/>
+      <c r="D29" s="68"/>
+      <c r="E29" s="68"/>
+      <c r="F29" s="66"/>
+    </row>
+    <row r="30" spans="2:8" ht="15" thickBot="1">
+      <c r="B30" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="C30" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="D30" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="E30" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="F30" s="27" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" ht="27" thickBot="1">
+      <c r="B31" s="81" t="s">
+        <v>90</v>
+      </c>
+      <c r="C31" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="D31" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="E18" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="F18" s="31"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="29"/>
+    </row>
+    <row r="32" spans="2:8" ht="15" thickBot="1">
+      <c r="B32" s="28"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="30"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="29"/>
+    </row>
+    <row r="33" spans="2:6" ht="15" thickBot="1">
+      <c r="B33" s="28"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="29"/>
+    </row>
+    <row r="34" spans="2:6" ht="15" thickBot="1">
+      <c r="B34" s="28"/>
+      <c r="C34" s="32"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="31"/>
+    </row>
+    <row r="35" spans="2:6" ht="15" thickBot="1">
+      <c r="B35" s="28"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="30"/>
+      <c r="E35" s="29"/>
+      <c r="F35" s="31"/>
+    </row>
+    <row r="36" spans="2:6" ht="15" thickBot="1">
+      <c r="B36" s="28"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="30"/>
+      <c r="E36" s="29"/>
+      <c r="F36" s="33"/>
+    </row>
+    <row r="37" spans="2:6" ht="15" thickBot="1">
+      <c r="B37" s="28"/>
+      <c r="C37" s="32"/>
+      <c r="D37" s="30"/>
+      <c r="E37" s="29"/>
+      <c r="F37" s="31"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="28">
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="E9:F9"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="D5:F5"/>
     <mergeCell ref="B2:C2"/>
@@ -2626,14 +3234,11 @@
     <mergeCell ref="D3:F3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="D4:F4"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="E9:F9"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B12" location="Ethernet!B13" display="T1" xr:uid="{121703C7-11C5-4D45-9096-442FD6A967FB}"/>
+    <hyperlink ref="B31" location="Ethernet!B3" display="T1" xr:uid="{B0CD6564-2A0A-4D2C-93D8-B46585536579}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modification de la planification
</commit_message>
<xml_diff>
--- a/PEA/Plan de test/Plan de tests - PEA.xlsx
+++ b/PEA/Plan de test/Plan de tests - PEA.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robin\Documents\GITHUB\ACCES_CAMPUS\Acc-s-campus-\PEA\Plan de test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B34F41E2-5089-41BE-BDF6-49C875B9328C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1E6EA26-2472-48CD-BBF8-91EBD8C85E3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{21D66C90-57CB-4BB7-B44F-BA6973DF79EF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{21D66C90-57CB-4BB7-B44F-BA6973DF79EF}"/>
   </bookViews>
   <sheets>
-    <sheet name="Microcontrôleur" sheetId="1" r:id="rId1"/>
-    <sheet name="Ethernet" sheetId="2" r:id="rId2"/>
-    <sheet name="RFID" sheetId="4" r:id="rId3"/>
-    <sheet name="Gâche" sheetId="3" r:id="rId4"/>
-    <sheet name="Alimentation PoE" sheetId="5" r:id="rId5"/>
-    <sheet name="Plan de tests" sheetId="6" r:id="rId6"/>
+    <sheet name="Plan de tests" sheetId="6" r:id="rId1"/>
+    <sheet name="Microcontrôleur" sheetId="1" r:id="rId2"/>
+    <sheet name="Intégration PEA &lt;-&gt; BDD" sheetId="7" r:id="rId3"/>
+    <sheet name="Ethernet" sheetId="2" r:id="rId4"/>
+    <sheet name="RFID" sheetId="4" r:id="rId5"/>
+    <sheet name="Gâche" sheetId="3" r:id="rId6"/>
+    <sheet name="Alimentation PoE" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="123">
   <si>
     <t>Identification du Test</t>
   </si>
@@ -106,9 +107,6 @@
     <t>Conclusion du test :</t>
   </si>
   <si>
-    <t>T1.1</t>
-  </si>
-  <si>
     <t>Robin MARTINEAU</t>
   </si>
   <si>
@@ -116,24 +114,6 @@
   </si>
   <si>
     <t>La PEA doit avoir le code de téléverser dans son microcontrôleur. L'utilisateur doit disposer d'un badge RFID adapté.</t>
-  </si>
-  <si>
-    <t>T1.2</t>
-  </si>
-  <si>
-    <t>Communication Wiegand - PEA</t>
-  </si>
-  <si>
-    <t>Le test consiste à vérifier que la bon fonctionnement du Wiegand (lecture)</t>
-  </si>
-  <si>
-    <t>Nous devons visualiser la clock et les informations du Badge RFID.</t>
-  </si>
-  <si>
-    <t>Placer les sondes de l'oscilloscope actif sur le PA11 et le PA10</t>
-  </si>
-  <si>
-    <t>Si l'UID reçue est le même que celui envoyé.</t>
   </si>
   <si>
     <t>La PEA doit avoir le code de téléverser dans son microcontrôleur. L'utilisateur doit disposer d'un badge RFID adapté, dont il connait l'UID.</t>
@@ -347,12 +327,6 @@
     <t>Le test consisiste à tester la bonne communication entre le microcontrolleur.</t>
   </si>
   <si>
-    <t>Placer les sondes de l'oscilloscope actif sur le PA11 et le PA10. Puis lancer la séquence de vérification en scannant un badge RFID. Une fois cela fait comparer la trame obtenu avec la trame attendue ou alors décoder la trame et avoir le même UID que la carte utilisé.</t>
-  </si>
-  <si>
-    <t>Nous devons visualiser le signal suivant ou ressemblant :</t>
-  </si>
-  <si>
     <t>Si l'UID décodé sur l'oscilloscope est le même que celui envoyé.</t>
   </si>
   <si>
@@ -375,6 +349,332 @@
   </si>
   <si>
     <t>Le test consisiste à tester la bonne communication entre le microcontrolleur via le protocole Wiegand 26b</t>
+  </si>
+  <si>
+    <t>Placer les sondes de l'oscilloscope actif sur le PC13 et le PA14. Rélgler la base de temps de l'oscilloscope à 5ms, et le delay à 24.5ms. Regler un Trigger sur CH2 reglé à 4,12V.Réglez la base de tension des 2 canaux à 1V et réglez les offsets sur -2.5V. Appuyez ensuite sur le bouton "Single". Puis lancer la séquence de vérification en scannant un badge RFID. Une fois cela fait comparer la trame obtenu avec la trame attendue ou alors décoder la trame et avoir le même UID que la carte utilisé.</t>
+  </si>
+  <si>
+    <t>DQ</t>
+  </si>
+  <si>
+    <t>Tester le bon fonctionnement de l'incrément 1.</t>
+  </si>
+  <si>
+    <t>Tests d'intégrations</t>
+  </si>
+  <si>
+    <t>Salle de cours</t>
+  </si>
+  <si>
+    <t>La base de données et les différents systèmes qui compose le projet "Accès campus", doivent être alimenter et fonctionnel.  Tout les systèmes doivent être minimum à l'incrément 1.</t>
+  </si>
+  <si>
+    <t>Le test permet de vérifier que la communication Ethernet est valide.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Robin MARTINEAU - Lorick FOUQUET </t>
+  </si>
+  <si>
+    <t>La connexion Ethernet fonctionne correctement.</t>
+  </si>
+  <si>
+    <t>Bloc testé.</t>
+  </si>
+  <si>
+    <t>Communication Ethernet</t>
+  </si>
+  <si>
+    <t>un Serial monitor</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>Outils de développement</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t> :</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">La PEA doit avoir le code de téléverser dans son microcontrôleur. Le système doit être alimenter et connecté au réseaux L'utilisateur doit disposer de 2 badges RFID adapté, dont il connait l'UID. L'UID de l'un des 2 badges doit être validé par la base de données. </t>
+  </si>
+  <si>
+    <t>Poser le badge RFID valide sur le capteur RFID.</t>
+  </si>
+  <si>
+    <r>
+      <t>La réponse du serveur, lu dans le serial monitor doit être la suivante :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="3" tint="0.249977111117893"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> HTTP/1.1 200 OK
+date: Tue, 04 Apr 2025 08:15:32 GMT
+server: uvicorn
+content-length: 67
+content-type: application/json
+{"nom":</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="6" tint="0.59999389629810485"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>"nom lier au badge"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="3" tint="0.249977111117893"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>,"prenom":</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="6" tint="0.59999389629810485"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>"prénom lier au badge"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="3" tint="0.249977111117893"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>,"role":</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="6" tint="0.59999389629810485"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>"rôle lié au badge"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="3" tint="0.249977111117893"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>,"autorise":</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="6" tint="0.59999389629810485"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>true</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="3" tint="0.249977111117893"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Le test est réussi si le message contient le code: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>HTTP/1.1 200 OK ,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">et le mesage : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>{"nom":"nom lier au badge","prenom":"prénom lier au badge","role":"rôle lié au badge","autorise":true}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Le code "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>HTTP/1.1 200</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>OK</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>" as bien été obtenue avec les informations de l'utilisateur.</t>
+    </r>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>Poser le badge RFID invalide sur le capteur RFID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La réponse du serveur, lu dans le serial monitor doit être la suivante : HTTP/1.1 403 Forbidden
+date: Wed, 02 Apr 2025 08:13:46 GMT
+server: uvicorn
+content-length: 27
+content-type: application/json
+Connection: close
+{"detail":"Accès refusé"}
+</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Le test est réussi si le message contient le code : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>HTTP/1.1 403</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>, et le message : {</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>"detail":"Accès refusé"}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Le code "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>HTTP/1.1 403 Forbidden</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>" as bien été obtenue avec le message de refus.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  [ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>X</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>] OK           Anomalie   [ ] mineure   [ ] majeure   [ ] bloquante           [ ] NOK</t>
+    </r>
+  </si>
+  <si>
+    <t>La connexion entre la PEA et la BDD est valide et fonctionne correctement.</t>
+  </si>
+  <si>
+    <t>T6</t>
   </si>
 </sst>
 </file>
@@ -384,7 +684,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -445,8 +745,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="3" tint="0.249977111117893"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="6" tint="0.59999389629810485"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -489,8 +807,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFCCCCCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="22">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -745,12 +1069,47 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -962,6 +1321,114 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -1433,11 +1900,441 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD219FCF-77B2-490B-816E-2F75E9617605}">
+  <dimension ref="B1:H37"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="3" max="3" width="35.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" customWidth="1"/>
+    <col min="5" max="5" width="17.5546875" customWidth="1"/>
+    <col min="6" max="6" width="19.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" ht="15" thickBot="1"/>
+    <row r="2" spans="2:6" ht="55.2" customHeight="1" thickBot="1">
+      <c r="B2" s="76" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="77"/>
+      <c r="D2" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="15" thickBot="1">
+      <c r="B3" s="78" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="69"/>
+      <c r="D3" s="67" t="s">
+        <v>76</v>
+      </c>
+      <c r="E3" s="68"/>
+      <c r="F3" s="69"/>
+    </row>
+    <row r="4" spans="2:6" ht="15" thickBot="1">
+      <c r="B4" s="79" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="80"/>
+      <c r="D4" s="81" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="82"/>
+      <c r="F4" s="80"/>
+    </row>
+    <row r="5" spans="2:6" ht="15" thickBot="1">
+      <c r="B5" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="69"/>
+      <c r="D5" s="67" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" s="68"/>
+      <c r="F5" s="69"/>
+    </row>
+    <row r="6" spans="2:6" ht="42" thickBot="1">
+      <c r="B6" s="72" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="73"/>
+      <c r="D6" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" s="25" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="15" thickBot="1">
+      <c r="B7" s="74" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="75"/>
+      <c r="D7" s="75"/>
+      <c r="E7" s="75"/>
+      <c r="F7" s="73"/>
+    </row>
+    <row r="8" spans="2:6" ht="18" customHeight="1" thickBot="1">
+      <c r="B8" s="70" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="68"/>
+      <c r="D8" s="69"/>
+      <c r="E8" s="70" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" s="69"/>
+    </row>
+    <row r="9" spans="2:6" ht="36.6" customHeight="1" thickBot="1">
+      <c r="B9" s="67" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="68"/>
+      <c r="D9" s="68"/>
+      <c r="E9" s="67"/>
+      <c r="F9" s="69"/>
+    </row>
+    <row r="10" spans="2:6" ht="15" thickBot="1">
+      <c r="B10" s="70" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="68"/>
+      <c r="D10" s="68"/>
+      <c r="E10" s="68"/>
+      <c r="F10" s="69"/>
+    </row>
+    <row r="11" spans="2:6" ht="20.399999999999999" customHeight="1" thickBot="1">
+      <c r="B11" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="F11" s="27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="27" thickBot="1">
+      <c r="B12" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+    </row>
+    <row r="13" spans="2:6" ht="27" thickBot="1">
+      <c r="B13" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="D13" s="30"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+    </row>
+    <row r="14" spans="2:6" ht="43.8" customHeight="1" thickBot="1">
+      <c r="B14" s="34" t="s">
+        <v>90</v>
+      </c>
+      <c r="C14" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="30"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+    </row>
+    <row r="15" spans="2:6" ht="30" customHeight="1" thickBot="1">
+      <c r="B15" s="117" t="s">
+        <v>122</v>
+      </c>
+      <c r="C15" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="30"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="31"/>
+    </row>
+    <row r="16" spans="2:6" ht="43.8" thickBot="1">
+      <c r="B16" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="C16" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="D16" s="30"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="31"/>
+    </row>
+    <row r="17" spans="2:8" ht="15" thickBot="1">
+      <c r="B17" s="28"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+    </row>
+    <row r="18" spans="2:8" ht="15" thickBot="1">
+      <c r="B18" s="28"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="31"/>
+    </row>
+    <row r="20" spans="2:8" ht="15" thickBot="1"/>
+    <row r="21" spans="2:8" ht="27" thickBot="1">
+      <c r="B21" s="76" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" s="77"/>
+      <c r="D21" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="E21" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="F21" s="23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="15" thickBot="1">
+      <c r="B22" s="78" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="69"/>
+      <c r="D22" s="67" t="s">
+        <v>78</v>
+      </c>
+      <c r="E22" s="68"/>
+      <c r="F22" s="69"/>
+    </row>
+    <row r="23" spans="2:8" ht="15" thickBot="1">
+      <c r="B23" s="79" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="80"/>
+      <c r="D23" s="81" t="s">
+        <v>67</v>
+      </c>
+      <c r="E23" s="82"/>
+      <c r="F23" s="80"/>
+    </row>
+    <row r="24" spans="2:8" ht="15" thickBot="1">
+      <c r="B24" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="69"/>
+      <c r="D24" s="67" t="s">
+        <v>63</v>
+      </c>
+      <c r="E24" s="68"/>
+      <c r="F24" s="69"/>
+    </row>
+    <row r="25" spans="2:8" ht="42" thickBot="1">
+      <c r="B25" s="72" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="73"/>
+      <c r="D25" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="E25" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="F25" s="25" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" ht="15" thickBot="1">
+      <c r="B26" s="74" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="75"/>
+      <c r="D26" s="75"/>
+      <c r="E26" s="75"/>
+      <c r="F26" s="73"/>
+    </row>
+    <row r="27" spans="2:8" ht="15" thickBot="1">
+      <c r="B27" s="70" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" s="68"/>
+      <c r="D27" s="69"/>
+      <c r="E27" s="70" t="s">
+        <v>54</v>
+      </c>
+      <c r="F27" s="69"/>
+    </row>
+    <row r="28" spans="2:8" ht="32.4" customHeight="1" thickBot="1">
+      <c r="B28" s="67" t="s">
+        <v>77</v>
+      </c>
+      <c r="C28" s="68"/>
+      <c r="D28" s="68"/>
+      <c r="E28" s="67"/>
+      <c r="F28" s="69"/>
+    </row>
+    <row r="29" spans="2:8" ht="15" thickBot="1">
+      <c r="B29" s="70" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" s="68"/>
+      <c r="D29" s="68"/>
+      <c r="E29" s="68"/>
+      <c r="F29" s="69"/>
+    </row>
+    <row r="30" spans="2:8" ht="15" thickBot="1">
+      <c r="B30" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="C30" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="D30" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="E30" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="F30" s="27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" ht="27" thickBot="1">
+      <c r="B31" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="C31" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="D31" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="E31" s="29"/>
+      <c r="F31" s="29"/>
+    </row>
+    <row r="32" spans="2:8" ht="27" thickBot="1">
+      <c r="B32" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="C32" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="D32" s="30"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="29"/>
+    </row>
+    <row r="33" spans="2:6" ht="15" thickBot="1">
+      <c r="B33" s="28"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="29"/>
+    </row>
+    <row r="34" spans="2:6" ht="15" thickBot="1">
+      <c r="B34" s="28"/>
+      <c r="C34" s="32"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="31"/>
+    </row>
+    <row r="35" spans="2:6" ht="15" thickBot="1">
+      <c r="B35" s="28"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="30"/>
+      <c r="E35" s="29"/>
+      <c r="F35" s="31"/>
+    </row>
+    <row r="36" spans="2:6" ht="15" thickBot="1">
+      <c r="B36" s="28"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="30"/>
+      <c r="E36" s="29"/>
+      <c r="F36" s="33"/>
+    </row>
+    <row r="37" spans="2:6" ht="15" thickBot="1">
+      <c r="B37" s="28"/>
+      <c r="C37" s="32"/>
+      <c r="D37" s="30"/>
+      <c r="E37" s="29"/>
+      <c r="F37" s="31"/>
+    </row>
+  </sheetData>
+  <mergeCells count="28">
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="E27:F27"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B12" location="Ethernet!B13" display="T1" xr:uid="{121703C7-11C5-4D45-9096-442FD6A967FB}"/>
+    <hyperlink ref="B31" location="Ethernet!B3" display="T1" xr:uid="{B0CD6564-2A0A-4D2C-93D8-B46585536579}"/>
+    <hyperlink ref="B13" location="RFID!B3" display="T3" xr:uid="{B2AEFDF5-8F01-49D2-A3A0-C26A02A9CC4A}"/>
+    <hyperlink ref="B14" location="Gâche!B4" display="T4" xr:uid="{6AD56DDE-1C0A-4EA1-A077-C61F03A921F9}"/>
+    <hyperlink ref="B32" location="'Alimentation PoE'!B2" display="T5" xr:uid="{EBFF8E81-F438-424D-BF71-85AC823D9304}"/>
+    <hyperlink ref="B15" location="Microcontrôleur!B13" display="T6" xr:uid="{2BA100AB-7AC9-4E47-81C2-DB640C1524D4}"/>
+    <hyperlink ref="B16" location="Ethernet!D13" display="T2" xr:uid="{85D303A3-B904-4421-9916-F3B4FF834A17}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E407FD9-0AE4-4A1C-B2E0-3161C8BCECA8}">
   <dimension ref="B2:I27"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19:D19"/>
+    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14:I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -1448,156 +2345,95 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="15" thickBot="1"/>
-    <row r="3" spans="2:9" ht="19.2" customHeight="1" thickBot="1">
-      <c r="B3" s="55" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="56"/>
-      <c r="D3" s="57" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="41"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H3" s="57" t="s">
-        <v>26</v>
-      </c>
-      <c r="I3" s="42"/>
-    </row>
-    <row r="4" spans="2:9" ht="15" thickBot="1">
-      <c r="B4" s="59" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="42"/>
-      <c r="D4" s="60" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="39"/>
-    </row>
-    <row r="5" spans="2:9" ht="15" thickBot="1">
-      <c r="B5" s="59" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="42"/>
-      <c r="D5" s="40" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H5" s="61">
-        <v>45734</v>
-      </c>
-      <c r="I5" s="42"/>
-    </row>
-    <row r="6" spans="2:9" ht="18.600000000000001" customHeight="1" thickBot="1">
-      <c r="B6" s="53" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="54"/>
-      <c r="D6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I6" s="5"/>
-    </row>
-    <row r="7" spans="2:9" ht="31.8" customHeight="1" thickBot="1">
-      <c r="B7" s="43" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="44"/>
-      <c r="D7" s="63" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
-      <c r="I7" s="47"/>
-    </row>
-    <row r="8" spans="2:9" ht="28.2" thickBot="1">
-      <c r="B8" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="48" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="49"/>
-      <c r="E8" s="48" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="50"/>
-      <c r="G8" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="I8" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" ht="78" customHeight="1" thickBot="1">
-      <c r="B9" s="13">
-        <v>1</v>
-      </c>
-      <c r="C9" s="62" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="52"/>
-      <c r="E9" s="62" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" s="52"/>
-      <c r="G9" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-    </row>
-    <row r="10" spans="2:9" ht="15" thickBot="1">
-      <c r="B10" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="37"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="37"/>
-      <c r="H10" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="I10" s="6"/>
+    <row r="3" spans="2:9" ht="19.2" customHeight="1">
+      <c r="B3" s="118"/>
+      <c r="C3" s="118"/>
+      <c r="D3" s="118"/>
+      <c r="E3" s="118"/>
+      <c r="F3" s="118"/>
+      <c r="G3" s="118"/>
+      <c r="H3" s="118"/>
+      <c r="I3" s="118"/>
+    </row>
+    <row r="4" spans="2:9">
+      <c r="B4" s="119"/>
+      <c r="C4" s="119"/>
+      <c r="D4" s="119"/>
+      <c r="E4" s="119"/>
+      <c r="F4" s="119"/>
+      <c r="G4" s="119"/>
+      <c r="H4" s="119"/>
+      <c r="I4" s="119"/>
+    </row>
+    <row r="5" spans="2:9">
+      <c r="B5" s="119"/>
+      <c r="C5" s="119"/>
+      <c r="D5" s="119"/>
+      <c r="E5" s="119"/>
+      <c r="F5" s="119"/>
+      <c r="G5" s="119"/>
+      <c r="H5" s="119"/>
+      <c r="I5" s="119"/>
+    </row>
+    <row r="6" spans="2:9" ht="18.600000000000001" customHeight="1">
+      <c r="B6" s="119"/>
+      <c r="C6" s="119"/>
+      <c r="D6" s="119"/>
+      <c r="E6" s="119"/>
+      <c r="F6" s="119"/>
+      <c r="G6" s="119"/>
+      <c r="H6" s="119"/>
+      <c r="I6" s="119"/>
+    </row>
+    <row r="7" spans="2:9" ht="31.8" customHeight="1">
+      <c r="B7" s="119"/>
+      <c r="C7" s="119"/>
+      <c r="D7" s="119"/>
+      <c r="E7" s="119"/>
+      <c r="F7" s="119"/>
+      <c r="G7" s="119"/>
+      <c r="H7" s="119"/>
+      <c r="I7" s="119"/>
+    </row>
+    <row r="8" spans="2:9">
+      <c r="B8" s="119"/>
+      <c r="C8" s="119"/>
+      <c r="D8" s="119"/>
+      <c r="E8" s="119"/>
+      <c r="F8" s="119"/>
+      <c r="G8" s="119"/>
+      <c r="H8" s="119"/>
+      <c r="I8" s="119"/>
+    </row>
+    <row r="9" spans="2:9" ht="78" customHeight="1">
+      <c r="B9" s="119"/>
+      <c r="C9" s="119"/>
+      <c r="D9" s="119"/>
+      <c r="E9" s="119"/>
+      <c r="F9" s="119"/>
+      <c r="G9" s="119"/>
+      <c r="H9" s="119"/>
+      <c r="I9" s="119"/>
+    </row>
+    <row r="10" spans="2:9">
+      <c r="B10" s="119"/>
+      <c r="C10" s="119"/>
+      <c r="D10" s="119"/>
+      <c r="E10" s="119"/>
+      <c r="F10" s="119"/>
+      <c r="G10" s="119"/>
+      <c r="H10" s="119"/>
+      <c r="I10" s="119"/>
     </row>
     <row r="11" spans="2:9" ht="28.95" customHeight="1" thickBot="1">
-      <c r="B11" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="39"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="42"/>
+      <c r="B11" s="120"/>
+      <c r="C11" s="120"/>
+      <c r="D11" s="120"/>
+      <c r="E11" s="120"/>
+      <c r="F11" s="120"/>
+      <c r="G11" s="120"/>
+      <c r="H11" s="120"/>
+      <c r="I11" s="120"/>
     </row>
     <row r="12" spans="2:9" ht="15" thickBot="1"/>
     <row r="13" spans="2:9" ht="15" thickBot="1">
@@ -1605,8 +2441,8 @@
         <v>0</v>
       </c>
       <c r="C13" s="56"/>
-      <c r="D13" s="57" t="s">
-        <v>21</v>
+      <c r="D13" s="58" t="s">
+        <v>122</v>
       </c>
       <c r="E13" s="41"/>
       <c r="F13" s="42"/>
@@ -1614,7 +2450,7 @@
         <v>1</v>
       </c>
       <c r="H13" s="58" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="I13" s="42"/>
     </row>
@@ -1624,7 +2460,7 @@
       </c>
       <c r="C14" s="42"/>
       <c r="D14" s="60" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E14" s="37"/>
       <c r="F14" s="37"/>
@@ -1638,7 +2474,7 @@
       </c>
       <c r="C15" s="42"/>
       <c r="D15" s="40" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E15" s="41"/>
       <c r="F15" s="41"/>
@@ -1659,14 +2495,14 @@
         <v>7</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>8</v>
       </c>
       <c r="G16" s="6"/>
       <c r="H16" s="16" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="I16" s="5"/>
     </row>
@@ -1676,7 +2512,7 @@
       </c>
       <c r="C17" s="44"/>
       <c r="D17" s="45" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E17" s="46"/>
       <c r="F17" s="46"/>
@@ -1711,15 +2547,15 @@
         <v>1</v>
       </c>
       <c r="C19" s="51" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D19" s="52"/>
       <c r="E19" s="51" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="F19" s="52"/>
       <c r="G19" s="17" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="H19" s="14"/>
       <c r="I19" s="14"/>
@@ -1754,26 +2590,8 @@
     </row>
     <row r="27" spans="2:9" ht="32.4" customHeight="1"/>
   </sheetData>
-  <mergeCells count="36">
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:I4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:I7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E8:F8"/>
+  <mergeCells count="18">
     <mergeCell ref="B16:C16"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:I11"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="D13:F13"/>
     <mergeCell ref="H13:I13"/>
@@ -1796,12 +2614,398 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03C07995-E43A-456B-A3EF-9847E2C4A809}">
+  <dimension ref="B4:I28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="3" max="3" width="25.6640625" customWidth="1"/>
+    <col min="5" max="5" width="17.88671875" customWidth="1"/>
+    <col min="6" max="6" width="22.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:6" ht="15" thickBot="1"/>
+    <row r="5" spans="2:6" ht="40.200000000000003" thickBot="1">
+      <c r="B5" s="76" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="77"/>
+      <c r="D5" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="28.8" customHeight="1" thickBot="1">
+      <c r="B6" s="78" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="69"/>
+      <c r="D6" s="67" t="s">
+        <v>99</v>
+      </c>
+      <c r="E6" s="68"/>
+      <c r="F6" s="69"/>
+    </row>
+    <row r="7" spans="2:6" ht="15" thickBot="1">
+      <c r="B7" s="79" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="80"/>
+      <c r="D7" s="81" t="s">
+        <v>100</v>
+      </c>
+      <c r="E7" s="82"/>
+      <c r="F7" s="80"/>
+    </row>
+    <row r="8" spans="2:6" ht="15" thickBot="1">
+      <c r="B8" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="69"/>
+      <c r="D8" s="67" t="s">
+        <v>101</v>
+      </c>
+      <c r="E8" s="68"/>
+      <c r="F8" s="69"/>
+    </row>
+    <row r="9" spans="2:6" ht="28.2" thickBot="1">
+      <c r="B9" s="72" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="73"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" s="25"/>
+    </row>
+    <row r="10" spans="2:6" ht="15" thickBot="1">
+      <c r="B10" s="74" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="75"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="75"/>
+      <c r="F10" s="73"/>
+    </row>
+    <row r="11" spans="2:6" ht="15" thickBot="1">
+      <c r="B11" s="70" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="68"/>
+      <c r="D11" s="69"/>
+      <c r="E11" s="70" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" s="69"/>
+    </row>
+    <row r="12" spans="2:6" ht="82.8" customHeight="1" thickBot="1">
+      <c r="B12" s="67" t="s">
+        <v>102</v>
+      </c>
+      <c r="C12" s="68"/>
+      <c r="D12" s="68"/>
+      <c r="E12" s="67"/>
+      <c r="F12" s="69"/>
+    </row>
+    <row r="13" spans="2:6" ht="15" thickBot="1">
+      <c r="B13" s="70" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="68"/>
+      <c r="D13" s="68"/>
+      <c r="E13" s="68"/>
+      <c r="F13" s="69"/>
+    </row>
+    <row r="14" spans="2:6" ht="15" thickBot="1">
+      <c r="B14" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="F14" s="27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" ht="65.400000000000006" customHeight="1" thickBot="1">
+      <c r="B15" s="117" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" s="116" t="s">
+        <v>103</v>
+      </c>
+      <c r="D15" s="30">
+        <v>45747</v>
+      </c>
+      <c r="E15" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="F15" s="29" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" ht="15" thickBot="1"/>
+    <row r="18" spans="2:9" ht="15" thickBot="1">
+      <c r="B18" s="83" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="84"/>
+      <c r="D18" s="58" t="s">
+        <v>68</v>
+      </c>
+      <c r="E18" s="68"/>
+      <c r="F18" s="69"/>
+      <c r="G18" s="85" t="s">
+        <v>106</v>
+      </c>
+      <c r="H18" s="58" t="s">
+        <v>107</v>
+      </c>
+      <c r="I18" s="69"/>
+    </row>
+    <row r="19" spans="2:9" ht="15" thickBot="1">
+      <c r="B19" s="86" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="69"/>
+      <c r="D19" s="60" t="s">
+        <v>103</v>
+      </c>
+      <c r="E19" s="75"/>
+      <c r="F19" s="75"/>
+      <c r="G19" s="75"/>
+      <c r="H19" s="75"/>
+      <c r="I19" s="73"/>
+    </row>
+    <row r="20" spans="2:9" ht="15" thickBot="1">
+      <c r="B20" s="86" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="69"/>
+      <c r="D20" s="64" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="68"/>
+      <c r="F20" s="68"/>
+      <c r="G20" s="87" t="s">
+        <v>4</v>
+      </c>
+      <c r="H20" s="88">
+        <v>45747</v>
+      </c>
+      <c r="I20" s="69"/>
+    </row>
+    <row r="21" spans="2:9" ht="24.6" thickBot="1">
+      <c r="B21" s="89" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="80"/>
+      <c r="D21" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="F21" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="G21" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H21" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="I21" s="90"/>
+    </row>
+    <row r="22" spans="2:9" ht="15" thickBot="1">
+      <c r="B22" s="91" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="92"/>
+      <c r="D22" s="45" t="s">
+        <v>110</v>
+      </c>
+      <c r="E22" s="93"/>
+      <c r="F22" s="93"/>
+      <c r="G22" s="93"/>
+      <c r="H22" s="93"/>
+      <c r="I22" s="94"/>
+    </row>
+    <row r="23" spans="2:9" ht="28.2" thickBot="1">
+      <c r="B23" s="95" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="96" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="97"/>
+      <c r="E23" s="96" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" s="98"/>
+      <c r="G23" s="99" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23" s="100" t="s">
+        <v>15</v>
+      </c>
+      <c r="I23" s="101" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" ht="235.2" thickBot="1">
+      <c r="B24" s="102">
+        <v>1</v>
+      </c>
+      <c r="C24" s="103" t="s">
+        <v>111</v>
+      </c>
+      <c r="D24" s="104"/>
+      <c r="E24" s="103" t="s">
+        <v>112</v>
+      </c>
+      <c r="F24" s="104"/>
+      <c r="G24" s="105" t="s">
+        <v>113</v>
+      </c>
+      <c r="H24" s="105" t="s">
+        <v>114</v>
+      </c>
+      <c r="I24" s="105" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" ht="124.8" thickBot="1">
+      <c r="B25" s="106">
+        <v>2</v>
+      </c>
+      <c r="C25" s="107" t="s">
+        <v>116</v>
+      </c>
+      <c r="D25" s="108"/>
+      <c r="E25" s="109" t="s">
+        <v>117</v>
+      </c>
+      <c r="F25" s="110"/>
+      <c r="G25" s="111" t="s">
+        <v>118</v>
+      </c>
+      <c r="H25" s="111" t="s">
+        <v>119</v>
+      </c>
+      <c r="I25" s="105" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" ht="15" thickBot="1">
+      <c r="B26" s="112"/>
+      <c r="C26" s="65"/>
+      <c r="D26" s="66"/>
+      <c r="E26" s="65"/>
+      <c r="F26" s="66"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
+    </row>
+    <row r="27" spans="2:9" ht="15" thickBot="1">
+      <c r="B27" s="113" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="114" t="s">
+        <v>120</v>
+      </c>
+      <c r="D27" s="75"/>
+      <c r="E27" s="75"/>
+      <c r="F27" s="75"/>
+      <c r="G27" s="75"/>
+      <c r="H27" s="113" t="s">
+        <v>19</v>
+      </c>
+      <c r="I27" s="19"/>
+    </row>
+    <row r="28" spans="2:9" ht="15" thickBot="1">
+      <c r="B28" s="115" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="73"/>
+      <c r="D28" s="64" t="s">
+        <v>121</v>
+      </c>
+      <c r="E28" s="68"/>
+      <c r="F28" s="68"/>
+      <c r="G28" s="68"/>
+      <c r="H28" s="68"/>
+      <c r="I28" s="69"/>
+    </row>
+  </sheetData>
+  <mergeCells count="36">
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:I28"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:I22"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:I19"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:F8"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B15" location="'Intégration PEA &lt;-&gt; BDD'!B18" display="T1" xr:uid="{BF1BECED-87E0-440D-8B2C-402A5AEC7E39}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7081FA0-4B60-41EA-8343-4988B4EF9AE5}">
   <dimension ref="B2:I20"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="95" zoomScaleNormal="92" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19:F19"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="92" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14:I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -1817,15 +3021,15 @@
       </c>
       <c r="C3" s="56"/>
       <c r="D3" s="57" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E3" s="41"/>
       <c r="F3" s="42"/>
       <c r="G3" s="35" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="H3" s="57" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="I3" s="42"/>
     </row>
@@ -1835,7 +3039,7 @@
       </c>
       <c r="C4" s="42"/>
       <c r="D4" s="60" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="E4" s="37"/>
       <c r="F4" s="37"/>
@@ -1849,7 +3053,7 @@
       </c>
       <c r="C5" s="42"/>
       <c r="D5" s="40" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E5" s="41"/>
       <c r="F5" s="41"/>
@@ -1871,7 +3075,7 @@
         <v>8</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>9</v>
@@ -1884,7 +3088,7 @@
       </c>
       <c r="C7" s="44"/>
       <c r="D7" s="63" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="E7" s="46"/>
       <c r="F7" s="46"/>
@@ -1919,15 +3123,15 @@
         <v>1</v>
       </c>
       <c r="C9" s="62" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D9" s="52"/>
       <c r="E9" s="62" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="F9" s="52"/>
       <c r="G9" s="14" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
@@ -1955,15 +3159,15 @@
       </c>
       <c r="C13" s="56"/>
       <c r="D13" s="57" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="E13" s="41"/>
       <c r="F13" s="42"/>
       <c r="G13" s="35" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="H13" s="57" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="I13" s="42"/>
     </row>
@@ -1973,7 +3177,7 @@
       </c>
       <c r="C14" s="42"/>
       <c r="D14" s="60" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="E14" s="37"/>
       <c r="F14" s="37"/>
@@ -1987,7 +3191,7 @@
       </c>
       <c r="C15" s="42"/>
       <c r="D15" s="40" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E15" s="41"/>
       <c r="F15" s="41"/>
@@ -2009,7 +3213,7 @@
         <v>8</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>9</v>
@@ -2022,7 +3226,7 @@
       </c>
       <c r="C17" s="44"/>
       <c r="D17" s="63" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E17" s="46"/>
       <c r="F17" s="46"/>
@@ -2057,15 +3261,15 @@
         <v>1</v>
       </c>
       <c r="C19" s="62" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="D19" s="52"/>
       <c r="E19" s="62" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="F19" s="52"/>
       <c r="G19" s="14" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="H19" s="14"/>
       <c r="I19" s="14"/>
@@ -2127,12 +3331,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2884834E-433A-4EB2-87FF-F40FDB4BF7E5}">
   <dimension ref="B2:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -2149,7 +3353,7 @@
       </c>
       <c r="C3" s="56"/>
       <c r="D3" s="58" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="E3" s="41"/>
       <c r="F3" s="42"/>
@@ -2157,7 +3361,7 @@
         <v>1</v>
       </c>
       <c r="H3" s="58" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="I3" s="42"/>
     </row>
@@ -2167,7 +3371,7 @@
       </c>
       <c r="C4" s="42"/>
       <c r="D4" s="60" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E4" s="37"/>
       <c r="F4" s="37"/>
@@ -2181,7 +3385,7 @@
       </c>
       <c r="C5" s="42"/>
       <c r="D5" s="64" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E5" s="41"/>
       <c r="F5" s="41"/>
@@ -2202,7 +3406,7 @@
         <v>7</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>8</v>
@@ -2219,7 +3423,7 @@
       </c>
       <c r="C7" s="44"/>
       <c r="D7" s="45" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E7" s="46"/>
       <c r="F7" s="46"/>
@@ -2249,20 +3453,20 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="2:9" ht="144" customHeight="1" thickBot="1">
+    <row r="9" spans="2:9" ht="259.2" customHeight="1" thickBot="1">
       <c r="B9" s="13">
         <v>1</v>
       </c>
       <c r="C9" s="51" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D9" s="52"/>
       <c r="E9" s="51" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F9" s="52"/>
       <c r="G9" s="14" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
@@ -2271,9 +3475,7 @@
       <c r="B10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="36" t="s">
-        <v>18</v>
-      </c>
+      <c r="C10" s="36"/>
       <c r="D10" s="37"/>
       <c r="E10" s="37"/>
       <c r="F10" s="37"/>
@@ -2320,7 +3522,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1017EADE-FD30-4EC7-BAFD-120E9F648406}">
   <dimension ref="B3:I12"/>
   <sheetViews>
@@ -2337,7 +3539,7 @@
       </c>
       <c r="C4" s="56"/>
       <c r="D4" s="58" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="E4" s="41"/>
       <c r="F4" s="42"/>
@@ -2345,7 +3547,7 @@
         <v>1</v>
       </c>
       <c r="H4" s="58" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I4" s="42"/>
     </row>
@@ -2355,7 +3557,7 @@
       </c>
       <c r="C5" s="42"/>
       <c r="D5" s="60" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="E5" s="37"/>
       <c r="F5" s="37"/>
@@ -2369,7 +3571,7 @@
       </c>
       <c r="C6" s="42"/>
       <c r="D6" s="40" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E6" s="41"/>
       <c r="F6" s="41"/>
@@ -2395,7 +3597,7 @@
       </c>
       <c r="G7" s="19"/>
       <c r="H7" s="16" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="I7" s="5"/>
     </row>
@@ -2405,7 +3607,7 @@
       </c>
       <c r="C8" s="44"/>
       <c r="D8" s="45" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="E8" s="46"/>
       <c r="F8" s="46"/>
@@ -2440,15 +3642,15 @@
         <v>1</v>
       </c>
       <c r="C10" s="51" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="D10" s="52"/>
       <c r="E10" s="51" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="F10" s="52"/>
       <c r="G10" s="17" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
@@ -2506,12 +3708,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71593B79-7DFE-41DF-8AB3-C2A73C2E14D0}">
   <dimension ref="B1:I11"/>
   <sheetViews>
     <sheetView zoomScale="93" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:I3"/>
+      <selection activeCell="D2" sqref="D2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -2523,7 +3725,7 @@
       </c>
       <c r="C2" s="56"/>
       <c r="D2" s="58" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="E2" s="41"/>
       <c r="F2" s="42"/>
@@ -2531,7 +3733,7 @@
         <v>1</v>
       </c>
       <c r="H2" s="58" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="I2" s="42"/>
     </row>
@@ -2541,7 +3743,7 @@
       </c>
       <c r="C3" s="42"/>
       <c r="D3" s="60" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="E3" s="37"/>
       <c r="F3" s="37"/>
@@ -2555,7 +3757,7 @@
       </c>
       <c r="C4" s="42"/>
       <c r="D4" s="40" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E4" s="41"/>
       <c r="F4" s="41"/>
@@ -2580,10 +3782,10 @@
         <v>8</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="I5" s="5"/>
     </row>
@@ -2593,7 +3795,7 @@
       </c>
       <c r="C6" s="44"/>
       <c r="D6" s="45" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="E6" s="46"/>
       <c r="F6" s="46"/>
@@ -2628,15 +3830,15 @@
         <v>1</v>
       </c>
       <c r="C8" s="51" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="D8" s="52"/>
       <c r="E8" s="51" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="F8" s="52"/>
       <c r="G8" s="17" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
@@ -2646,15 +3848,15 @@
         <v>2</v>
       </c>
       <c r="C9" s="65" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="D9" s="66"/>
       <c r="E9" s="65" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="F9" s="66"/>
       <c r="G9" s="17" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
@@ -2713,424 +3915,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD219FCF-77B2-490B-816E-2F75E9617605}">
-  <dimension ref="B1:H37"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
-  <cols>
-    <col min="3" max="3" width="35.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" customWidth="1"/>
-    <col min="5" max="5" width="17.5546875" customWidth="1"/>
-    <col min="6" max="6" width="19.5546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:6" ht="15" thickBot="1"/>
-    <row r="2" spans="2:6" ht="55.2" customHeight="1" thickBot="1">
-      <c r="B2" s="76" t="s">
-        <v>73</v>
-      </c>
-      <c r="C2" s="77"/>
-      <c r="D2" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="E2" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="F2" s="23" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" ht="15" thickBot="1">
-      <c r="B3" s="78" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="69"/>
-      <c r="D3" s="67" t="s">
-        <v>83</v>
-      </c>
-      <c r="E3" s="68"/>
-      <c r="F3" s="69"/>
-    </row>
-    <row r="4" spans="2:6" ht="15" thickBot="1">
-      <c r="B4" s="79" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" s="80"/>
-      <c r="D4" s="81" t="s">
-        <v>74</v>
-      </c>
-      <c r="E4" s="82"/>
-      <c r="F4" s="80"/>
-    </row>
-    <row r="5" spans="2:6" ht="15" thickBot="1">
-      <c r="B5" s="71" t="s">
-        <v>56</v>
-      </c>
-      <c r="C5" s="69"/>
-      <c r="D5" s="67" t="s">
-        <v>70</v>
-      </c>
-      <c r="E5" s="68"/>
-      <c r="F5" s="69"/>
-    </row>
-    <row r="6" spans="2:6" ht="42" thickBot="1">
-      <c r="B6" s="72" t="s">
-        <v>57</v>
-      </c>
-      <c r="C6" s="73"/>
-      <c r="D6" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="F6" s="25" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="15" thickBot="1">
-      <c r="B7" s="74" t="s">
-        <v>59</v>
-      </c>
-      <c r="C7" s="75"/>
-      <c r="D7" s="75"/>
-      <c r="E7" s="75"/>
-      <c r="F7" s="73"/>
-    </row>
-    <row r="8" spans="2:6" ht="18" customHeight="1" thickBot="1">
-      <c r="B8" s="70" t="s">
-        <v>60</v>
-      </c>
-      <c r="C8" s="68"/>
-      <c r="D8" s="69"/>
-      <c r="E8" s="70" t="s">
-        <v>61</v>
-      </c>
-      <c r="F8" s="69"/>
-    </row>
-    <row r="9" spans="2:6" ht="36.6" customHeight="1" thickBot="1">
-      <c r="B9" s="67" t="s">
-        <v>84</v>
-      </c>
-      <c r="C9" s="68"/>
-      <c r="D9" s="68"/>
-      <c r="E9" s="67"/>
-      <c r="F9" s="69"/>
-    </row>
-    <row r="10" spans="2:6" ht="15" thickBot="1">
-      <c r="B10" s="70" t="s">
-        <v>62</v>
-      </c>
-      <c r="C10" s="68"/>
-      <c r="D10" s="68"/>
-      <c r="E10" s="68"/>
-      <c r="F10" s="69"/>
-    </row>
-    <row r="11" spans="2:6" ht="20.399999999999999" customHeight="1" thickBot="1">
-      <c r="B11" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="C11" s="27" t="s">
-        <v>64</v>
-      </c>
-      <c r="D11" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="E11" s="27" t="s">
-        <v>66</v>
-      </c>
-      <c r="F11" s="27" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" ht="27" thickBot="1">
-      <c r="B12" s="34" t="s">
-        <v>75</v>
-      </c>
-      <c r="C12" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="D12" s="30" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
-    </row>
-    <row r="13" spans="2:6" ht="27" thickBot="1">
-      <c r="B13" s="34" t="s">
-        <v>94</v>
-      </c>
-      <c r="C13" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="D13" s="30"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29"/>
-    </row>
-    <row r="14" spans="2:6" ht="43.8" customHeight="1" thickBot="1">
-      <c r="B14" s="34" t="s">
-        <v>99</v>
-      </c>
-      <c r="C14" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" s="30"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
-    </row>
-    <row r="15" spans="2:6" ht="30" customHeight="1" thickBot="1">
-      <c r="B15" s="28"/>
-      <c r="C15" s="32"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="31"/>
-    </row>
-    <row r="16" spans="2:6" ht="15" thickBot="1">
-      <c r="B16" s="28"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="31"/>
-    </row>
-    <row r="17" spans="2:8" ht="15" thickBot="1">
-      <c r="B17" s="28"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-    </row>
-    <row r="18" spans="2:8" ht="15" thickBot="1">
-      <c r="B18" s="28"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="31"/>
-    </row>
-    <row r="20" spans="2:8" ht="15" thickBot="1"/>
-    <row r="21" spans="2:8" ht="27" thickBot="1">
-      <c r="B21" s="76" t="s">
-        <v>73</v>
-      </c>
-      <c r="C21" s="77"/>
-      <c r="D21" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="E21" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="F21" s="23" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" ht="15" thickBot="1">
-      <c r="B22" s="78" t="s">
-        <v>2</v>
-      </c>
-      <c r="C22" s="69"/>
-      <c r="D22" s="67" t="s">
-        <v>85</v>
-      </c>
-      <c r="E22" s="68"/>
-      <c r="F22" s="69"/>
-    </row>
-    <row r="23" spans="2:8" ht="15" thickBot="1">
-      <c r="B23" s="79" t="s">
-        <v>55</v>
-      </c>
-      <c r="C23" s="80"/>
-      <c r="D23" s="81" t="s">
-        <v>74</v>
-      </c>
-      <c r="E23" s="82"/>
-      <c r="F23" s="80"/>
-    </row>
-    <row r="24" spans="2:8" ht="15" thickBot="1">
-      <c r="B24" s="71" t="s">
-        <v>56</v>
-      </c>
-      <c r="C24" s="69"/>
-      <c r="D24" s="67" t="s">
-        <v>70</v>
-      </c>
-      <c r="E24" s="68"/>
-      <c r="F24" s="69"/>
-    </row>
-    <row r="25" spans="2:8" ht="42" thickBot="1">
-      <c r="B25" s="72" t="s">
-        <v>57</v>
-      </c>
-      <c r="C25" s="73"/>
-      <c r="D25" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="E25" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="F25" s="25" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" ht="15" thickBot="1">
-      <c r="B26" s="74" t="s">
-        <v>59</v>
-      </c>
-      <c r="C26" s="75"/>
-      <c r="D26" s="75"/>
-      <c r="E26" s="75"/>
-      <c r="F26" s="73"/>
-    </row>
-    <row r="27" spans="2:8" ht="15" thickBot="1">
-      <c r="B27" s="70" t="s">
-        <v>60</v>
-      </c>
-      <c r="C27" s="68"/>
-      <c r="D27" s="69"/>
-      <c r="E27" s="70" t="s">
-        <v>61</v>
-      </c>
-      <c r="F27" s="69"/>
-    </row>
-    <row r="28" spans="2:8" ht="32.4" customHeight="1" thickBot="1">
-      <c r="B28" s="67" t="s">
-        <v>84</v>
-      </c>
-      <c r="C28" s="68"/>
-      <c r="D28" s="68"/>
-      <c r="E28" s="67"/>
-      <c r="F28" s="69"/>
-    </row>
-    <row r="29" spans="2:8" ht="15" thickBot="1">
-      <c r="B29" s="70" t="s">
-        <v>62</v>
-      </c>
-      <c r="C29" s="68"/>
-      <c r="D29" s="68"/>
-      <c r="E29" s="68"/>
-      <c r="F29" s="69"/>
-    </row>
-    <row r="30" spans="2:8" ht="15" thickBot="1">
-      <c r="B30" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="C30" s="27" t="s">
-        <v>64</v>
-      </c>
-      <c r="D30" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="E30" s="27" t="s">
-        <v>66</v>
-      </c>
-      <c r="F30" s="27" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="31" spans="2:8" ht="27" thickBot="1">
-      <c r="B31" s="34" t="s">
-        <v>75</v>
-      </c>
-      <c r="C31" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="D31" s="30" t="s">
-        <v>5</v>
-      </c>
-      <c r="E31" s="29"/>
-      <c r="F31" s="29"/>
-    </row>
-    <row r="32" spans="2:8" ht="27" thickBot="1">
-      <c r="B32" s="34" t="s">
-        <v>102</v>
-      </c>
-      <c r="C32" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="D32" s="30"/>
-      <c r="E32" s="29"/>
-      <c r="F32" s="29"/>
-    </row>
-    <row r="33" spans="2:6" ht="15" thickBot="1">
-      <c r="B33" s="28"/>
-      <c r="C33" s="29"/>
-      <c r="D33" s="30"/>
-      <c r="E33" s="29"/>
-      <c r="F33" s="29"/>
-    </row>
-    <row r="34" spans="2:6" ht="15" thickBot="1">
-      <c r="B34" s="28"/>
-      <c r="C34" s="32"/>
-      <c r="D34" s="30"/>
-      <c r="E34" s="29"/>
-      <c r="F34" s="31"/>
-    </row>
-    <row r="35" spans="2:6" ht="15" thickBot="1">
-      <c r="B35" s="28"/>
-      <c r="C35" s="32"/>
-      <c r="D35" s="30"/>
-      <c r="E35" s="29"/>
-      <c r="F35" s="31"/>
-    </row>
-    <row r="36" spans="2:6" ht="15" thickBot="1">
-      <c r="B36" s="28"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="30"/>
-      <c r="E36" s="29"/>
-      <c r="F36" s="33"/>
-    </row>
-    <row r="37" spans="2:6" ht="15" thickBot="1">
-      <c r="B37" s="28"/>
-      <c r="C37" s="32"/>
-      <c r="D37" s="30"/>
-      <c r="E37" s="29"/>
-      <c r="F37" s="31"/>
-    </row>
-  </sheetData>
-  <mergeCells count="28">
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="E27:F27"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="B12" location="Ethernet!B13" display="T1" xr:uid="{121703C7-11C5-4D45-9096-442FD6A967FB}"/>
-    <hyperlink ref="B31" location="Ethernet!B3" display="T1" xr:uid="{B0CD6564-2A0A-4D2C-93D8-B46585536579}"/>
-    <hyperlink ref="B13" location="RFID!B3" display="T3" xr:uid="{B2AEFDF5-8F01-49D2-A3A0-C26A02A9CC4A}"/>
-    <hyperlink ref="B14" location="Gâche!B4" display="T4" xr:uid="{6AD56DDE-1C0A-4EA1-A077-C61F03A921F9}"/>
-    <hyperlink ref="B32" location="'Alimentation PoE'!B2" display="T5" xr:uid="{EBFF8E81-F438-424D-BF71-85AC823D9304}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Ajout d'un fichier README.md pour la PEA
</commit_message>
<xml_diff>
--- a/PEA/Plan de test/Plan de tests - PEA.xlsx
+++ b/PEA/Plan de test/Plan de tests - PEA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robin\Documents\GITHUB\ACCES_CAMPUS\Acc-s-campus-\PEA\Plan de test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robin\Documents\Github\ACCES_CAMPUS\Acc-s-campus-\PEA\Plan de test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1E6EA26-2472-48CD-BBF8-91EBD8C85E3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D11601D-0709-489F-A072-210B8DB5862E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{21D66C90-57CB-4BB7-B44F-BA6973DF79EF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{21D66C90-57CB-4BB7-B44F-BA6973DF79EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan de tests" sheetId="6" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="129">
   <si>
     <t>Identification du Test</t>
   </si>
@@ -324,9 +324,6 @@
     <t>T3</t>
   </si>
   <si>
-    <t>Le test consisiste à tester la bonne communication entre le microcontrolleur.</t>
-  </si>
-  <si>
     <t>Si l'UID décodé sur l'oscilloscope est le même que celui envoyé.</t>
   </si>
   <si>
@@ -348,15 +345,9 @@
     <t>Placer les broches du multimètres sur les pins de sortie du AG9705 + et -. Passer le multimètres en mode V ( DC). La sortie correspond au pin 7 et 8.</t>
   </si>
   <si>
-    <t>Le test consisiste à tester la bonne communication entre le microcontrolleur via le protocole Wiegand 26b</t>
-  </si>
-  <si>
     <t>Placer les sondes de l'oscilloscope actif sur le PC13 et le PA14. Rélgler la base de temps de l'oscilloscope à 5ms, et le delay à 24.5ms. Regler un Trigger sur CH2 reglé à 4,12V.Réglez la base de tension des 2 canaux à 1V et réglez les offsets sur -2.5V. Appuyez ensuite sur le bouton "Single". Puis lancer la séquence de vérification en scannant un badge RFID. Une fois cela fait comparer la trame obtenu avec la trame attendue ou alors décoder la trame et avoir le même UID que la carte utilisé.</t>
   </si>
   <si>
-    <t>DQ</t>
-  </si>
-  <si>
     <t>Tester le bon fonctionnement de l'incrément 1.</t>
   </si>
   <si>
@@ -364,9 +355,6 @@
   </si>
   <si>
     <t>Salle de cours</t>
-  </si>
-  <si>
-    <t>La base de données et les différents systèmes qui compose le projet "Accès campus", doivent être alimenter et fonctionnel.  Tout les systèmes doivent être minimum à l'incrément 1.</t>
   </si>
   <si>
     <t>Le test permet de vérifier que la communication Ethernet est valide.</t>
@@ -675,6 +663,36 @@
   </si>
   <si>
     <t>T6</t>
+  </si>
+  <si>
+    <t>La base de données et les différents systèmes qui compose le projet "Accès campus", doivent être alimenter et fonctionnel.  Tous les systèmes doivent être minimum à l'incrément 1.</t>
+  </si>
+  <si>
+    <t>Le résultat attendu ressemble à une superposition de signal Wiegand formant une suite d'interruption à intervalle régulié.</t>
+  </si>
+  <si>
+    <t>Une fois les 2 signaux décodé, nous obtenons le même UID lu via le lecteur de badge du PGS.</t>
+  </si>
+  <si>
+    <t>RFID fonctionnel</t>
+  </si>
+  <si>
+    <t>La lecture d'un badge RFID fonctionne correctement.</t>
+  </si>
+  <si>
+    <t>Le test consisiste à tester la bonne communication entre le microcontrolleur et lecteur RFID via le protocole Wiegand 34b</t>
+  </si>
+  <si>
+    <t>Le test consisiste à tester la bonne communication entre le microcontrolleur et lecteur RFID via le protocole Wiegand 34b.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 21/03/2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 24/03/2025</t>
+  </si>
+  <si>
+    <t>La trame envoyé est la même que celle envoyé.</t>
   </si>
 </sst>
 </file>
@@ -1210,19 +1228,127 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1249,185 +1375,77 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1903,8 +1921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD219FCF-77B2-490B-816E-2F75E9617605}">
   <dimension ref="B1:H37"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -1917,10 +1935,10 @@
   <sheetData>
     <row r="1" spans="2:6" ht="15" thickBot="1"/>
     <row r="2" spans="2:6" ht="55.2" customHeight="1" thickBot="1">
-      <c r="B2" s="76" t="s">
+      <c r="B2" s="58" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="77"/>
+      <c r="C2" s="59"/>
       <c r="D2" s="20" t="s">
         <v>61</v>
       </c>
@@ -1932,43 +1950,43 @@
       </c>
     </row>
     <row r="3" spans="2:6" ht="15" thickBot="1">
-      <c r="B3" s="78" t="s">
+      <c r="B3" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="69"/>
-      <c r="D3" s="67" t="s">
+      <c r="C3" s="55"/>
+      <c r="D3" s="56" t="s">
         <v>76</v>
       </c>
-      <c r="E3" s="68"/>
-      <c r="F3" s="69"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="55"/>
     </row>
     <row r="4" spans="2:6" ht="15" thickBot="1">
-      <c r="B4" s="79" t="s">
+      <c r="B4" s="61" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="80"/>
-      <c r="D4" s="81" t="s">
+      <c r="C4" s="62"/>
+      <c r="D4" s="63" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="82"/>
-      <c r="F4" s="80"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="62"/>
     </row>
     <row r="5" spans="2:6" ht="15" thickBot="1">
-      <c r="B5" s="71" t="s">
+      <c r="B5" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="69"/>
-      <c r="D5" s="67" t="s">
+      <c r="C5" s="55"/>
+      <c r="D5" s="56" t="s">
         <v>63</v>
       </c>
-      <c r="E5" s="68"/>
-      <c r="F5" s="69"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="55"/>
     </row>
     <row r="6" spans="2:6" ht="42" thickBot="1">
-      <c r="B6" s="72" t="s">
+      <c r="B6" s="66" t="s">
         <v>50</v>
       </c>
-      <c r="C6" s="73"/>
+      <c r="C6" s="67"/>
       <c r="D6" s="18" t="s">
         <v>22</v>
       </c>
@@ -1980,42 +1998,42 @@
       </c>
     </row>
     <row r="7" spans="2:6" ht="15" thickBot="1">
-      <c r="B7" s="74" t="s">
+      <c r="B7" s="68" t="s">
         <v>52</v>
       </c>
-      <c r="C7" s="75"/>
-      <c r="D7" s="75"/>
-      <c r="E7" s="75"/>
-      <c r="F7" s="73"/>
+      <c r="C7" s="69"/>
+      <c r="D7" s="69"/>
+      <c r="E7" s="69"/>
+      <c r="F7" s="67"/>
     </row>
     <row r="8" spans="2:6" ht="18" customHeight="1" thickBot="1">
-      <c r="B8" s="70" t="s">
+      <c r="B8" s="65" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="68"/>
-      <c r="D8" s="69"/>
-      <c r="E8" s="70" t="s">
+      <c r="C8" s="57"/>
+      <c r="D8" s="55"/>
+      <c r="E8" s="65" t="s">
         <v>54</v>
       </c>
-      <c r="F8" s="69"/>
+      <c r="F8" s="55"/>
     </row>
     <row r="9" spans="2:6" ht="36.6" customHeight="1" thickBot="1">
-      <c r="B9" s="67" t="s">
+      <c r="B9" s="56" t="s">
         <v>77</v>
       </c>
-      <c r="C9" s="68"/>
-      <c r="D9" s="68"/>
-      <c r="E9" s="67"/>
-      <c r="F9" s="69"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="56"/>
+      <c r="F9" s="55"/>
     </row>
     <row r="10" spans="2:6" ht="15" thickBot="1">
-      <c r="B10" s="70" t="s">
+      <c r="B10" s="65" t="s">
         <v>55</v>
       </c>
-      <c r="C10" s="68"/>
-      <c r="D10" s="68"/>
-      <c r="E10" s="68"/>
-      <c r="F10" s="69"/>
+      <c r="C10" s="57"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="55"/>
     </row>
     <row r="11" spans="2:6" ht="20.399999999999999" customHeight="1" thickBot="1">
       <c r="B11" s="26" t="s">
@@ -2042,36 +2060,44 @@
         <v>75</v>
       </c>
       <c r="D12" s="30" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="29"/>
+        <v>126</v>
+      </c>
+      <c r="E12" s="29" t="s">
+        <v>21</v>
+      </c>
       <c r="F12" s="29"/>
     </row>
-    <row r="13" spans="2:6" ht="27" thickBot="1">
+    <row r="13" spans="2:6" ht="42.6" customHeight="1" thickBot="1">
       <c r="B13" s="34" t="s">
         <v>87</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>88</v>
-      </c>
-      <c r="D13" s="30"/>
-      <c r="E13" s="29"/>
+        <v>125</v>
+      </c>
+      <c r="D13" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="E13" s="29" t="s">
+        <v>21</v>
+      </c>
       <c r="F13" s="29"/>
     </row>
     <row r="14" spans="2:6" ht="43.8" customHeight="1" thickBot="1">
       <c r="B14" s="34" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C14" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="30"/>
+      <c r="D14" s="30">
+        <v>45737</v>
+      </c>
       <c r="E14" s="29"/>
       <c r="F14" s="29"/>
     </row>
     <row r="15" spans="2:6" ht="30" customHeight="1" thickBot="1">
-      <c r="B15" s="117" t="s">
-        <v>122</v>
+      <c r="B15" s="50" t="s">
+        <v>118</v>
       </c>
       <c r="C15" s="32" t="s">
         <v>26</v>
@@ -2109,10 +2135,10 @@
     </row>
     <row r="20" spans="2:8" ht="15" thickBot="1"/>
     <row r="21" spans="2:8" ht="27" thickBot="1">
-      <c r="B21" s="76" t="s">
+      <c r="B21" s="58" t="s">
         <v>66</v>
       </c>
-      <c r="C21" s="77"/>
+      <c r="C21" s="59"/>
       <c r="D21" s="20" t="s">
         <v>79</v>
       </c>
@@ -2124,43 +2150,43 @@
       </c>
     </row>
     <row r="22" spans="2:8" ht="15" thickBot="1">
-      <c r="B22" s="78" t="s">
+      <c r="B22" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="C22" s="69"/>
-      <c r="D22" s="67" t="s">
+      <c r="C22" s="55"/>
+      <c r="D22" s="56" t="s">
         <v>78</v>
       </c>
-      <c r="E22" s="68"/>
-      <c r="F22" s="69"/>
+      <c r="E22" s="57"/>
+      <c r="F22" s="55"/>
     </row>
     <row r="23" spans="2:8" ht="15" thickBot="1">
-      <c r="B23" s="79" t="s">
+      <c r="B23" s="61" t="s">
         <v>48</v>
       </c>
-      <c r="C23" s="80"/>
-      <c r="D23" s="81" t="s">
+      <c r="C23" s="62"/>
+      <c r="D23" s="63" t="s">
         <v>67</v>
       </c>
-      <c r="E23" s="82"/>
-      <c r="F23" s="80"/>
+      <c r="E23" s="64"/>
+      <c r="F23" s="62"/>
     </row>
     <row r="24" spans="2:8" ht="15" thickBot="1">
-      <c r="B24" s="71" t="s">
+      <c r="B24" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="C24" s="69"/>
-      <c r="D24" s="67" t="s">
+      <c r="C24" s="55"/>
+      <c r="D24" s="56" t="s">
         <v>63</v>
       </c>
-      <c r="E24" s="68"/>
-      <c r="F24" s="69"/>
+      <c r="E24" s="57"/>
+      <c r="F24" s="55"/>
     </row>
     <row r="25" spans="2:8" ht="42" thickBot="1">
-      <c r="B25" s="72" t="s">
+      <c r="B25" s="66" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="73"/>
+      <c r="C25" s="67"/>
       <c r="D25" s="18" t="s">
         <v>64</v>
       </c>
@@ -2172,42 +2198,42 @@
       </c>
     </row>
     <row r="26" spans="2:8" ht="15" thickBot="1">
-      <c r="B26" s="74" t="s">
+      <c r="B26" s="68" t="s">
         <v>52</v>
       </c>
-      <c r="C26" s="75"/>
-      <c r="D26" s="75"/>
-      <c r="E26" s="75"/>
-      <c r="F26" s="73"/>
+      <c r="C26" s="69"/>
+      <c r="D26" s="69"/>
+      <c r="E26" s="69"/>
+      <c r="F26" s="67"/>
     </row>
     <row r="27" spans="2:8" ht="15" thickBot="1">
-      <c r="B27" s="70" t="s">
+      <c r="B27" s="65" t="s">
         <v>53</v>
       </c>
-      <c r="C27" s="68"/>
-      <c r="D27" s="69"/>
-      <c r="E27" s="70" t="s">
+      <c r="C27" s="57"/>
+      <c r="D27" s="55"/>
+      <c r="E27" s="65" t="s">
         <v>54</v>
       </c>
-      <c r="F27" s="69"/>
+      <c r="F27" s="55"/>
     </row>
     <row r="28" spans="2:8" ht="32.4" customHeight="1" thickBot="1">
-      <c r="B28" s="67" t="s">
+      <c r="B28" s="56" t="s">
         <v>77</v>
       </c>
-      <c r="C28" s="68"/>
-      <c r="D28" s="68"/>
-      <c r="E28" s="67"/>
-      <c r="F28" s="69"/>
+      <c r="C28" s="57"/>
+      <c r="D28" s="57"/>
+      <c r="E28" s="56"/>
+      <c r="F28" s="55"/>
     </row>
     <row r="29" spans="2:8" ht="15" thickBot="1">
-      <c r="B29" s="70" t="s">
+      <c r="B29" s="65" t="s">
         <v>55</v>
       </c>
-      <c r="C29" s="68"/>
-      <c r="D29" s="68"/>
-      <c r="E29" s="68"/>
-      <c r="F29" s="69"/>
+      <c r="C29" s="57"/>
+      <c r="D29" s="57"/>
+      <c r="E29" s="57"/>
+      <c r="F29" s="55"/>
     </row>
     <row r="30" spans="2:8" ht="15" thickBot="1">
       <c r="B30" s="26" t="s">
@@ -2241,7 +2267,7 @@
     </row>
     <row r="32" spans="2:8" ht="27" thickBot="1">
       <c r="B32" s="34" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C32" s="29" t="s">
         <v>40</v>
@@ -2287,25 +2313,6 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:F23"/>
     <mergeCell ref="B28:D28"/>
     <mergeCell ref="E28:F28"/>
     <mergeCell ref="B29:F29"/>
@@ -2315,6 +2322,25 @@
     <mergeCell ref="B26:F26"/>
     <mergeCell ref="B27:D27"/>
     <mergeCell ref="E27:F27"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:F4"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B12" location="Ethernet!B13" display="T1" xr:uid="{121703C7-11C5-4D45-9096-442FD6A967FB}"/>
@@ -2346,151 +2372,151 @@
   <sheetData>
     <row r="2" spans="2:9" ht="15" thickBot="1"/>
     <row r="3" spans="2:9" ht="19.2" customHeight="1">
-      <c r="B3" s="118"/>
-      <c r="C3" s="118"/>
-      <c r="D3" s="118"/>
-      <c r="E3" s="118"/>
-      <c r="F3" s="118"/>
-      <c r="G3" s="118"/>
-      <c r="H3" s="118"/>
-      <c r="I3" s="118"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
     </row>
     <row r="4" spans="2:9">
-      <c r="B4" s="119"/>
-      <c r="C4" s="119"/>
-      <c r="D4" s="119"/>
-      <c r="E4" s="119"/>
-      <c r="F4" s="119"/>
-      <c r="G4" s="119"/>
-      <c r="H4" s="119"/>
-      <c r="I4" s="119"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
     </row>
     <row r="5" spans="2:9">
-      <c r="B5" s="119"/>
-      <c r="C5" s="119"/>
-      <c r="D5" s="119"/>
-      <c r="E5" s="119"/>
-      <c r="F5" s="119"/>
-      <c r="G5" s="119"/>
-      <c r="H5" s="119"/>
-      <c r="I5" s="119"/>
+      <c r="B5" s="52"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="52"/>
     </row>
     <row r="6" spans="2:9" ht="18.600000000000001" customHeight="1">
-      <c r="B6" s="119"/>
-      <c r="C6" s="119"/>
-      <c r="D6" s="119"/>
-      <c r="E6" s="119"/>
-      <c r="F6" s="119"/>
-      <c r="G6" s="119"/>
-      <c r="H6" s="119"/>
-      <c r="I6" s="119"/>
+      <c r="B6" s="52"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="52"/>
+      <c r="I6" s="52"/>
     </row>
     <row r="7" spans="2:9" ht="31.8" customHeight="1">
-      <c r="B7" s="119"/>
-      <c r="C7" s="119"/>
-      <c r="D7" s="119"/>
-      <c r="E7" s="119"/>
-      <c r="F7" s="119"/>
-      <c r="G7" s="119"/>
-      <c r="H7" s="119"/>
-      <c r="I7" s="119"/>
+      <c r="B7" s="52"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="52"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="52"/>
     </row>
     <row r="8" spans="2:9">
-      <c r="B8" s="119"/>
-      <c r="C8" s="119"/>
-      <c r="D8" s="119"/>
-      <c r="E8" s="119"/>
-      <c r="F8" s="119"/>
-      <c r="G8" s="119"/>
-      <c r="H8" s="119"/>
-      <c r="I8" s="119"/>
+      <c r="B8" s="52"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="52"/>
+      <c r="G8" s="52"/>
+      <c r="H8" s="52"/>
+      <c r="I8" s="52"/>
     </row>
     <row r="9" spans="2:9" ht="78" customHeight="1">
-      <c r="B9" s="119"/>
-      <c r="C9" s="119"/>
-      <c r="D9" s="119"/>
-      <c r="E9" s="119"/>
-      <c r="F9" s="119"/>
-      <c r="G9" s="119"/>
-      <c r="H9" s="119"/>
-      <c r="I9" s="119"/>
+      <c r="B9" s="52"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="52"/>
+      <c r="F9" s="52"/>
+      <c r="G9" s="52"/>
+      <c r="H9" s="52"/>
+      <c r="I9" s="52"/>
     </row>
     <row r="10" spans="2:9">
-      <c r="B10" s="119"/>
-      <c r="C10" s="119"/>
-      <c r="D10" s="119"/>
-      <c r="E10" s="119"/>
-      <c r="F10" s="119"/>
-      <c r="G10" s="119"/>
-      <c r="H10" s="119"/>
-      <c r="I10" s="119"/>
+      <c r="B10" s="52"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="52"/>
+      <c r="G10" s="52"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="52"/>
     </row>
     <row r="11" spans="2:9" ht="28.95" customHeight="1" thickBot="1">
-      <c r="B11" s="120"/>
-      <c r="C11" s="120"/>
-      <c r="D11" s="120"/>
-      <c r="E11" s="120"/>
-      <c r="F11" s="120"/>
-      <c r="G11" s="120"/>
-      <c r="H11" s="120"/>
-      <c r="I11" s="120"/>
+      <c r="B11" s="53"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="53"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="53"/>
+      <c r="H11" s="53"/>
+      <c r="I11" s="53"/>
     </row>
     <row r="12" spans="2:9" ht="15" thickBot="1"/>
     <row r="13" spans="2:9" ht="15" thickBot="1">
-      <c r="B13" s="55" t="s">
+      <c r="B13" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="56"/>
-      <c r="D13" s="58" t="s">
-        <v>122</v>
-      </c>
-      <c r="E13" s="41"/>
-      <c r="F13" s="42"/>
+      <c r="C13" s="73"/>
+      <c r="D13" s="74" t="s">
+        <v>118</v>
+      </c>
+      <c r="E13" s="75"/>
+      <c r="F13" s="76"/>
       <c r="G13" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H13" s="58" t="s">
+      <c r="H13" s="74" t="s">
         <v>25</v>
       </c>
-      <c r="I13" s="42"/>
+      <c r="I13" s="76"/>
     </row>
     <row r="14" spans="2:9" ht="15" thickBot="1">
-      <c r="B14" s="59" t="s">
+      <c r="B14" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="42"/>
-      <c r="D14" s="60" t="s">
+      <c r="C14" s="76"/>
+      <c r="D14" s="78" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="37"/>
-      <c r="I14" s="39"/>
+      <c r="E14" s="79"/>
+      <c r="F14" s="79"/>
+      <c r="G14" s="79"/>
+      <c r="H14" s="79"/>
+      <c r="I14" s="80"/>
     </row>
     <row r="15" spans="2:9" ht="15" thickBot="1">
-      <c r="B15" s="59" t="s">
+      <c r="B15" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="42"/>
-      <c r="D15" s="40" t="s">
+      <c r="C15" s="76"/>
+      <c r="D15" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
+      <c r="E15" s="75"/>
+      <c r="F15" s="75"/>
       <c r="G15" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H15" s="61">
+      <c r="H15" s="82">
         <v>45734</v>
       </c>
-      <c r="I15" s="42"/>
+      <c r="I15" s="76"/>
     </row>
     <row r="16" spans="2:9" ht="22.2" thickBot="1">
-      <c r="B16" s="53" t="s">
+      <c r="B16" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="54"/>
+      <c r="C16" s="71"/>
       <c r="D16" s="3" t="s">
         <v>7</v>
       </c>
@@ -2507,31 +2533,31 @@
       <c r="I16" s="5"/>
     </row>
     <row r="17" spans="2:9" ht="28.95" customHeight="1" thickBot="1">
-      <c r="B17" s="43" t="s">
+      <c r="B17" s="85" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="44"/>
-      <c r="D17" s="45" t="s">
+      <c r="C17" s="86"/>
+      <c r="D17" s="87" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="46"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="46"/>
-      <c r="H17" s="46"/>
-      <c r="I17" s="47"/>
+      <c r="E17" s="88"/>
+      <c r="F17" s="88"/>
+      <c r="G17" s="88"/>
+      <c r="H17" s="88"/>
+      <c r="I17" s="89"/>
     </row>
     <row r="18" spans="2:9" ht="28.2" thickBot="1">
       <c r="B18" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="48" t="s">
+      <c r="C18" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="49"/>
-      <c r="E18" s="48" t="s">
+      <c r="D18" s="91"/>
+      <c r="E18" s="90" t="s">
         <v>13</v>
       </c>
-      <c r="F18" s="50"/>
+      <c r="F18" s="92"/>
       <c r="G18" s="10" t="s">
         <v>14</v>
       </c>
@@ -2546,14 +2572,14 @@
       <c r="B19" s="13">
         <v>1</v>
       </c>
-      <c r="C19" s="51" t="s">
+      <c r="C19" s="93" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="52"/>
-      <c r="E19" s="51" t="s">
+      <c r="D19" s="94"/>
+      <c r="E19" s="93" t="s">
         <v>30</v>
       </c>
-      <c r="F19" s="52"/>
+      <c r="F19" s="94"/>
       <c r="G19" s="17" t="s">
         <v>31</v>
       </c>
@@ -2564,33 +2590,42 @@
       <c r="B20" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="36" t="s">
+      <c r="C20" s="83" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="37"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="37"/>
-      <c r="G20" s="37"/>
+      <c r="D20" s="79"/>
+      <c r="E20" s="79"/>
+      <c r="F20" s="79"/>
+      <c r="G20" s="79"/>
       <c r="H20" s="7" t="s">
         <v>19</v>
       </c>
       <c r="I20" s="6"/>
     </row>
     <row r="21" spans="2:9" ht="15" thickBot="1">
-      <c r="B21" s="38" t="s">
+      <c r="B21" s="84" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="39"/>
-      <c r="D21" s="40"/>
-      <c r="E21" s="41"/>
-      <c r="F21" s="41"/>
-      <c r="G21" s="41"/>
-      <c r="H21" s="41"/>
-      <c r="I21" s="42"/>
+      <c r="C21" s="80"/>
+      <c r="D21" s="81"/>
+      <c r="E21" s="75"/>
+      <c r="F21" s="75"/>
+      <c r="G21" s="75"/>
+      <c r="H21" s="75"/>
+      <c r="I21" s="76"/>
     </row>
     <row r="27" spans="2:9" ht="32.4" customHeight="1"/>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:I21"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:I17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:F19"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="D13:F13"/>
@@ -2600,15 +2635,6 @@
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:F15"/>
     <mergeCell ref="H15:I15"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:I21"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:I17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:F19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2618,8 +2644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03C07995-E43A-456B-A3EF-9847E2C4A809}">
   <dimension ref="B4:I28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+    <sheetView zoomScale="68" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -2627,14 +2653,15 @@
     <col min="3" max="3" width="25.6640625" customWidth="1"/>
     <col min="5" max="5" width="17.88671875" customWidth="1"/>
     <col min="6" max="6" width="22.109375" customWidth="1"/>
+    <col min="7" max="7" width="19.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:6" ht="15" thickBot="1"/>
-    <row r="5" spans="2:6" ht="40.200000000000003" thickBot="1">
-      <c r="B5" s="76" t="s">
+    <row r="5" spans="2:6" ht="27" thickBot="1">
+      <c r="B5" s="58" t="s">
         <v>66</v>
       </c>
-      <c r="C5" s="77"/>
+      <c r="C5" s="59"/>
       <c r="D5" s="20" t="s">
         <v>61</v>
       </c>
@@ -2646,43 +2673,43 @@
       </c>
     </row>
     <row r="6" spans="2:6" ht="28.8" customHeight="1" thickBot="1">
-      <c r="B6" s="78" t="s">
+      <c r="B6" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="69"/>
-      <c r="D6" s="67" t="s">
-        <v>99</v>
-      </c>
-      <c r="E6" s="68"/>
-      <c r="F6" s="69"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="56" t="s">
+        <v>96</v>
+      </c>
+      <c r="E6" s="57"/>
+      <c r="F6" s="55"/>
     </row>
     <row r="7" spans="2:6" ht="15" thickBot="1">
-      <c r="B7" s="79" t="s">
+      <c r="B7" s="61" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="80"/>
-      <c r="D7" s="81" t="s">
-        <v>100</v>
-      </c>
-      <c r="E7" s="82"/>
-      <c r="F7" s="80"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="63" t="s">
+        <v>97</v>
+      </c>
+      <c r="E7" s="64"/>
+      <c r="F7" s="62"/>
     </row>
     <row r="8" spans="2:6" ht="15" thickBot="1">
-      <c r="B8" s="71" t="s">
+      <c r="B8" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="69"/>
-      <c r="D8" s="67" t="s">
-        <v>101</v>
-      </c>
-      <c r="E8" s="68"/>
-      <c r="F8" s="69"/>
-    </row>
-    <row r="9" spans="2:6" ht="28.2" thickBot="1">
-      <c r="B9" s="72" t="s">
+      <c r="C8" s="55"/>
+      <c r="D8" s="56" t="s">
+        <v>98</v>
+      </c>
+      <c r="E8" s="57"/>
+      <c r="F8" s="55"/>
+    </row>
+    <row r="9" spans="2:6" ht="15" thickBot="1">
+      <c r="B9" s="66" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="73"/>
+      <c r="C9" s="67"/>
       <c r="D9" s="18"/>
       <c r="E9" s="24" t="s">
         <v>51</v>
@@ -2690,42 +2717,42 @@
       <c r="F9" s="25"/>
     </row>
     <row r="10" spans="2:6" ht="15" thickBot="1">
-      <c r="B10" s="74" t="s">
+      <c r="B10" s="68" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="75"/>
-      <c r="D10" s="75"/>
-      <c r="E10" s="75"/>
-      <c r="F10" s="73"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="67"/>
     </row>
     <row r="11" spans="2:6" ht="15" thickBot="1">
-      <c r="B11" s="70" t="s">
+      <c r="B11" s="65" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="68"/>
-      <c r="D11" s="69"/>
-      <c r="E11" s="70" t="s">
+      <c r="C11" s="57"/>
+      <c r="D11" s="55"/>
+      <c r="E11" s="65" t="s">
         <v>54</v>
       </c>
-      <c r="F11" s="69"/>
+      <c r="F11" s="55"/>
     </row>
     <row r="12" spans="2:6" ht="82.8" customHeight="1" thickBot="1">
-      <c r="B12" s="67" t="s">
-        <v>102</v>
-      </c>
-      <c r="C12" s="68"/>
-      <c r="D12" s="68"/>
-      <c r="E12" s="67"/>
-      <c r="F12" s="69"/>
+      <c r="B12" s="56" t="s">
+        <v>119</v>
+      </c>
+      <c r="C12" s="57"/>
+      <c r="D12" s="57"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="55"/>
     </row>
     <row r="13" spans="2:6" ht="15" thickBot="1">
-      <c r="B13" s="70" t="s">
+      <c r="B13" s="65" t="s">
         <v>55</v>
       </c>
-      <c r="C13" s="68"/>
-      <c r="D13" s="68"/>
-      <c r="E13" s="68"/>
-      <c r="F13" s="69"/>
+      <c r="C13" s="57"/>
+      <c r="D13" s="57"/>
+      <c r="E13" s="57"/>
+      <c r="F13" s="55"/>
     </row>
     <row r="14" spans="2:6" ht="15" thickBot="1">
       <c r="B14" s="26" t="s">
@@ -2745,83 +2772,83 @@
       </c>
     </row>
     <row r="15" spans="2:6" ht="65.400000000000006" customHeight="1" thickBot="1">
-      <c r="B15" s="117" t="s">
+      <c r="B15" s="50" t="s">
         <v>68</v>
       </c>
-      <c r="C15" s="116" t="s">
-        <v>103</v>
+      <c r="C15" s="49" t="s">
+        <v>99</v>
       </c>
       <c r="D15" s="30">
         <v>45747</v>
       </c>
       <c r="E15" s="29" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F15" s="29" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="2:9" ht="15" thickBot="1"/>
     <row r="18" spans="2:9" ht="15" thickBot="1">
-      <c r="B18" s="83" t="s">
+      <c r="B18" s="116" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="84"/>
-      <c r="D18" s="58" t="s">
+      <c r="C18" s="117"/>
+      <c r="D18" s="74" t="s">
         <v>68</v>
       </c>
-      <c r="E18" s="68"/>
-      <c r="F18" s="69"/>
-      <c r="G18" s="85" t="s">
-        <v>106</v>
-      </c>
-      <c r="H18" s="58" t="s">
-        <v>107</v>
-      </c>
-      <c r="I18" s="69"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="55"/>
+      <c r="G18" s="36" t="s">
+        <v>102</v>
+      </c>
+      <c r="H18" s="74" t="s">
+        <v>103</v>
+      </c>
+      <c r="I18" s="55"/>
     </row>
     <row r="19" spans="2:9" ht="15" thickBot="1">
-      <c r="B19" s="86" t="s">
+      <c r="B19" s="109" t="s">
         <v>2</v>
       </c>
-      <c r="C19" s="69"/>
-      <c r="D19" s="60" t="s">
-        <v>103</v>
-      </c>
-      <c r="E19" s="75"/>
-      <c r="F19" s="75"/>
-      <c r="G19" s="75"/>
-      <c r="H19" s="75"/>
-      <c r="I19" s="73"/>
+      <c r="C19" s="55"/>
+      <c r="D19" s="78" t="s">
+        <v>99</v>
+      </c>
+      <c r="E19" s="69"/>
+      <c r="F19" s="69"/>
+      <c r="G19" s="69"/>
+      <c r="H19" s="69"/>
+      <c r="I19" s="67"/>
     </row>
     <row r="20" spans="2:9" ht="15" thickBot="1">
-      <c r="B20" s="86" t="s">
+      <c r="B20" s="109" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="69"/>
-      <c r="D20" s="64" t="s">
+      <c r="C20" s="55"/>
+      <c r="D20" s="99" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="68"/>
-      <c r="F20" s="68"/>
-      <c r="G20" s="87" t="s">
+      <c r="E20" s="57"/>
+      <c r="F20" s="57"/>
+      <c r="G20" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="H20" s="88">
+      <c r="H20" s="110">
         <v>45747</v>
       </c>
-      <c r="I20" s="69"/>
+      <c r="I20" s="55"/>
     </row>
     <row r="21" spans="2:9" ht="24.6" thickBot="1">
-      <c r="B21" s="89" t="s">
+      <c r="B21" s="111" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="80"/>
+      <c r="C21" s="62"/>
       <c r="D21" s="20" t="s">
         <v>7</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="F21" s="20" t="s">
         <v>8</v>
@@ -2830,168 +2857,168 @@
         <v>22</v>
       </c>
       <c r="H21" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="I21" s="90"/>
+        <v>105</v>
+      </c>
+      <c r="I21" s="38"/>
     </row>
     <row r="22" spans="2:9" ht="15" thickBot="1">
-      <c r="B22" s="91" t="s">
+      <c r="B22" s="112" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="92"/>
-      <c r="D22" s="45" t="s">
-        <v>110</v>
-      </c>
-      <c r="E22" s="93"/>
-      <c r="F22" s="93"/>
-      <c r="G22" s="93"/>
-      <c r="H22" s="93"/>
-      <c r="I22" s="94"/>
+      <c r="C22" s="113"/>
+      <c r="D22" s="87" t="s">
+        <v>106</v>
+      </c>
+      <c r="E22" s="114"/>
+      <c r="F22" s="114"/>
+      <c r="G22" s="114"/>
+      <c r="H22" s="114"/>
+      <c r="I22" s="115"/>
     </row>
     <row r="23" spans="2:9" ht="28.2" thickBot="1">
-      <c r="B23" s="95" t="s">
+      <c r="B23" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="96" t="s">
+      <c r="C23" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="D23" s="97"/>
-      <c r="E23" s="96" t="s">
+      <c r="D23" s="101"/>
+      <c r="E23" s="100" t="s">
         <v>13</v>
       </c>
-      <c r="F23" s="98"/>
-      <c r="G23" s="99" t="s">
+      <c r="F23" s="102"/>
+      <c r="G23" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="H23" s="100" t="s">
+      <c r="H23" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="I23" s="101" t="s">
+      <c r="I23" s="42" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="2:9" ht="235.2" thickBot="1">
-      <c r="B24" s="102">
+    <row r="24" spans="2:9" ht="166.2" customHeight="1" thickBot="1">
+      <c r="B24" s="43">
         <v>1</v>
       </c>
       <c r="C24" s="103" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D24" s="104"/>
       <c r="E24" s="103" t="s">
+        <v>108</v>
+      </c>
+      <c r="F24" s="104"/>
+      <c r="G24" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="H24" s="44" t="s">
+        <v>110</v>
+      </c>
+      <c r="I24" s="44" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" ht="124.8" thickBot="1">
+      <c r="B25" s="45">
+        <v>2</v>
+      </c>
+      <c r="C25" s="105" t="s">
         <v>112</v>
       </c>
-      <c r="F24" s="104"/>
-      <c r="G24" s="105" t="s">
+      <c r="D25" s="106"/>
+      <c r="E25" s="107" t="s">
         <v>113</v>
       </c>
-      <c r="H24" s="105" t="s">
+      <c r="F25" s="108"/>
+      <c r="G25" s="46" t="s">
         <v>114</v>
       </c>
-      <c r="I24" s="105" t="s">
+      <c r="H25" s="46" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="25" spans="2:9" ht="124.8" thickBot="1">
-      <c r="B25" s="106">
-        <v>2</v>
-      </c>
-      <c r="C25" s="107" t="s">
-        <v>116</v>
-      </c>
-      <c r="D25" s="108"/>
-      <c r="E25" s="109" t="s">
-        <v>117</v>
-      </c>
-      <c r="F25" s="110"/>
-      <c r="G25" s="111" t="s">
-        <v>118</v>
-      </c>
-      <c r="H25" s="111" t="s">
-        <v>119</v>
-      </c>
-      <c r="I25" s="105" t="s">
-        <v>115</v>
+      <c r="I25" s="44" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="26" spans="2:9" ht="15" thickBot="1">
-      <c r="B26" s="112"/>
-      <c r="C26" s="65"/>
-      <c r="D26" s="66"/>
-      <c r="E26" s="65"/>
-      <c r="F26" s="66"/>
+      <c r="B26" s="47"/>
+      <c r="C26" s="95"/>
+      <c r="D26" s="96"/>
+      <c r="E26" s="95"/>
+      <c r="F26" s="96"/>
       <c r="G26" s="17"/>
       <c r="H26" s="17"/>
       <c r="I26" s="17"/>
     </row>
     <row r="27" spans="2:9" ht="15" thickBot="1">
-      <c r="B27" s="113" t="s">
+      <c r="B27" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="114" t="s">
-        <v>120</v>
-      </c>
-      <c r="D27" s="75"/>
-      <c r="E27" s="75"/>
-      <c r="F27" s="75"/>
-      <c r="G27" s="75"/>
-      <c r="H27" s="113" t="s">
+      <c r="C27" s="97" t="s">
+        <v>116</v>
+      </c>
+      <c r="D27" s="69"/>
+      <c r="E27" s="69"/>
+      <c r="F27" s="69"/>
+      <c r="G27" s="69"/>
+      <c r="H27" s="48" t="s">
         <v>19</v>
       </c>
       <c r="I27" s="19"/>
     </row>
     <row r="28" spans="2:9" ht="15" thickBot="1">
-      <c r="B28" s="115" t="s">
+      <c r="B28" s="98" t="s">
         <v>20</v>
       </c>
-      <c r="C28" s="73"/>
-      <c r="D28" s="64" t="s">
-        <v>121</v>
-      </c>
-      <c r="E28" s="68"/>
-      <c r="F28" s="68"/>
-      <c r="G28" s="68"/>
-      <c r="H28" s="68"/>
-      <c r="I28" s="69"/>
+      <c r="C28" s="67"/>
+      <c r="D28" s="99" t="s">
+        <v>117</v>
+      </c>
+      <c r="E28" s="57"/>
+      <c r="F28" s="57"/>
+      <c r="G28" s="57"/>
+      <c r="H28" s="57"/>
+      <c r="I28" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D28:I28"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:I19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:I22"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="E23:F23"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="E24:F24"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="E25:F25"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:I22"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:I19"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:I28"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B15" location="'Intégration PEA &lt;-&gt; BDD'!B18" display="T1" xr:uid="{BF1BECED-87E0-440D-8B2C-402A5AEC7E39}"/>
@@ -3004,8 +3031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7081FA0-4B60-41EA-8343-4988B4EF9AE5}">
   <dimension ref="B2:I20"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="92" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14:I14"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="92" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15:I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -3016,58 +3043,58 @@
   <sheetData>
     <row r="2" spans="2:9" ht="15" thickBot="1"/>
     <row r="3" spans="2:9" ht="18.600000000000001" customHeight="1" thickBot="1">
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="56"/>
-      <c r="D3" s="57" t="s">
+      <c r="C3" s="73"/>
+      <c r="D3" s="119" t="s">
         <v>68</v>
       </c>
-      <c r="E3" s="41"/>
-      <c r="F3" s="42"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="76"/>
       <c r="G3" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="H3" s="57" t="s">
+      <c r="H3" s="119" t="s">
         <v>70</v>
       </c>
-      <c r="I3" s="42"/>
+      <c r="I3" s="76"/>
     </row>
     <row r="4" spans="2:9" ht="15" thickBot="1">
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="42"/>
-      <c r="D4" s="60" t="s">
+      <c r="C4" s="76"/>
+      <c r="D4" s="78" t="s">
         <v>75</v>
       </c>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="39"/>
+      <c r="E4" s="79"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="79"/>
+      <c r="H4" s="79"/>
+      <c r="I4" s="80"/>
     </row>
     <row r="5" spans="2:9" ht="15" thickBot="1">
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="42"/>
-      <c r="D5" s="40" t="s">
+      <c r="C5" s="76"/>
+      <c r="D5" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
       <c r="G5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="61"/>
-      <c r="I5" s="42"/>
+      <c r="H5" s="82"/>
+      <c r="I5" s="76"/>
     </row>
     <row r="6" spans="2:9" ht="19.8" customHeight="1" thickBot="1">
-      <c r="B6" s="53" t="s">
+      <c r="B6" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="54"/>
+      <c r="C6" s="71"/>
       <c r="D6" s="3" t="s">
         <v>7</v>
       </c>
@@ -3083,31 +3110,31 @@
       <c r="I6" s="5"/>
     </row>
     <row r="7" spans="2:9" ht="15" thickBot="1">
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="85" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="44"/>
-      <c r="D7" s="63" t="s">
+      <c r="C7" s="86"/>
+      <c r="D7" s="120" t="s">
         <v>82</v>
       </c>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
-      <c r="I7" s="47"/>
+      <c r="E7" s="88"/>
+      <c r="F7" s="88"/>
+      <c r="G7" s="88"/>
+      <c r="H7" s="88"/>
+      <c r="I7" s="89"/>
     </row>
     <row r="8" spans="2:9" ht="28.2" thickBot="1">
       <c r="B8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="48" t="s">
+      <c r="C8" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="49"/>
-      <c r="E8" s="48" t="s">
+      <c r="D8" s="91"/>
+      <c r="E8" s="90" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="50"/>
+      <c r="F8" s="92"/>
       <c r="G8" s="10" t="s">
         <v>14</v>
       </c>
@@ -3122,14 +3149,14 @@
       <c r="B9" s="13">
         <v>1</v>
       </c>
-      <c r="C9" s="62" t="s">
+      <c r="C9" s="118" t="s">
         <v>72</v>
       </c>
-      <c r="D9" s="52"/>
-      <c r="E9" s="62" t="s">
+      <c r="D9" s="94"/>
+      <c r="E9" s="118" t="s">
         <v>73</v>
       </c>
-      <c r="F9" s="52"/>
+      <c r="F9" s="94"/>
       <c r="G9" s="14" t="s">
         <v>74</v>
       </c>
@@ -3140,13 +3167,13 @@
       <c r="B10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="36" t="s">
+      <c r="C10" s="83" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="37"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="37"/>
+      <c r="D10" s="79"/>
+      <c r="E10" s="79"/>
+      <c r="F10" s="79"/>
+      <c r="G10" s="79"/>
       <c r="H10" s="7" t="s">
         <v>19</v>
       </c>
@@ -3154,58 +3181,58 @@
     </row>
     <row r="12" spans="2:9" ht="15" thickBot="1"/>
     <row r="13" spans="2:9" ht="19.8" customHeight="1" thickBot="1">
-      <c r="B13" s="55" t="s">
+      <c r="B13" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="56"/>
-      <c r="D13" s="57" t="s">
+      <c r="C13" s="73"/>
+      <c r="D13" s="119" t="s">
         <v>86</v>
       </c>
-      <c r="E13" s="41"/>
-      <c r="F13" s="42"/>
+      <c r="E13" s="75"/>
+      <c r="F13" s="76"/>
       <c r="G13" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="H13" s="57" t="s">
+      <c r="H13" s="119" t="s">
         <v>81</v>
       </c>
-      <c r="I13" s="42"/>
+      <c r="I13" s="76"/>
     </row>
     <row r="14" spans="2:9" ht="15" thickBot="1">
-      <c r="B14" s="59" t="s">
+      <c r="B14" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="42"/>
-      <c r="D14" s="60" t="s">
+      <c r="C14" s="76"/>
+      <c r="D14" s="78" t="s">
         <v>80</v>
       </c>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="37"/>
-      <c r="I14" s="39"/>
+      <c r="E14" s="79"/>
+      <c r="F14" s="79"/>
+      <c r="G14" s="79"/>
+      <c r="H14" s="79"/>
+      <c r="I14" s="80"/>
     </row>
     <row r="15" spans="2:9" ht="15" thickBot="1">
-      <c r="B15" s="59" t="s">
+      <c r="B15" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="42"/>
-      <c r="D15" s="40" t="s">
+      <c r="C15" s="76"/>
+      <c r="D15" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
+      <c r="E15" s="75"/>
+      <c r="F15" s="75"/>
       <c r="G15" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H15" s="61"/>
-      <c r="I15" s="42"/>
+      <c r="H15" s="82"/>
+      <c r="I15" s="76"/>
     </row>
     <row r="16" spans="2:9" ht="28.2" thickBot="1">
-      <c r="B16" s="53" t="s">
+      <c r="B16" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="54"/>
+      <c r="C16" s="71"/>
       <c r="D16" s="3" t="s">
         <v>7</v>
       </c>
@@ -3221,31 +3248,31 @@
       <c r="I16" s="5"/>
     </row>
     <row r="17" spans="2:9" ht="15" thickBot="1">
-      <c r="B17" s="43" t="s">
+      <c r="B17" s="85" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="44"/>
-      <c r="D17" s="63" t="s">
+      <c r="C17" s="86"/>
+      <c r="D17" s="120" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="46"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="46"/>
-      <c r="H17" s="46"/>
-      <c r="I17" s="47"/>
+      <c r="E17" s="88"/>
+      <c r="F17" s="88"/>
+      <c r="G17" s="88"/>
+      <c r="H17" s="88"/>
+      <c r="I17" s="89"/>
     </row>
     <row r="18" spans="2:9" ht="28.2" thickBot="1">
       <c r="B18" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="48" t="s">
+      <c r="C18" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="49"/>
-      <c r="E18" s="48" t="s">
+      <c r="D18" s="91"/>
+      <c r="E18" s="90" t="s">
         <v>13</v>
       </c>
-      <c r="F18" s="50"/>
+      <c r="F18" s="92"/>
       <c r="G18" s="10" t="s">
         <v>14</v>
       </c>
@@ -3260,31 +3287,35 @@
       <c r="B19" s="13">
         <v>1</v>
       </c>
-      <c r="C19" s="62" t="s">
+      <c r="C19" s="118" t="s">
         <v>83</v>
       </c>
-      <c r="D19" s="52"/>
-      <c r="E19" s="62" t="s">
+      <c r="D19" s="94"/>
+      <c r="E19" s="118" t="s">
         <v>84</v>
       </c>
-      <c r="F19" s="52"/>
+      <c r="F19" s="94"/>
       <c r="G19" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
+      <c r="H19" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="I19" s="14" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="20" spans="2:9" ht="15" thickBot="1">
       <c r="B20" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="36" t="s">
+      <c r="C20" s="83" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="37"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="37"/>
-      <c r="G20" s="37"/>
+      <c r="D20" s="79"/>
+      <c r="E20" s="79"/>
+      <c r="F20" s="79"/>
+      <c r="G20" s="79"/>
       <c r="H20" s="7" t="s">
         <v>19</v>
       </c>
@@ -3292,6 +3323,23 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:I17"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:I14"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="B3:C3"/>
@@ -3307,23 +3355,6 @@
     <mergeCell ref="D7:I7"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="E8:F8"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:I14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:I17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="C20:G20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -3335,8 +3366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2884834E-433A-4EB2-87FF-F40FDB4BF7E5}">
   <dimension ref="B2:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9:F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -3348,60 +3379,60 @@
   <sheetData>
     <row r="2" spans="2:9" ht="15" thickBot="1"/>
     <row r="3" spans="2:9" ht="19.8" customHeight="1" thickBot="1">
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="56"/>
-      <c r="D3" s="58" t="s">
+      <c r="C3" s="73"/>
+      <c r="D3" s="74" t="s">
         <v>87</v>
       </c>
-      <c r="E3" s="41"/>
-      <c r="F3" s="42"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="76"/>
       <c r="G3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="58" t="s">
+      <c r="H3" s="74" t="s">
         <v>37</v>
       </c>
-      <c r="I3" s="42"/>
+      <c r="I3" s="76"/>
     </row>
     <row r="4" spans="2:9" ht="15" thickBot="1">
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="42"/>
-      <c r="D4" s="60" t="s">
-        <v>96</v>
-      </c>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="39"/>
+      <c r="C4" s="76"/>
+      <c r="D4" s="78" t="s">
+        <v>124</v>
+      </c>
+      <c r="E4" s="79"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="79"/>
+      <c r="H4" s="79"/>
+      <c r="I4" s="80"/>
     </row>
     <row r="5" spans="2:9" ht="15" thickBot="1">
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="42"/>
-      <c r="D5" s="64" t="s">
+      <c r="C5" s="76"/>
+      <c r="D5" s="99" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
       <c r="G5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="61">
+      <c r="H5" s="82">
         <v>45734</v>
       </c>
-      <c r="I5" s="42"/>
+      <c r="I5" s="76"/>
     </row>
     <row r="6" spans="2:9" ht="20.399999999999999" customHeight="1" thickBot="1">
-      <c r="B6" s="53" t="s">
+      <c r="B6" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="54"/>
+      <c r="C6" s="71"/>
       <c r="D6" s="3" t="s">
         <v>7</v>
       </c>
@@ -3411,38 +3442,40 @@
       <c r="F6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="19"/>
+      <c r="G6" s="19" t="s">
+        <v>22</v>
+      </c>
       <c r="H6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="I6" s="5"/>
     </row>
     <row r="7" spans="2:9" ht="33" customHeight="1" thickBot="1">
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="85" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="44"/>
-      <c r="D7" s="45" t="s">
+      <c r="C7" s="86"/>
+      <c r="D7" s="87" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
-      <c r="I7" s="47"/>
+      <c r="E7" s="88"/>
+      <c r="F7" s="88"/>
+      <c r="G7" s="88"/>
+      <c r="H7" s="88"/>
+      <c r="I7" s="89"/>
     </row>
     <row r="8" spans="2:9" ht="28.2" thickBot="1">
       <c r="B8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="48" t="s">
+      <c r="C8" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="49"/>
-      <c r="E8" s="48" t="s">
+      <c r="D8" s="91"/>
+      <c r="E8" s="90" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="50"/>
+      <c r="F8" s="92"/>
       <c r="G8" s="10" t="s">
         <v>14</v>
       </c>
@@ -3457,56 +3490,56 @@
       <c r="B9" s="13">
         <v>1</v>
       </c>
-      <c r="C9" s="51" t="s">
-        <v>97</v>
-      </c>
-      <c r="D9" s="52"/>
-      <c r="E9" s="51" t="s">
-        <v>98</v>
-      </c>
-      <c r="F9" s="52"/>
+      <c r="C9" s="93" t="s">
+        <v>95</v>
+      </c>
+      <c r="D9" s="94"/>
+      <c r="E9" s="93" t="s">
+        <v>120</v>
+      </c>
+      <c r="F9" s="94"/>
       <c r="G9" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
+        <v>88</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="I9" s="14" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="10" spans="2:9" ht="15" thickBot="1">
       <c r="B10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="36"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="37"/>
+      <c r="C10" s="83" t="s">
+        <v>122</v>
+      </c>
+      <c r="D10" s="79"/>
+      <c r="E10" s="79"/>
+      <c r="F10" s="79"/>
+      <c r="G10" s="79"/>
       <c r="H10" s="7" t="s">
         <v>19</v>
       </c>
       <c r="I10" s="6"/>
     </row>
     <row r="11" spans="2:9" ht="15" thickBot="1">
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="84" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="39"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="42"/>
+      <c r="C11" s="80"/>
+      <c r="D11" s="81" t="s">
+        <v>123</v>
+      </c>
+      <c r="E11" s="75"/>
+      <c r="F11" s="75"/>
+      <c r="G11" s="75"/>
+      <c r="H11" s="75"/>
+      <c r="I11" s="76"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:I4"/>
     <mergeCell ref="C10:G10"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="D11:I11"/>
@@ -3517,6 +3550,14 @@
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="E9:F9"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3534,60 +3575,60 @@
   <sheetData>
     <row r="3" spans="2:9" ht="15" thickBot="1"/>
     <row r="4" spans="2:9" ht="28.2" thickBot="1">
-      <c r="B4" s="55" t="s">
+      <c r="B4" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="56"/>
-      <c r="D4" s="58" t="s">
-        <v>90</v>
-      </c>
-      <c r="E4" s="41"/>
-      <c r="F4" s="42"/>
+      <c r="C4" s="73"/>
+      <c r="D4" s="74" t="s">
+        <v>89</v>
+      </c>
+      <c r="E4" s="75"/>
+      <c r="F4" s="76"/>
       <c r="G4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="58" t="s">
+      <c r="H4" s="74" t="s">
         <v>33</v>
       </c>
-      <c r="I4" s="42"/>
+      <c r="I4" s="76"/>
     </row>
     <row r="5" spans="2:9" ht="15" thickBot="1">
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="42"/>
-      <c r="D5" s="60" t="s">
+      <c r="C5" s="76"/>
+      <c r="D5" s="78" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="39"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
+      <c r="G5" s="79"/>
+      <c r="H5" s="79"/>
+      <c r="I5" s="80"/>
     </row>
     <row r="6" spans="2:9" ht="15" thickBot="1">
-      <c r="B6" s="59" t="s">
+      <c r="B6" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="42"/>
-      <c r="D6" s="40" t="s">
+      <c r="C6" s="76"/>
+      <c r="D6" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
+      <c r="E6" s="75"/>
+      <c r="F6" s="75"/>
       <c r="G6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="61">
+      <c r="H6" s="82">
         <v>45734</v>
       </c>
-      <c r="I6" s="42"/>
+      <c r="I6" s="76"/>
     </row>
     <row r="7" spans="2:9" ht="24.6" thickBot="1">
-      <c r="B7" s="53" t="s">
+      <c r="B7" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="54"/>
+      <c r="C7" s="71"/>
       <c r="D7" s="3" t="s">
         <v>7</v>
       </c>
@@ -3602,31 +3643,31 @@
       <c r="I7" s="5"/>
     </row>
     <row r="8" spans="2:9" ht="28.95" customHeight="1" thickBot="1">
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="85" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="44"/>
-      <c r="D8" s="45" t="s">
+      <c r="C8" s="86"/>
+      <c r="D8" s="87" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
-      <c r="I8" s="47"/>
+      <c r="E8" s="88"/>
+      <c r="F8" s="88"/>
+      <c r="G8" s="88"/>
+      <c r="H8" s="88"/>
+      <c r="I8" s="89"/>
     </row>
     <row r="9" spans="2:9" ht="28.2" thickBot="1">
       <c r="B9" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="48" t="s">
+      <c r="C9" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="49"/>
-      <c r="E9" s="48" t="s">
+      <c r="D9" s="91"/>
+      <c r="E9" s="90" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="50"/>
+      <c r="F9" s="92"/>
       <c r="G9" s="10" t="s">
         <v>14</v>
       </c>
@@ -3641,14 +3682,14 @@
       <c r="B10" s="13">
         <v>1</v>
       </c>
-      <c r="C10" s="51" t="s">
+      <c r="C10" s="93" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10" s="94"/>
+      <c r="E10" s="93" t="s">
         <v>91</v>
       </c>
-      <c r="D10" s="52"/>
-      <c r="E10" s="51" t="s">
-        <v>92</v>
-      </c>
-      <c r="F10" s="52"/>
+      <c r="F10" s="94"/>
       <c r="G10" s="17" t="s">
         <v>36</v>
       </c>
@@ -3659,40 +3700,32 @@
       <c r="B11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="36" t="s">
+      <c r="C11" s="83" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="37"/>
+      <c r="D11" s="79"/>
+      <c r="E11" s="79"/>
+      <c r="F11" s="79"/>
+      <c r="G11" s="79"/>
       <c r="H11" s="7" t="s">
         <v>19</v>
       </c>
       <c r="I11" s="6"/>
     </row>
     <row r="12" spans="2:9" ht="15" thickBot="1">
-      <c r="B12" s="38" t="s">
+      <c r="B12" s="84" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="39"/>
-      <c r="D12" s="40"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="41"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="41"/>
-      <c r="I12" s="42"/>
+      <c r="C12" s="80"/>
+      <c r="D12" s="81"/>
+      <c r="E12" s="75"/>
+      <c r="F12" s="75"/>
+      <c r="G12" s="75"/>
+      <c r="H12" s="75"/>
+      <c r="I12" s="76"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:I5"/>
     <mergeCell ref="C11:G11"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="D12:I12"/>
@@ -3703,6 +3736,14 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="E10:F10"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:I5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3712,7 +3753,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71593B79-7DFE-41DF-8AB3-C2A73C2E14D0}">
   <dimension ref="B1:I11"/>
   <sheetViews>
-    <sheetView zoomScale="93" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScale="93" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="D2" sqref="D2:F2"/>
     </sheetView>
   </sheetViews>
@@ -3720,60 +3761,60 @@
   <sheetData>
     <row r="1" spans="2:9" ht="15" thickBot="1"/>
     <row r="2" spans="2:9" ht="28.2" thickBot="1">
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="56"/>
-      <c r="D2" s="58" t="s">
-        <v>93</v>
-      </c>
-      <c r="E2" s="41"/>
-      <c r="F2" s="42"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="74" t="s">
+        <v>92</v>
+      </c>
+      <c r="E2" s="75"/>
+      <c r="F2" s="76"/>
       <c r="G2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="58" t="s">
+      <c r="H2" s="74" t="s">
         <v>39</v>
       </c>
-      <c r="I2" s="42"/>
+      <c r="I2" s="76"/>
     </row>
     <row r="3" spans="2:9" ht="15" customHeight="1" thickBot="1">
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="42"/>
-      <c r="D3" s="60" t="s">
+      <c r="C3" s="76"/>
+      <c r="D3" s="78" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="39"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="80"/>
     </row>
     <row r="4" spans="2:9" ht="15" thickBot="1">
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="42"/>
-      <c r="D4" s="40" t="s">
+      <c r="C4" s="76"/>
+      <c r="D4" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
       <c r="G4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="61">
+      <c r="H4" s="82">
         <v>45734</v>
       </c>
-      <c r="I4" s="42"/>
+      <c r="I4" s="76"/>
     </row>
     <row r="5" spans="2:9" ht="24.6" thickBot="1">
-      <c r="B5" s="53" t="s">
+      <c r="B5" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="54"/>
+      <c r="C5" s="71"/>
       <c r="D5" s="3" t="s">
         <v>7</v>
       </c>
@@ -3790,31 +3831,31 @@
       <c r="I5" s="5"/>
     </row>
     <row r="6" spans="2:9" ht="15" thickBot="1">
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="85" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="44"/>
-      <c r="D6" s="45" t="s">
+      <c r="C6" s="86"/>
+      <c r="D6" s="87" t="s">
         <v>42</v>
       </c>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
-      <c r="I6" s="47"/>
+      <c r="E6" s="88"/>
+      <c r="F6" s="88"/>
+      <c r="G6" s="88"/>
+      <c r="H6" s="88"/>
+      <c r="I6" s="89"/>
     </row>
     <row r="7" spans="2:9" ht="28.2" thickBot="1">
       <c r="B7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="48" t="s">
+      <c r="C7" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="49"/>
-      <c r="E7" s="48" t="s">
+      <c r="D7" s="91"/>
+      <c r="E7" s="90" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="50"/>
+      <c r="F7" s="92"/>
       <c r="G7" s="10" t="s">
         <v>14</v>
       </c>
@@ -3829,14 +3870,14 @@
       <c r="B8" s="13">
         <v>1</v>
       </c>
-      <c r="C8" s="51" t="s">
-        <v>94</v>
-      </c>
-      <c r="D8" s="52"/>
-      <c r="E8" s="51" t="s">
+      <c r="C8" s="93" t="s">
+        <v>93</v>
+      </c>
+      <c r="D8" s="94"/>
+      <c r="E8" s="93" t="s">
         <v>43</v>
       </c>
-      <c r="F8" s="52"/>
+      <c r="F8" s="94"/>
       <c r="G8" s="17" t="s">
         <v>44</v>
       </c>
@@ -3847,14 +3888,14 @@
       <c r="B9" s="13">
         <v>2</v>
       </c>
-      <c r="C9" s="65" t="s">
-        <v>95</v>
-      </c>
-      <c r="D9" s="66"/>
-      <c r="E9" s="65" t="s">
+      <c r="C9" s="95" t="s">
+        <v>94</v>
+      </c>
+      <c r="D9" s="96"/>
+      <c r="E9" s="95" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="66"/>
+      <c r="F9" s="96"/>
       <c r="G9" s="17" t="s">
         <v>46</v>
       </c>
@@ -3865,32 +3906,37 @@
       <c r="B10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="36" t="s">
+      <c r="C10" s="83" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="37"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="37"/>
+      <c r="D10" s="79"/>
+      <c r="E10" s="79"/>
+      <c r="F10" s="79"/>
+      <c r="G10" s="79"/>
       <c r="H10" s="7" t="s">
         <v>19</v>
       </c>
       <c r="I10" s="6"/>
     </row>
     <row r="11" spans="2:9" ht="15" thickBot="1">
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="84" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="39"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="42"/>
+      <c r="C11" s="80"/>
+      <c r="D11" s="81"/>
+      <c r="E11" s="75"/>
+      <c r="F11" s="75"/>
+      <c r="G11" s="75"/>
+      <c r="H11" s="75"/>
+      <c r="I11" s="76"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:I11"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="D2:F2"/>
@@ -3906,11 +3952,6 @@
     <mergeCell ref="D6:I6"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:I11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>